<commit_message>
docs: Borrowed $200 HK Dollar From My Mother.
</commit_message>
<xml_diff>
--- a/Alan Tang_s Income Expense Now.xlsx
+++ b/Alan Tang_s Income Expense Now.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Income-Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B5DC82-89F0-43B5-BCA8-57248C1AF9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5EF225-5EEA-4248-A9B4-C0B77C7D2EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="153">
   <si>
     <t>Assets</t>
   </si>
@@ -554,8 +554,11 @@
     <t>1. Payback $1200 to Mom</t>
   </si>
   <si>
+    <t xml:space="preserve">1. Payback $1300 to Mom </t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">1. Payback $1339 to Mom - </t>
+      <t xml:space="preserve">1. Payback $1439 to Mom - </t>
     </r>
     <r>
       <rPr>
@@ -1445,49 +1448,34 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1496,20 +1484,14 @@
     <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1523,50 +1505,17 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1589,6 +1538,90 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1598,41 +1631,8 @@
     <xf numFmtId="0" fontId="22" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="22" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1652,11 +1652,14 @@
     <xf numFmtId="166" fontId="22" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2316,8 +2319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1010"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:D25"/>
+    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2334,13 +2337,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="113" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="110"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -2361,7 +2364,7 @@
         <v>89</v>
       </c>
       <c r="C3" s="5">
-        <v>0.47</v>
+        <v>100.47</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2517,7 +2520,7 @@
       </c>
       <c r="C8" s="5">
         <f>SUM(C3:C7)</f>
-        <v>49.17</v>
+        <v>149.16999999999999</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -2549,7 +2552,7 @@
       </c>
       <c r="C9" s="58">
         <f>E97-(C73-SUM(E86,E95))</f>
-        <v>-12745.83</v>
+        <v>-12845.83</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -2603,13 +2606,13 @@
     </row>
     <row r="11" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="12" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A12" s="113" t="s">
+      <c r="A12" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="114"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="115"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="86"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
@@ -2637,7 +2640,7 @@
       <c r="B13" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="100" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="81"/>
@@ -2652,10 +2655,10 @@
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="111" t="s">
+      <c r="C14" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="112"/>
+      <c r="D14" s="83"/>
       <c r="E14" s="18">
         <v>2405</v>
       </c>
@@ -2677,13 +2680,13 @@
       <c r="B16" s="11"/>
     </row>
     <row r="17" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A17" s="113" t="s">
+      <c r="A17" s="116" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="114"/>
-      <c r="C17" s="114"/>
-      <c r="D17" s="114"/>
-      <c r="E17" s="115"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="86"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
@@ -2714,7 +2717,7 @@
       <c r="C18" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="91"/>
+      <c r="D18" s="118"/>
       <c r="E18" s="75" t="s">
         <v>5</v>
       </c>
@@ -2726,10 +2729,10 @@
       <c r="B19" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="118" t="s">
+      <c r="C19" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="119"/>
+      <c r="D19" s="120"/>
       <c r="E19" s="68">
         <v>2405</v>
       </c>
@@ -2754,13 +2757,13 @@
       <c r="E21" s="52"/>
     </row>
     <row r="22" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A22" s="113" t="s">
+      <c r="A22" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="114"/>
-      <c r="C22" s="114"/>
-      <c r="D22" s="114"/>
-      <c r="E22" s="115"/>
+      <c r="B22" s="85"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="86"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
@@ -2788,7 +2791,7 @@
       <c r="B23" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="116" t="s">
+      <c r="C23" s="100" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="81"/>
@@ -2803,7 +2806,7 @@
       <c r="B24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="111" t="s">
+      <c r="C24" s="101" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="81"/>
@@ -2818,10 +2821,10 @@
       <c r="B25" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="132" t="s">
+      <c r="C25" s="111" t="s">
         <v>95</v>
       </c>
-      <c r="D25" s="133"/>
+      <c r="D25" s="112"/>
       <c r="E25" s="68">
         <v>0</v>
       </c>
@@ -2857,10 +2860,10 @@
       <c r="B29" s="11"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="126" t="s">
+      <c r="A30" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="80"/>
+      <c r="B30" s="109"/>
       <c r="C30" s="81"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
@@ -2876,10 +2879,10 @@
       <c r="D31" s="22"/>
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A32" s="79" t="s">
+      <c r="A32" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="80"/>
+      <c r="B32" s="109"/>
       <c r="C32" s="81"/>
     </row>
     <row r="33" spans="1:3" ht="13.5" customHeight="1">
@@ -2913,16 +2916,16 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="120" t="s">
+      <c r="A36" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="121"/>
-      <c r="C36" s="122"/>
+      <c r="B36" s="103"/>
+      <c r="C36" s="104"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A37" s="123"/>
-      <c r="B37" s="124"/>
-      <c r="C37" s="125"/>
+      <c r="A37" s="105"/>
+      <c r="B37" s="106"/>
+      <c r="C37" s="107"/>
     </row>
     <row r="38" spans="1:3" ht="13.5" customHeight="1">
       <c r="A38" s="2" t="s">
@@ -2971,10 +2974,10 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A43" s="79" t="s">
+      <c r="A43" s="110" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="80"/>
+      <c r="B43" s="109"/>
       <c r="C43" s="81"/>
     </row>
     <row r="44" spans="1:3" ht="13.5" customHeight="1">
@@ -3010,11 +3013,11 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A47" s="79" t="s">
+      <c r="A47" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="82"/>
-      <c r="C47" s="83"/>
+      <c r="B47" s="128"/>
+      <c r="C47" s="129"/>
     </row>
     <row r="48" spans="1:3" ht="13.5" customHeight="1">
       <c r="A48" s="2" t="s">
@@ -3056,11 +3059,11 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A52" s="79" t="s">
+      <c r="A52" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="B52" s="82"/>
-      <c r="C52" s="83"/>
+      <c r="B52" s="128"/>
+      <c r="C52" s="129"/>
     </row>
     <row r="53" spans="1:3" ht="13.5" customHeight="1">
       <c r="A53" s="2" t="s">
@@ -3084,11 +3087,11 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A55" s="89" t="s">
+      <c r="A55" s="134" t="s">
         <v>56</v>
       </c>
-      <c r="B55" s="90"/>
-      <c r="C55" s="91"/>
+      <c r="B55" s="135"/>
+      <c r="C55" s="118"/>
     </row>
     <row r="56" spans="1:3" ht="33" customHeight="1">
       <c r="A56" s="33" t="s">
@@ -3112,11 +3115,11 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A58" s="129" t="s">
+      <c r="A58" s="139" t="s">
         <v>36</v>
       </c>
-      <c r="B58" s="124"/>
-      <c r="C58" s="115"/>
+      <c r="B58" s="106"/>
+      <c r="C58" s="86"/>
     </row>
     <row r="59" spans="1:3" ht="13.5" customHeight="1">
       <c r="A59" s="27" t="s">
@@ -3160,11 +3163,11 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A63" s="92" t="s">
+      <c r="A63" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="93"/>
-      <c r="C63" s="94"/>
+      <c r="B63" s="136"/>
+      <c r="C63" s="89"/>
     </row>
     <row r="64" spans="1:3" ht="13.5" customHeight="1">
       <c r="A64" s="59" t="s">
@@ -3220,11 +3223,11 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A69" s="92" t="s">
+      <c r="A69" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="B69" s="136"/>
-      <c r="C69" s="94"/>
+      <c r="B69" s="88"/>
+      <c r="C69" s="89"/>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
       <c r="A70" s="43" t="s">
@@ -3232,7 +3235,7 @@
       </c>
       <c r="B70" s="39"/>
       <c r="C70" s="50">
-        <v>9739</v>
+        <v>9939</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="13.5" customHeight="1">
@@ -3260,7 +3263,7 @@
       </c>
       <c r="C73" s="50">
         <f>SUM(C70:C72)</f>
-        <v>14739</v>
+        <v>14939</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="13.5" customHeight="1">
@@ -3283,64 +3286,64 @@
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="86" t="s">
+      <c r="A77" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="B77" s="127"/>
-      <c r="C77" s="127"/>
-      <c r="D77" s="127"/>
-      <c r="E77" s="128"/>
+      <c r="B77" s="137"/>
+      <c r="C77" s="137"/>
+      <c r="D77" s="137"/>
+      <c r="E77" s="138"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="87" t="s">
+      <c r="A78" s="132" t="s">
         <v>39</v>
       </c>
-      <c r="B78" s="88"/>
-      <c r="C78" s="87" t="s">
+      <c r="B78" s="133"/>
+      <c r="C78" s="132" t="s">
         <v>38</v>
       </c>
-      <c r="D78" s="88"/>
+      <c r="D78" s="133"/>
       <c r="E78" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="106" t="s">
+      <c r="A79" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="B79" s="107"/>
-      <c r="C79" s="84"/>
-      <c r="D79" s="85"/>
+      <c r="B79" s="123"/>
+      <c r="C79" s="130"/>
+      <c r="D79" s="131"/>
       <c r="E79" s="45">
         <f>C74</f>
         <v>1461</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="C80" s="130" t="s">
+      <c r="C80" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="D80" s="131"/>
+      <c r="D80" s="125"/>
       <c r="E80" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="82" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A82" s="86" t="s">
+      <c r="A82" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="B82" s="80"/>
-      <c r="C82" s="80"/>
-      <c r="D82" s="80"/>
+      <c r="B82" s="109"/>
+      <c r="C82" s="109"/>
+      <c r="D82" s="109"/>
       <c r="E82" s="81"/>
     </row>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="86" t="s">
+      <c r="A83" s="92" t="s">
         <v>39</v>
       </c>
       <c r="B83" s="81"/>
-      <c r="C83" s="86" t="s">
+      <c r="C83" s="92" t="s">
         <v>38</v>
       </c>
       <c r="D83" s="81"/>
@@ -3349,63 +3352,63 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="134" t="s">
+      <c r="A84" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="B84" s="138"/>
-      <c r="C84" s="95"/>
-      <c r="D84" s="137"/>
+      <c r="B84" s="93"/>
+      <c r="C84" s="90"/>
+      <c r="D84" s="91"/>
       <c r="E84" s="38">
         <f>E80</f>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="101" t="s">
+      <c r="A85" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="B85" s="102"/>
-      <c r="C85" s="99" t="s">
+      <c r="B85" s="95"/>
+      <c r="C85" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="D85" s="100"/>
+      <c r="D85" s="99"/>
       <c r="E85" s="53">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="103"/>
-      <c r="B86" s="104"/>
-      <c r="C86" s="99" t="s">
+      <c r="A86" s="96"/>
+      <c r="B86" s="97"/>
+      <c r="C86" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="D86" s="105"/>
+      <c r="D86" s="121"/>
       <c r="E86" s="53">
         <v>1000</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="134" t="s">
+      <c r="A87" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="B87" s="112"/>
-      <c r="C87" s="96" t="s">
+      <c r="B87" s="83"/>
+      <c r="C87" s="126" t="s">
         <v>93</v>
       </c>
-      <c r="D87" s="97"/>
+      <c r="D87" s="127"/>
       <c r="E87" s="67">
         <f>C74</f>
         <v>1461</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C88" s="98" t="s">
+      <c r="C88" s="80" t="s">
         <v>29</v>
       </c>
       <c r="D88" s="81"/>
       <c r="E88" s="38">
         <f>SUM(C3:C7)</f>
-        <v>49.17</v>
+        <v>149.16999999999999</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="13.5" customHeight="1">
@@ -3423,20 +3426,20 @@
       <c r="E90" s="25"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="135" t="s">
+      <c r="A91" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="B91" s="114"/>
-      <c r="C91" s="114"/>
-      <c r="D91" s="114"/>
-      <c r="E91" s="115"/>
+      <c r="B91" s="85"/>
+      <c r="C91" s="85"/>
+      <c r="D91" s="85"/>
+      <c r="E91" s="86"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="86" t="s">
+      <c r="A92" s="92" t="s">
         <v>39</v>
       </c>
       <c r="B92" s="81"/>
-      <c r="C92" s="86" t="s">
+      <c r="C92" s="92" t="s">
         <v>38</v>
       </c>
       <c r="D92" s="81"/>
@@ -3445,47 +3448,47 @@
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="134" t="s">
+      <c r="A93" s="82" t="s">
         <v>79</v>
       </c>
-      <c r="B93" s="112"/>
-      <c r="C93" s="95"/>
+      <c r="B93" s="83"/>
+      <c r="C93" s="90"/>
       <c r="D93" s="81"/>
       <c r="E93" s="38">
         <f>E88</f>
-        <v>49.17</v>
+        <v>149.16999999999999</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="101" t="s">
+      <c r="A94" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="B94" s="102"/>
-      <c r="C94" s="99" t="s">
+      <c r="B94" s="95"/>
+      <c r="C94" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="D94" s="100"/>
+      <c r="D94" s="99"/>
       <c r="E94" s="53">
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="103"/>
-      <c r="B95" s="104"/>
-      <c r="C95" s="99" t="s">
+      <c r="A95" s="96"/>
+      <c r="B95" s="97"/>
+      <c r="C95" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="D95" s="105"/>
+      <c r="D95" s="121"/>
       <c r="E95" s="53">
         <v>1000</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A96" s="134" t="s">
+      <c r="A96" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="B96" s="112"/>
-      <c r="C96" s="95"/>
+      <c r="B96" s="83"/>
+      <c r="C96" s="90"/>
       <c r="D96" s="81"/>
       <c r="E96" s="24">
         <f>C74</f>
@@ -3493,13 +3496,13 @@
       </c>
     </row>
     <row r="97" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C97" s="98" t="s">
+      <c r="C97" s="80" t="s">
         <v>30</v>
       </c>
       <c r="D97" s="81"/>
       <c r="E97" s="53">
         <f>(E26+E93)-SUM(E94:E96)</f>
-        <v>-6.8299999999999272</v>
+        <v>93.170000000000073</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="13.5" customHeight="1">
@@ -7156,6 +7159,39 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A77:E77"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A85:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A36:C37"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="C25:D25"/>
     <mergeCell ref="C97:D97"/>
     <mergeCell ref="A93:B93"/>
     <mergeCell ref="A91:E91"/>
@@ -7168,43 +7204,10 @@
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="A94:B95"/>
     <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A36:C37"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
     <mergeCell ref="A83:B83"/>
     <mergeCell ref="C92:D92"/>
     <mergeCell ref="A92:B92"/>
     <mergeCell ref="C95:D95"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="A85:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="A82:E82"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A77:E77"/>
-    <mergeCell ref="A58:C58"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="C9">
@@ -7261,8 +7264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5F3FA5-5013-4B35-A74B-6269617B858B}">
   <dimension ref="A1:Y1012"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -7279,13 +7282,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="113" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="110"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -7307,7 +7310,7 @@
       </c>
       <c r="C3" s="5">
         <f>'April 2024 - June 2024'!E97</f>
-        <v>-6.8299999999999272</v>
+        <v>93.170000000000073</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7402,7 +7405,7 @@
       </c>
       <c r="C6" s="5">
         <f>SUM(C3:C5)</f>
-        <v>23.370000000000072</v>
+        <v>123.37000000000008</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -7488,13 +7491,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="116" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="114"/>
-      <c r="C10" s="114"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="115"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="86"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -7522,7 +7525,7 @@
       <c r="B11" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="116" t="s">
+      <c r="C11" s="100" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="81"/>
@@ -7537,10 +7540,10 @@
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="111" t="s">
+      <c r="C12" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="112"/>
+      <c r="D12" s="83"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -7562,13 +7565,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="113" t="s">
+      <c r="A15" s="116" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="114"/>
-      <c r="D15" s="114"/>
-      <c r="E15" s="115"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="86"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -7596,7 +7599,7 @@
       <c r="B16" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="116" t="s">
+      <c r="C16" s="100" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="81"/>
@@ -7611,7 +7614,7 @@
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="111" t="s">
+      <c r="C17" s="101" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="81"/>
@@ -7639,13 +7642,13 @@
       <c r="E19" s="52"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="113" t="s">
+      <c r="A20" s="116" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="114"/>
-      <c r="C20" s="114"/>
-      <c r="D20" s="114"/>
-      <c r="E20" s="115"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="86"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -7676,7 +7679,7 @@
       <c r="C21" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="91"/>
+      <c r="D21" s="118"/>
       <c r="E21" s="75" t="s">
         <v>5</v>
       </c>
@@ -7688,10 +7691,10 @@
       <c r="B22" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="118" t="s">
+      <c r="C22" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="119"/>
+      <c r="D22" s="120"/>
       <c r="E22" s="68">
         <v>2405</v>
       </c>
@@ -7701,8 +7704,8 @@
       <c r="B23" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="118"/>
-      <c r="D23" s="118"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
       <c r="E23" s="68">
         <v>204</v>
       </c>
@@ -7745,10 +7748,10 @@
       <c r="B28" s="11"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A29" s="148" t="s">
+      <c r="A29" s="140" t="s">
         <v>101</v>
       </c>
-      <c r="B29" s="80"/>
+      <c r="B29" s="109"/>
       <c r="C29" s="81"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
@@ -7764,10 +7767,10 @@
       <c r="D30" s="22"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A31" s="79" t="s">
+      <c r="A31" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="80"/>
+      <c r="B31" s="109"/>
       <c r="C31" s="81"/>
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
@@ -7801,16 +7804,16 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="120" t="s">
+      <c r="A35" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="121"/>
-      <c r="C35" s="122"/>
+      <c r="B35" s="103"/>
+      <c r="C35" s="104"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="123"/>
-      <c r="B36" s="124"/>
-      <c r="C36" s="125"/>
+      <c r="A36" s="105"/>
+      <c r="B36" s="106"/>
+      <c r="C36" s="107"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -7859,10 +7862,10 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A42" s="79" t="s">
+      <c r="A42" s="110" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="80"/>
+      <c r="B42" s="109"/>
       <c r="C42" s="81"/>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
@@ -7898,11 +7901,11 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A46" s="79" t="s">
+      <c r="A46" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="82"/>
-      <c r="C46" s="83"/>
+      <c r="B46" s="128"/>
+      <c r="C46" s="129"/>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -7944,11 +7947,11 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="79" t="s">
+      <c r="A51" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="B51" s="82"/>
-      <c r="C51" s="83"/>
+      <c r="B51" s="128"/>
+      <c r="C51" s="129"/>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="2" t="s">
@@ -7972,11 +7975,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="89" t="s">
+      <c r="A54" s="134" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="90"/>
-      <c r="C54" s="91"/>
+      <c r="B54" s="135"/>
+      <c r="C54" s="118"/>
     </row>
     <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="33" t="s">
@@ -8000,11 +8003,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="129" t="s">
+      <c r="A57" s="139" t="s">
         <v>36</v>
       </c>
-      <c r="B57" s="124"/>
-      <c r="C57" s="115"/>
+      <c r="B57" s="106"/>
+      <c r="C57" s="86"/>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
       <c r="A58" s="27" t="s">
@@ -8048,11 +8051,11 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A62" s="92" t="s">
+      <c r="A62" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="B62" s="93"/>
-      <c r="C62" s="94"/>
+      <c r="B62" s="136"/>
+      <c r="C62" s="89"/>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
       <c r="A63" s="59" t="s">
@@ -8069,7 +8072,7 @@
       <c r="A64" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="B64" s="149" t="s">
+      <c r="B64" s="79" t="s">
         <v>86</v>
       </c>
       <c r="C64" s="71">
@@ -8119,11 +8122,11 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A69" s="92" t="s">
+      <c r="A69" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="B69" s="136"/>
-      <c r="C69" s="94"/>
+      <c r="B69" s="88"/>
+      <c r="C69" s="89"/>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
       <c r="A70" s="43" t="s">
@@ -8131,8 +8134,8 @@
       </c>
       <c r="B70" s="39"/>
       <c r="C70" s="50">
-        <f>'April 2024 - June 2024'!C70-'April 2024 - June 2024'!E94</f>
-        <v>9739</v>
+        <f>'April 2024 - June 2024'!C70</f>
+        <v>9939</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="13.5" customHeight="1">
@@ -8160,7 +8163,7 @@
       </c>
       <c r="C73" s="50">
         <f>SUM(C70:C72)</f>
-        <v>14739</v>
+        <v>14939</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="13.5" customHeight="1">
@@ -8183,89 +8186,89 @@
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="86" t="s">
+      <c r="A77" s="92" t="s">
         <v>102</v>
       </c>
-      <c r="B77" s="80"/>
-      <c r="C77" s="80"/>
-      <c r="D77" s="80"/>
+      <c r="B77" s="109"/>
+      <c r="C77" s="109"/>
+      <c r="D77" s="109"/>
       <c r="E77" s="81"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="87" t="s">
+      <c r="A78" s="132" t="s">
         <v>39</v>
       </c>
-      <c r="B78" s="91"/>
-      <c r="C78" s="87" t="s">
+      <c r="B78" s="118"/>
+      <c r="C78" s="132" t="s">
         <v>38</v>
       </c>
-      <c r="D78" s="91"/>
+      <c r="D78" s="118"/>
       <c r="E78" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="144" t="s">
+      <c r="A79" s="143" t="s">
         <v>83</v>
       </c>
-      <c r="B79" s="144"/>
-      <c r="C79" s="142" t="s">
+      <c r="B79" s="143"/>
+      <c r="C79" s="141" t="s">
         <v>84</v>
       </c>
-      <c r="D79" s="143"/>
+      <c r="D79" s="142"/>
       <c r="E79" s="76">
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="145"/>
-      <c r="B80" s="145"/>
-      <c r="C80" s="146" t="s">
+      <c r="A80" s="144"/>
+      <c r="B80" s="144"/>
+      <c r="C80" s="145" t="s">
         <v>121</v>
       </c>
-      <c r="D80" s="147"/>
+      <c r="D80" s="146"/>
       <c r="E80" s="53">
         <v>850</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A81" s="106" t="s">
+      <c r="A81" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="B81" s="107"/>
-      <c r="C81" s="84"/>
-      <c r="D81" s="85"/>
+      <c r="B81" s="123"/>
+      <c r="C81" s="130"/>
+      <c r="D81" s="131"/>
       <c r="E81" s="45">
         <f>C74</f>
         <v>1461</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C82" s="130" t="s">
+      <c r="C82" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="D82" s="80"/>
+      <c r="D82" s="109"/>
       <c r="E82" s="38">
         <f>(C6+E13)-SUM(E79:E81)</f>
-        <v>117.36999999999989</v>
+        <v>217.36999999999989</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="86" t="s">
+      <c r="A84" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="B84" s="80"/>
-      <c r="C84" s="80"/>
-      <c r="D84" s="80"/>
+      <c r="B84" s="109"/>
+      <c r="C84" s="109"/>
+      <c r="D84" s="109"/>
       <c r="E84" s="81"/>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="86" t="s">
+      <c r="A85" s="92" t="s">
         <v>39</v>
       </c>
       <c r="B85" s="81"/>
-      <c r="C85" s="86" t="s">
+      <c r="C85" s="92" t="s">
         <v>38</v>
       </c>
       <c r="D85" s="81"/>
@@ -8274,47 +8277,47 @@
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="134" t="s">
+      <c r="A86" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="B86" s="112"/>
-      <c r="C86" s="96"/>
-      <c r="D86" s="141"/>
+      <c r="B86" s="83"/>
+      <c r="C86" s="126"/>
+      <c r="D86" s="149"/>
       <c r="E86" s="38">
         <f>E82</f>
-        <v>117.36999999999989</v>
+        <v>217.36999999999989</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="101" t="s">
+      <c r="A87" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="B87" s="102"/>
-      <c r="C87" s="96" t="s">
+      <c r="B87" s="95"/>
+      <c r="C87" s="126" t="s">
         <v>84</v>
       </c>
-      <c r="D87" s="140"/>
+      <c r="D87" s="148"/>
       <c r="E87" s="53">
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A88" s="103"/>
-      <c r="B88" s="104"/>
-      <c r="C88" s="99" t="s">
+      <c r="A88" s="96"/>
+      <c r="B88" s="97"/>
+      <c r="C88" s="98" t="s">
         <v>121</v>
       </c>
-      <c r="D88" s="139"/>
+      <c r="D88" s="147"/>
       <c r="E88" s="53">
         <v>850</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A89" s="134" t="s">
+      <c r="A89" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="B89" s="112"/>
-      <c r="C89" s="95"/>
+      <c r="B89" s="83"/>
+      <c r="C89" s="90"/>
       <c r="D89" s="81"/>
       <c r="E89" s="67">
         <f>C74</f>
@@ -8322,13 +8325,13 @@
       </c>
     </row>
     <row r="90" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C90" s="98" t="s">
+      <c r="C90" s="80" t="s">
         <v>29</v>
       </c>
       <c r="D90" s="81"/>
       <c r="E90" s="38">
         <f>(E18+E86)-SUM(E87:E89)</f>
-        <v>211.36999999999989</v>
+        <v>311.36999999999989</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
@@ -8346,20 +8349,20 @@
       <c r="E92" s="25"/>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="135" t="s">
+      <c r="A93" s="84" t="s">
         <v>104</v>
       </c>
-      <c r="B93" s="114"/>
-      <c r="C93" s="114"/>
-      <c r="D93" s="114"/>
-      <c r="E93" s="115"/>
+      <c r="B93" s="85"/>
+      <c r="C93" s="85"/>
+      <c r="D93" s="85"/>
+      <c r="E93" s="86"/>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="86" t="s">
+      <c r="A94" s="92" t="s">
         <v>39</v>
       </c>
       <c r="B94" s="81"/>
-      <c r="C94" s="86" t="s">
+      <c r="C94" s="92" t="s">
         <v>38</v>
       </c>
       <c r="D94" s="81"/>
@@ -8368,26 +8371,26 @@
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="134" t="s">
+      <c r="A95" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="B95" s="112"/>
-      <c r="C95" s="95"/>
+      <c r="B95" s="83"/>
+      <c r="C95" s="90"/>
       <c r="D95" s="81"/>
       <c r="E95" s="38">
         <f>E90</f>
-        <v>211.36999999999989</v>
+        <v>311.36999999999989</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A96" s="134" t="s">
+      <c r="A96" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="B96" s="138"/>
-      <c r="C96" s="99" t="s">
+      <c r="B96" s="93"/>
+      <c r="C96" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="D96" s="100"/>
+      <c r="D96" s="99"/>
       <c r="E96" s="53">
         <v>0</v>
       </c>
@@ -8395,20 +8398,20 @@
     <row r="97" spans="1:5" ht="13.5" customHeight="1">
       <c r="A97" s="77"/>
       <c r="B97" s="78"/>
-      <c r="C97" s="99" t="s">
+      <c r="C97" s="98" t="s">
         <v>122</v>
       </c>
-      <c r="D97" s="139"/>
+      <c r="D97" s="147"/>
       <c r="E97" s="53">
         <v>800</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A98" s="134" t="s">
+      <c r="A98" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="B98" s="112"/>
-      <c r="C98" s="95"/>
+      <c r="B98" s="83"/>
+      <c r="C98" s="90"/>
       <c r="D98" s="81"/>
       <c r="E98" s="67">
         <f>C74</f>
@@ -8416,13 +8419,13 @@
       </c>
     </row>
     <row r="99" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C99" s="98" t="s">
+      <c r="C99" s="80" t="s">
         <v>29</v>
       </c>
       <c r="D99" s="81"/>
       <c r="E99" s="53">
         <f>(E24+E95)-SUM(E96:E98)</f>
-        <v>559.36999999999989</v>
+        <v>659.36999999999989</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="13.5" customHeight="1">
@@ -12079,6 +12082,42 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="A87:B88"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="A84:E84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="A35:C36"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="A93:E93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="A79:B80"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A62:C62"/>
     <mergeCell ref="A81:B81"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A1:E1"/>
@@ -12095,42 +12134,6 @@
     <mergeCell ref="A69:C69"/>
     <mergeCell ref="A77:E77"/>
     <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="A79:B80"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="A93:E93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="A87:B88"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="A84:E84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="A35:C36"/>
-    <mergeCell ref="A42:C42"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="47" priority="2" operator="lessThan">
@@ -12192,7 +12195,7 @@
   <dimension ref="A1:Y1008"/>
   <sheetViews>
     <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -12209,13 +12212,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="113" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="110"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -12237,7 +12240,7 @@
       </c>
       <c r="C3" s="5">
         <f>'July 2024 - September 2024'!E99</f>
-        <v>559.36999999999989</v>
+        <v>659.36999999999989</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -12332,7 +12335,7 @@
       </c>
       <c r="C6" s="5">
         <f>SUM(C3:C5)</f>
-        <v>589.56999999999994</v>
+        <v>689.56999999999994</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -12364,7 +12367,7 @@
       </c>
       <c r="C7" s="58">
         <f>('July 2024 - September 2024'!C7+E95)+SUM(E78,E85,E93)</f>
-        <v>-5652.8899999999994</v>
+        <v>-5552.8899999999994</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -12418,13 +12421,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="116" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="114"/>
-      <c r="C10" s="114"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="115"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="86"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -12452,7 +12455,7 @@
       <c r="B11" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="116" t="s">
+      <c r="C11" s="100" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="81"/>
@@ -12467,10 +12470,10 @@
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="111" t="s">
+      <c r="C12" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="112"/>
+      <c r="D12" s="83"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -12492,13 +12495,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="113" t="s">
+      <c r="A15" s="116" t="s">
         <v>115</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="114"/>
-      <c r="D15" s="114"/>
-      <c r="E15" s="115"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="86"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -12526,7 +12529,7 @@
       <c r="B16" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="116" t="s">
+      <c r="C16" s="100" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="81"/>
@@ -12541,7 +12544,7 @@
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="111" t="s">
+      <c r="C17" s="101" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="81"/>
@@ -12569,13 +12572,13 @@
       <c r="E19" s="52"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="113" t="s">
+      <c r="A20" s="116" t="s">
         <v>111</v>
       </c>
-      <c r="B20" s="114"/>
-      <c r="C20" s="114"/>
-      <c r="D20" s="114"/>
-      <c r="E20" s="115"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="86"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -12606,7 +12609,7 @@
       <c r="C21" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="91"/>
+      <c r="D21" s="118"/>
       <c r="E21" s="75" t="s">
         <v>5</v>
       </c>
@@ -12618,10 +12621,10 @@
       <c r="B22" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="118" t="s">
+      <c r="C22" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="119"/>
+      <c r="D22" s="120"/>
       <c r="E22" s="68">
         <v>2405</v>
       </c>
@@ -12664,10 +12667,10 @@
       <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A28" s="148" t="s">
+      <c r="A28" s="140" t="s">
         <v>113</v>
       </c>
-      <c r="B28" s="80"/>
+      <c r="B28" s="109"/>
       <c r="C28" s="81"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
@@ -12683,10 +12686,10 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="79" t="s">
+      <c r="A30" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="80"/>
+      <c r="B30" s="109"/>
       <c r="C30" s="81"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
@@ -12720,16 +12723,16 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A34" s="120" t="s">
+      <c r="A34" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="121"/>
-      <c r="C34" s="122"/>
+      <c r="B34" s="103"/>
+      <c r="C34" s="104"/>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="123"/>
-      <c r="B35" s="124"/>
-      <c r="C35" s="125"/>
+      <c r="A35" s="105"/>
+      <c r="B35" s="106"/>
+      <c r="C35" s="107"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
       <c r="A36" s="2" t="s">
@@ -12778,10 +12781,10 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A41" s="79" t="s">
+      <c r="A41" s="110" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="80"/>
+      <c r="B41" s="109"/>
       <c r="C41" s="81"/>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
@@ -12817,11 +12820,11 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A45" s="79" t="s">
+      <c r="A45" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="82"/>
-      <c r="C45" s="83"/>
+      <c r="B45" s="128"/>
+      <c r="C45" s="129"/>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
       <c r="A46" s="2" t="s">
@@ -12863,11 +12866,11 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A50" s="79" t="s">
+      <c r="A50" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="B50" s="82"/>
-      <c r="C50" s="83"/>
+      <c r="B50" s="128"/>
+      <c r="C50" s="129"/>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
       <c r="A51" s="2" t="s">
@@ -12891,11 +12894,11 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A53" s="89" t="s">
+      <c r="A53" s="134" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="90"/>
-      <c r="C53" s="91"/>
+      <c r="B53" s="135"/>
+      <c r="C53" s="118"/>
     </row>
     <row r="54" spans="1:3" ht="33" customHeight="1">
       <c r="A54" s="33" t="s">
@@ -12919,11 +12922,11 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A56" s="129" t="s">
+      <c r="A56" s="139" t="s">
         <v>36</v>
       </c>
-      <c r="B56" s="124"/>
-      <c r="C56" s="115"/>
+      <c r="B56" s="106"/>
+      <c r="C56" s="86"/>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
       <c r="A57" s="27" t="s">
@@ -12967,11 +12970,11 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A61" s="92" t="s">
+      <c r="A61" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="93"/>
-      <c r="C61" s="94"/>
+      <c r="B61" s="136"/>
+      <c r="C61" s="89"/>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
       <c r="A62" s="59" t="s">
@@ -13038,11 +13041,11 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A68" s="92" t="s">
+      <c r="A68" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="136"/>
-      <c r="C68" s="94"/>
+      <c r="B68" s="88"/>
+      <c r="C68" s="89"/>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
       <c r="A69" s="43" t="s">
@@ -13050,8 +13053,8 @@
       </c>
       <c r="B69" s="39"/>
       <c r="C69" s="50">
-        <f>'April 2024 - June 2024'!C70-'April 2024 - June 2024'!E94</f>
-        <v>9739</v>
+        <f>'July 2024 - September 2024'!C70</f>
+        <v>9939</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
@@ -13079,7 +13082,7 @@
       </c>
       <c r="C72" s="50">
         <f>SUM(C69:C71)</f>
-        <v>14739</v>
+        <v>14939</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="13.5" customHeight="1">
@@ -13102,78 +13105,78 @@
       <c r="B75" s="11"/>
     </row>
     <row r="76" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A76" s="86" t="s">
+      <c r="A76" s="92" t="s">
         <v>108</v>
       </c>
-      <c r="B76" s="80"/>
-      <c r="C76" s="80"/>
-      <c r="D76" s="80"/>
+      <c r="B76" s="109"/>
+      <c r="C76" s="109"/>
+      <c r="D76" s="109"/>
       <c r="E76" s="81"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="87" t="s">
+      <c r="A77" s="132" t="s">
         <v>39</v>
       </c>
-      <c r="B77" s="91"/>
-      <c r="C77" s="87" t="s">
+      <c r="B77" s="118"/>
+      <c r="C77" s="132" t="s">
         <v>38</v>
       </c>
-      <c r="D77" s="91"/>
+      <c r="D77" s="118"/>
       <c r="E77" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="144" t="s">
+      <c r="A78" s="143" t="s">
         <v>83</v>
       </c>
-      <c r="B78" s="102"/>
-      <c r="C78" s="142" t="s">
+      <c r="B78" s="95"/>
+      <c r="C78" s="141" t="s">
         <v>150</v>
       </c>
-      <c r="D78" s="143"/>
+      <c r="D78" s="142"/>
       <c r="E78" s="76">
         <v>1200</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="106" t="s">
+      <c r="A79" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="B79" s="107"/>
-      <c r="C79" s="84"/>
-      <c r="D79" s="85"/>
+      <c r="B79" s="123"/>
+      <c r="C79" s="130"/>
+      <c r="D79" s="131"/>
       <c r="E79" s="45">
         <f>C73</f>
         <v>1257</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="C80" s="130" t="s">
+      <c r="C80" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="D80" s="80"/>
+      <c r="D80" s="109"/>
       <c r="E80" s="38">
         <f>(C6+E13)-SUM(E78:E79)</f>
-        <v>537.56999999999971</v>
+        <v>637.56999999999971</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="82" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A82" s="86" t="s">
+      <c r="A82" s="92" t="s">
         <v>117</v>
       </c>
-      <c r="B82" s="80"/>
-      <c r="C82" s="80"/>
-      <c r="D82" s="80"/>
+      <c r="B82" s="109"/>
+      <c r="C82" s="109"/>
+      <c r="D82" s="109"/>
       <c r="E82" s="81"/>
     </row>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="86" t="s">
+      <c r="A83" s="92" t="s">
         <v>39</v>
       </c>
       <c r="B83" s="81"/>
-      <c r="C83" s="86" t="s">
+      <c r="C83" s="92" t="s">
         <v>38</v>
       </c>
       <c r="D83" s="81"/>
@@ -13182,36 +13185,36 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="134" t="s">
+      <c r="A84" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="B84" s="112"/>
-      <c r="C84" s="96"/>
-      <c r="D84" s="141"/>
+      <c r="B84" s="83"/>
+      <c r="C84" s="126"/>
+      <c r="D84" s="149"/>
       <c r="E84" s="38">
         <f>E80</f>
-        <v>537.56999999999971</v>
+        <v>637.56999999999971</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="134" t="s">
+      <c r="A85" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="B85" s="138"/>
-      <c r="C85" s="99" t="s">
+      <c r="B85" s="93"/>
+      <c r="C85" s="98" t="s">
         <v>150</v>
       </c>
-      <c r="D85" s="140"/>
+      <c r="D85" s="148"/>
       <c r="E85" s="53">
         <v>1200</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="134" t="s">
+      <c r="A86" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="B86" s="112"/>
-      <c r="C86" s="95"/>
+      <c r="B86" s="83"/>
+      <c r="C86" s="90"/>
       <c r="D86" s="81"/>
       <c r="E86" s="67">
         <f>C73</f>
@@ -13219,13 +13222,13 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C87" s="98" t="s">
+      <c r="C87" s="80" t="s">
         <v>29</v>
       </c>
       <c r="D87" s="81"/>
       <c r="E87" s="38">
         <f>(E18+E84)-SUM(E85:E86)</f>
-        <v>485.56999999999971</v>
+        <v>585.56999999999971</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
@@ -13243,20 +13246,20 @@
       <c r="E89" s="25"/>
     </row>
     <row r="90" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A90" s="135" t="s">
+      <c r="A90" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="B90" s="114"/>
-      <c r="C90" s="114"/>
-      <c r="D90" s="114"/>
-      <c r="E90" s="115"/>
+      <c r="B90" s="85"/>
+      <c r="C90" s="85"/>
+      <c r="D90" s="85"/>
+      <c r="E90" s="86"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="86" t="s">
+      <c r="A91" s="92" t="s">
         <v>39</v>
       </c>
       <c r="B91" s="81"/>
-      <c r="C91" s="86" t="s">
+      <c r="C91" s="92" t="s">
         <v>38</v>
       </c>
       <c r="D91" s="81"/>
@@ -13265,36 +13268,36 @@
       </c>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="134" t="s">
+      <c r="A92" s="82" t="s">
         <v>118</v>
       </c>
-      <c r="B92" s="112"/>
-      <c r="C92" s="95"/>
+      <c r="B92" s="83"/>
+      <c r="C92" s="90"/>
       <c r="D92" s="81"/>
       <c r="E92" s="38">
         <f>E87</f>
-        <v>485.56999999999971</v>
+        <v>585.56999999999971</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="134" t="s">
+      <c r="A93" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="B93" s="138"/>
-      <c r="C93" s="99" t="s">
+      <c r="B93" s="93"/>
+      <c r="C93" s="98" t="s">
         <v>150</v>
       </c>
-      <c r="D93" s="100"/>
+      <c r="D93" s="99"/>
       <c r="E93" s="53">
         <v>1200</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="134" t="s">
+      <c r="A94" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="B94" s="112"/>
-      <c r="C94" s="95"/>
+      <c r="B94" s="83"/>
+      <c r="C94" s="90"/>
       <c r="D94" s="81"/>
       <c r="E94" s="67">
         <f>C73</f>
@@ -13302,13 +13305,13 @@
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C95" s="98" t="s">
+      <c r="C95" s="80" t="s">
         <v>29</v>
       </c>
       <c r="D95" s="81"/>
       <c r="E95" s="53">
         <f>(E23+E92)-SUM(E93:E94)</f>
-        <v>433.56999999999971</v>
+        <v>533.56999999999971</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
@@ -16965,36 +16968,11 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A34:C35"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A76:E76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="C87:D87"/>
@@ -17008,11 +16986,36 @@
     <mergeCell ref="A83:B83"/>
     <mergeCell ref="C83:D83"/>
     <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A76:E76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A34:C35"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A15:E15"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="35" priority="2" operator="lessThan">
@@ -17072,8 +17075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5AAEA1-C3EE-4B36-938E-0F583AF15471}">
   <dimension ref="A1:Y1008"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -17090,13 +17093,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="113" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="110"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -17118,7 +17121,7 @@
       </c>
       <c r="C3" s="5">
         <f>'October 2024 - December 2024'!E95</f>
-        <v>433.56999999999971</v>
+        <v>533.56999999999971</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -17213,7 +17216,7 @@
       </c>
       <c r="C6" s="5">
         <f>SUM(C3:C5)</f>
-        <v>463.7699999999997</v>
+        <v>563.76999999999975</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -17245,7 +17248,7 @@
       </c>
       <c r="C7" s="58">
         <f>('October 2024 - December 2024'!C7+E95)+SUM(E78,E85,E93)</f>
-        <v>-1745.12</v>
+        <v>-1545.12</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -17299,13 +17302,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="116" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="114"/>
-      <c r="C10" s="114"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="115"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="86"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -17333,7 +17336,7 @@
       <c r="B11" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="116" t="s">
+      <c r="C11" s="100" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="81"/>
@@ -17348,10 +17351,10 @@
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="111" t="s">
+      <c r="C12" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="112"/>
+      <c r="D12" s="83"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -17373,13 +17376,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="113" t="s">
+      <c r="A15" s="116" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="114"/>
-      <c r="D15" s="114"/>
-      <c r="E15" s="115"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="86"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -17407,7 +17410,7 @@
       <c r="B16" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="116" t="s">
+      <c r="C16" s="100" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="81"/>
@@ -17422,7 +17425,7 @@
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="111" t="s">
+      <c r="C17" s="101" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="81"/>
@@ -17450,13 +17453,13 @@
       <c r="E19" s="52"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="113" t="s">
+      <c r="A20" s="116" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="114"/>
-      <c r="C20" s="114"/>
-      <c r="D20" s="114"/>
-      <c r="E20" s="115"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="86"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -17487,7 +17490,7 @@
       <c r="C21" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="91"/>
+      <c r="D21" s="118"/>
       <c r="E21" s="75" t="s">
         <v>5</v>
       </c>
@@ -17499,10 +17502,10 @@
       <c r="B22" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="118" t="s">
+      <c r="C22" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="119"/>
+      <c r="D22" s="120"/>
       <c r="E22" s="68">
         <v>2405</v>
       </c>
@@ -17545,10 +17548,10 @@
       <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A28" s="148" t="s">
+      <c r="A28" s="140" t="s">
         <v>129</v>
       </c>
-      <c r="B28" s="80"/>
+      <c r="B28" s="109"/>
       <c r="C28" s="81"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
@@ -17564,10 +17567,10 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="79" t="s">
+      <c r="A30" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="80"/>
+      <c r="B30" s="109"/>
       <c r="C30" s="81"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
@@ -17601,16 +17604,16 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A34" s="120" t="s">
+      <c r="A34" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="121"/>
-      <c r="C34" s="122"/>
+      <c r="B34" s="103"/>
+      <c r="C34" s="104"/>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="123"/>
-      <c r="B35" s="124"/>
-      <c r="C35" s="125"/>
+      <c r="A35" s="105"/>
+      <c r="B35" s="106"/>
+      <c r="C35" s="107"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
       <c r="A36" s="2" t="s">
@@ -17659,10 +17662,10 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A41" s="79" t="s">
+      <c r="A41" s="110" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="80"/>
+      <c r="B41" s="109"/>
       <c r="C41" s="81"/>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
@@ -17698,11 +17701,11 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A45" s="79" t="s">
+      <c r="A45" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="82"/>
-      <c r="C45" s="83"/>
+      <c r="B45" s="128"/>
+      <c r="C45" s="129"/>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
       <c r="A46" s="2" t="s">
@@ -17744,11 +17747,11 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A50" s="79" t="s">
+      <c r="A50" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="B50" s="82"/>
-      <c r="C50" s="83"/>
+      <c r="B50" s="128"/>
+      <c r="C50" s="129"/>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
       <c r="A51" s="2" t="s">
@@ -17772,11 +17775,11 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A53" s="89" t="s">
+      <c r="A53" s="134" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="90"/>
-      <c r="C53" s="91"/>
+      <c r="B53" s="135"/>
+      <c r="C53" s="118"/>
     </row>
     <row r="54" spans="1:3" ht="33" customHeight="1">
       <c r="A54" s="33" t="s">
@@ -17800,11 +17803,11 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A56" s="129" t="s">
+      <c r="A56" s="139" t="s">
         <v>36</v>
       </c>
-      <c r="B56" s="124"/>
-      <c r="C56" s="115"/>
+      <c r="B56" s="106"/>
+      <c r="C56" s="86"/>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
       <c r="A57" s="27" t="s">
@@ -17848,11 +17851,11 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A61" s="92" t="s">
+      <c r="A61" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="93"/>
-      <c r="C61" s="94"/>
+      <c r="B61" s="136"/>
+      <c r="C61" s="89"/>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
       <c r="A62" s="59" t="s">
@@ -17919,11 +17922,11 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A68" s="92" t="s">
+      <c r="A68" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="136"/>
-      <c r="C68" s="94"/>
+      <c r="B68" s="88"/>
+      <c r="C68" s="89"/>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
       <c r="A69" s="43" t="s">
@@ -17931,8 +17934,8 @@
       </c>
       <c r="B69" s="39"/>
       <c r="C69" s="50">
-        <f>'April 2024 - June 2024'!C70-'April 2024 - June 2024'!E94</f>
-        <v>9739</v>
+        <f>'October 2024 - December 2024'!C69</f>
+        <v>9939</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
@@ -17960,7 +17963,7 @@
       </c>
       <c r="C72" s="50">
         <f>SUM(C69:C71)</f>
-        <v>14739</v>
+        <v>14939</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="13.5" customHeight="1">
@@ -17983,78 +17986,78 @@
       <c r="B75" s="11"/>
     </row>
     <row r="76" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A76" s="86" t="s">
+      <c r="A76" s="92" t="s">
         <v>130</v>
       </c>
-      <c r="B76" s="80"/>
-      <c r="C76" s="80"/>
-      <c r="D76" s="80"/>
+      <c r="B76" s="109"/>
+      <c r="C76" s="109"/>
+      <c r="D76" s="109"/>
       <c r="E76" s="81"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="87" t="s">
+      <c r="A77" s="132" t="s">
         <v>39</v>
       </c>
-      <c r="B77" s="91"/>
-      <c r="C77" s="87" t="s">
+      <c r="B77" s="118"/>
+      <c r="C77" s="132" t="s">
         <v>38</v>
       </c>
-      <c r="D77" s="91"/>
+      <c r="D77" s="118"/>
       <c r="E77" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="144" t="s">
+      <c r="A78" s="143" t="s">
         <v>83</v>
       </c>
-      <c r="B78" s="102"/>
-      <c r="C78" s="142" t="s">
+      <c r="B78" s="95"/>
+      <c r="C78" s="141" t="s">
         <v>150</v>
       </c>
-      <c r="D78" s="143"/>
+      <c r="D78" s="142"/>
       <c r="E78" s="76">
         <v>1200</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="106" t="s">
+      <c r="A79" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="B79" s="107"/>
-      <c r="C79" s="84"/>
-      <c r="D79" s="85"/>
+      <c r="B79" s="123"/>
+      <c r="C79" s="130"/>
+      <c r="D79" s="131"/>
       <c r="E79" s="45">
         <f>C73</f>
         <v>1257</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="C80" s="130" t="s">
+      <c r="C80" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="D80" s="80"/>
+      <c r="D80" s="109"/>
       <c r="E80" s="38">
         <f>(C6+E13)-SUM(E78:E79)</f>
-        <v>411.76999999999953</v>
+        <v>511.76999999999953</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="82" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A82" s="86" t="s">
+      <c r="A82" s="92" t="s">
         <v>134</v>
       </c>
-      <c r="B82" s="80"/>
-      <c r="C82" s="80"/>
-      <c r="D82" s="80"/>
+      <c r="B82" s="109"/>
+      <c r="C82" s="109"/>
+      <c r="D82" s="109"/>
       <c r="E82" s="81"/>
     </row>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="86" t="s">
+      <c r="A83" s="92" t="s">
         <v>39</v>
       </c>
       <c r="B83" s="81"/>
-      <c r="C83" s="86" t="s">
+      <c r="C83" s="92" t="s">
         <v>38</v>
       </c>
       <c r="D83" s="81"/>
@@ -18063,36 +18066,36 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="134" t="s">
+      <c r="A84" s="82" t="s">
         <v>148</v>
       </c>
-      <c r="B84" s="112"/>
-      <c r="C84" s="96"/>
-      <c r="D84" s="141"/>
+      <c r="B84" s="83"/>
+      <c r="C84" s="126"/>
+      <c r="D84" s="149"/>
       <c r="E84" s="38">
         <f>E80</f>
-        <v>411.76999999999953</v>
+        <v>511.76999999999953</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="134" t="s">
+      <c r="A85" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="B85" s="138"/>
-      <c r="C85" s="99" t="s">
+      <c r="B85" s="93"/>
+      <c r="C85" s="98" t="s">
         <v>150</v>
       </c>
-      <c r="D85" s="140"/>
+      <c r="D85" s="148"/>
       <c r="E85" s="53">
         <v>1200</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="134" t="s">
+      <c r="A86" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="B86" s="112"/>
-      <c r="C86" s="95"/>
+      <c r="B86" s="83"/>
+      <c r="C86" s="90"/>
       <c r="D86" s="81"/>
       <c r="E86" s="67">
         <f>C73</f>
@@ -18100,13 +18103,13 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C87" s="98" t="s">
+      <c r="C87" s="80" t="s">
         <v>29</v>
       </c>
       <c r="D87" s="81"/>
       <c r="E87" s="38">
         <f>(E18+E84)-SUM(E85:E86)</f>
-        <v>359.76999999999953</v>
+        <v>459.76999999999953</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
@@ -18124,20 +18127,20 @@
       <c r="E89" s="25"/>
     </row>
     <row r="90" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A90" s="135" t="s">
+      <c r="A90" s="84" t="s">
         <v>131</v>
       </c>
-      <c r="B90" s="114"/>
-      <c r="C90" s="114"/>
-      <c r="D90" s="114"/>
-      <c r="E90" s="115"/>
+      <c r="B90" s="85"/>
+      <c r="C90" s="85"/>
+      <c r="D90" s="85"/>
+      <c r="E90" s="86"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="86" t="s">
+      <c r="A91" s="92" t="s">
         <v>39</v>
       </c>
       <c r="B91" s="81"/>
-      <c r="C91" s="86" t="s">
+      <c r="C91" s="92" t="s">
         <v>38</v>
       </c>
       <c r="D91" s="81"/>
@@ -18146,36 +18149,36 @@
       </c>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="134" t="s">
+      <c r="A92" s="82" t="s">
         <v>149</v>
       </c>
-      <c r="B92" s="112"/>
-      <c r="C92" s="95"/>
+      <c r="B92" s="83"/>
+      <c r="C92" s="90"/>
       <c r="D92" s="81"/>
       <c r="E92" s="38">
         <f>E87</f>
-        <v>359.76999999999953</v>
+        <v>459.76999999999953</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="134" t="s">
+      <c r="A93" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="B93" s="138"/>
-      <c r="C93" s="99" t="s">
+      <c r="B93" s="93"/>
+      <c r="C93" s="98" t="s">
         <v>150</v>
       </c>
-      <c r="D93" s="100"/>
+      <c r="D93" s="99"/>
       <c r="E93" s="53">
         <v>1200</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="134" t="s">
+      <c r="A94" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="B94" s="112"/>
-      <c r="C94" s="95"/>
+      <c r="B94" s="83"/>
+      <c r="C94" s="90"/>
       <c r="D94" s="81"/>
       <c r="E94" s="67">
         <f>C73</f>
@@ -18183,13 +18186,13 @@
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C95" s="98" t="s">
+      <c r="C95" s="80" t="s">
         <v>29</v>
       </c>
       <c r="D95" s="81"/>
       <c r="E95" s="53">
         <f>(E23+E92)-SUM(E93:E94)</f>
-        <v>307.76999999999953</v>
+        <v>407.76999999999953</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
@@ -21846,34 +21849,18 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="A90:E90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="A82:E82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A76:E76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A28:C28"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="A34:C35"/>
@@ -21882,18 +21869,34 @@
     <mergeCell ref="A50:C50"/>
     <mergeCell ref="A53:C53"/>
     <mergeCell ref="A56:C56"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A76:E76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="A90:E90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="23" priority="2" operator="lessThan">
@@ -21954,7 +21957,7 @@
   <dimension ref="A1:Y1008"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -21971,13 +21974,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="110"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -21999,7 +22002,7 @@
       </c>
       <c r="C3" s="5">
         <f>'January 2025 - March 2025'!E95</f>
-        <v>307.76999999999953</v>
+        <v>407.76999999999953</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -22094,7 +22097,7 @@
       </c>
       <c r="C6" s="5">
         <f>SUM(C3:C5)</f>
-        <v>337.96999999999952</v>
+        <v>437.96999999999952</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -22126,7 +22129,7 @@
       </c>
       <c r="C7" s="58">
         <f>('January 2025 - March 2025'!C7+E95)+SUM(E78,E85,E93)</f>
-        <v>2036.8499999999995</v>
+        <v>2336.8499999999995</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -22180,13 +22183,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="116" t="s">
         <v>135</v>
       </c>
-      <c r="B10" s="114"/>
-      <c r="C10" s="114"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="115"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="86"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -22214,7 +22217,7 @@
       <c r="B11" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="116" t="s">
+      <c r="C11" s="100" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="81"/>
@@ -22229,10 +22232,10 @@
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="111" t="s">
+      <c r="C12" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="112"/>
+      <c r="D12" s="83"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -22254,13 +22257,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="113" t="s">
+      <c r="A15" s="116" t="s">
         <v>143</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="114"/>
-      <c r="D15" s="114"/>
-      <c r="E15" s="115"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="86"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -22288,7 +22291,7 @@
       <c r="B16" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="116" t="s">
+      <c r="C16" s="100" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="81"/>
@@ -22303,7 +22306,7 @@
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="111" t="s">
+      <c r="C17" s="101" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="81"/>
@@ -22331,13 +22334,13 @@
       <c r="E19" s="52"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="113" t="s">
+      <c r="A20" s="116" t="s">
         <v>139</v>
       </c>
-      <c r="B20" s="114"/>
-      <c r="C20" s="114"/>
-      <c r="D20" s="114"/>
-      <c r="E20" s="115"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="86"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -22368,7 +22371,7 @@
       <c r="C21" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="91"/>
+      <c r="D21" s="118"/>
       <c r="E21" s="75" t="s">
         <v>5</v>
       </c>
@@ -22380,10 +22383,10 @@
       <c r="B22" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="118" t="s">
+      <c r="C22" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="119"/>
+      <c r="D22" s="120"/>
       <c r="E22" s="68">
         <v>2405</v>
       </c>
@@ -22426,10 +22429,10 @@
       <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A28" s="148" t="s">
+      <c r="A28" s="140" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="80"/>
+      <c r="B28" s="109"/>
       <c r="C28" s="81"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
@@ -22445,10 +22448,10 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="79" t="s">
+      <c r="A30" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="80"/>
+      <c r="B30" s="109"/>
       <c r="C30" s="81"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
@@ -22482,16 +22485,16 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A34" s="120" t="s">
+      <c r="A34" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="121"/>
-      <c r="C34" s="122"/>
+      <c r="B34" s="103"/>
+      <c r="C34" s="104"/>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="123"/>
-      <c r="B35" s="124"/>
-      <c r="C35" s="125"/>
+      <c r="A35" s="105"/>
+      <c r="B35" s="106"/>
+      <c r="C35" s="107"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
       <c r="A36" s="2" t="s">
@@ -22540,10 +22543,10 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A41" s="79" t="s">
+      <c r="A41" s="110" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="80"/>
+      <c r="B41" s="109"/>
       <c r="C41" s="81"/>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
@@ -22579,11 +22582,11 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A45" s="79" t="s">
+      <c r="A45" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="82"/>
-      <c r="C45" s="83"/>
+      <c r="B45" s="128"/>
+      <c r="C45" s="129"/>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
       <c r="A46" s="2" t="s">
@@ -22625,11 +22628,11 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A50" s="79" t="s">
+      <c r="A50" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="B50" s="82"/>
-      <c r="C50" s="83"/>
+      <c r="B50" s="128"/>
+      <c r="C50" s="129"/>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
       <c r="A51" s="2" t="s">
@@ -22653,11 +22656,11 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A53" s="89" t="s">
+      <c r="A53" s="134" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="90"/>
-      <c r="C53" s="91"/>
+      <c r="B53" s="135"/>
+      <c r="C53" s="118"/>
     </row>
     <row r="54" spans="1:3" ht="33" customHeight="1">
       <c r="A54" s="33" t="s">
@@ -22681,11 +22684,11 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A56" s="129" t="s">
+      <c r="A56" s="139" t="s">
         <v>36</v>
       </c>
-      <c r="B56" s="124"/>
-      <c r="C56" s="115"/>
+      <c r="B56" s="106"/>
+      <c r="C56" s="86"/>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
       <c r="A57" s="27" t="s">
@@ -22729,11 +22732,11 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A61" s="92" t="s">
+      <c r="A61" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="93"/>
-      <c r="C61" s="94"/>
+      <c r="B61" s="136"/>
+      <c r="C61" s="89"/>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
       <c r="A62" s="59" t="s">
@@ -22800,11 +22803,11 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A68" s="92" t="s">
+      <c r="A68" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="136"/>
-      <c r="C68" s="94"/>
+      <c r="B68" s="88"/>
+      <c r="C68" s="89"/>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
       <c r="A69" s="43" t="s">
@@ -22812,8 +22815,8 @@
       </c>
       <c r="B69" s="39"/>
       <c r="C69" s="50">
-        <f>'April 2024 - June 2024'!C70-'April 2024 - June 2024'!E94</f>
-        <v>9739</v>
+        <f>'January 2025 - March 2025'!C69</f>
+        <v>9939</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
@@ -22841,7 +22844,7 @@
       </c>
       <c r="C72" s="50">
         <f>SUM(C69:C71)</f>
-        <v>14739</v>
+        <v>14939</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="13.5" customHeight="1">
@@ -22864,78 +22867,78 @@
       <c r="B75" s="11"/>
     </row>
     <row r="76" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A76" s="86" t="s">
+      <c r="A76" s="92" t="s">
         <v>137</v>
       </c>
-      <c r="B76" s="80"/>
-      <c r="C76" s="80"/>
-      <c r="D76" s="80"/>
+      <c r="B76" s="109"/>
+      <c r="C76" s="109"/>
+      <c r="D76" s="109"/>
       <c r="E76" s="81"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="87" t="s">
+      <c r="A77" s="132" t="s">
         <v>39</v>
       </c>
-      <c r="B77" s="91"/>
-      <c r="C77" s="87" t="s">
+      <c r="B77" s="118"/>
+      <c r="C77" s="132" t="s">
         <v>38</v>
       </c>
-      <c r="D77" s="91"/>
+      <c r="D77" s="118"/>
       <c r="E77" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="144" t="s">
+      <c r="A78" s="143" t="s">
         <v>83</v>
       </c>
-      <c r="B78" s="102"/>
-      <c r="C78" s="142" t="s">
+      <c r="B78" s="95"/>
+      <c r="C78" s="141" t="s">
         <v>150</v>
       </c>
-      <c r="D78" s="143"/>
+      <c r="D78" s="142"/>
       <c r="E78" s="76">
         <v>1200</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="106" t="s">
+      <c r="A79" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="B79" s="107"/>
-      <c r="C79" s="84"/>
-      <c r="D79" s="85"/>
+      <c r="B79" s="123"/>
+      <c r="C79" s="130"/>
+      <c r="D79" s="131"/>
       <c r="E79" s="45">
         <f>C73</f>
         <v>1257</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="C80" s="130" t="s">
+      <c r="C80" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="D80" s="80"/>
+      <c r="D80" s="109"/>
       <c r="E80" s="38">
         <f>(C6+E13)-SUM(E78:E79)</f>
-        <v>285.96999999999935</v>
+        <v>385.96999999999935</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="82" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A82" s="86" t="s">
+      <c r="A82" s="92" t="s">
         <v>145</v>
       </c>
-      <c r="B82" s="80"/>
-      <c r="C82" s="80"/>
-      <c r="D82" s="80"/>
+      <c r="B82" s="109"/>
+      <c r="C82" s="109"/>
+      <c r="D82" s="109"/>
       <c r="E82" s="81"/>
     </row>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="86" t="s">
+      <c r="A83" s="92" t="s">
         <v>39</v>
       </c>
       <c r="B83" s="81"/>
-      <c r="C83" s="86" t="s">
+      <c r="C83" s="92" t="s">
         <v>38</v>
       </c>
       <c r="D83" s="81"/>
@@ -22944,36 +22947,36 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="134" t="s">
+      <c r="A84" s="82" t="s">
         <v>146</v>
       </c>
-      <c r="B84" s="112"/>
-      <c r="C84" s="96"/>
-      <c r="D84" s="141"/>
+      <c r="B84" s="83"/>
+      <c r="C84" s="126"/>
+      <c r="D84" s="149"/>
       <c r="E84" s="38">
         <f>E80</f>
-        <v>285.96999999999935</v>
+        <v>385.96999999999935</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="134" t="s">
+      <c r="A85" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="B85" s="138"/>
-      <c r="C85" s="99" t="s">
+      <c r="B85" s="93"/>
+      <c r="C85" s="98" t="s">
         <v>151</v>
       </c>
-      <c r="D85" s="140"/>
+      <c r="D85" s="148"/>
       <c r="E85" s="53">
-        <v>1339</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="134" t="s">
+      <c r="A86" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="B86" s="112"/>
-      <c r="C86" s="95"/>
+      <c r="B86" s="83"/>
+      <c r="C86" s="90"/>
       <c r="D86" s="81"/>
       <c r="E86" s="67">
         <f>C73</f>
@@ -22981,13 +22984,13 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C87" s="98" t="s">
+      <c r="C87" s="80" t="s">
         <v>29</v>
       </c>
       <c r="D87" s="81"/>
       <c r="E87" s="38">
         <f>(E18+E84)-SUM(E85:E86)</f>
-        <v>94.969999999999345</v>
+        <v>233.96999999999935</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
@@ -23005,20 +23008,20 @@
       <c r="E89" s="25"/>
     </row>
     <row r="90" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A90" s="135" t="s">
+      <c r="A90" s="84" t="s">
         <v>142</v>
       </c>
-      <c r="B90" s="114"/>
-      <c r="C90" s="114"/>
-      <c r="D90" s="114"/>
-      <c r="E90" s="115"/>
+      <c r="B90" s="85"/>
+      <c r="C90" s="85"/>
+      <c r="D90" s="85"/>
+      <c r="E90" s="86"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="86" t="s">
+      <c r="A91" s="92" t="s">
         <v>39</v>
       </c>
       <c r="B91" s="81"/>
-      <c r="C91" s="86" t="s">
+      <c r="C91" s="92" t="s">
         <v>38</v>
       </c>
       <c r="D91" s="81"/>
@@ -23027,34 +23030,36 @@
       </c>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="134" t="s">
+      <c r="A92" s="82" t="s">
         <v>147</v>
       </c>
-      <c r="B92" s="112"/>
-      <c r="C92" s="95"/>
+      <c r="B92" s="83"/>
+      <c r="C92" s="90"/>
       <c r="D92" s="81"/>
       <c r="E92" s="38">
         <f>E87</f>
-        <v>94.969999999999345</v>
+        <v>233.96999999999935</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="134" t="s">
+      <c r="A93" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="B93" s="138"/>
-      <c r="C93" s="99"/>
-      <c r="D93" s="100"/>
+      <c r="B93" s="93"/>
+      <c r="C93" s="98" t="s">
+        <v>152</v>
+      </c>
+      <c r="D93" s="99"/>
       <c r="E93" s="53">
-        <v>0</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="134" t="s">
+      <c r="A94" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="B94" s="112"/>
-      <c r="C94" s="95"/>
+      <c r="B94" s="83"/>
+      <c r="C94" s="90"/>
       <c r="D94" s="81"/>
       <c r="E94" s="67">
         <f>C73</f>
@@ -23062,13 +23067,13 @@
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C95" s="98" t="s">
+      <c r="C95" s="80" t="s">
         <v>29</v>
       </c>
       <c r="D95" s="81"/>
       <c r="E95" s="53">
         <f>(E23+E92)-SUM(E93:E94)</f>
-        <v>1242.9699999999993</v>
+        <v>-57.030000000000655</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
@@ -26725,34 +26730,18 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="A90:E90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="A82:E82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A76:E76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A28:C28"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="A34:C35"/>
@@ -26761,18 +26750,34 @@
     <mergeCell ref="A50:C50"/>
     <mergeCell ref="A53:C53"/>
     <mergeCell ref="A56:C56"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A76:E76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="A90:E90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
docs: Updated the HSBC Account
</commit_message>
<xml_diff>
--- a/Alan Tang_s Income Expense Now.xlsx
+++ b/Alan Tang_s Income Expense Now.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Income-Expenditure-Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27159B14-4B4F-4E60-9165-2B7063F14116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B727C8-FF4E-4F50-A43C-2083928310A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="April 2024 - June 2024" sheetId="1" r:id="rId1"/>
@@ -1546,55 +1546,22 @@
     <xf numFmtId="0" fontId="25" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1603,94 +1570,13 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1705,8 +1591,26 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1716,6 +1620,12 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1729,8 +1639,116 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="22" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1750,23 +1768,11 @@
     <xf numFmtId="166" fontId="22" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1774,16 +1780,10 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2534,8 +2534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1013"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2552,13 +2552,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="113" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="125"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -2579,7 +2579,7 @@
         <v>88</v>
       </c>
       <c r="C3" s="5">
-        <v>944.97</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2610,7 +2610,7 @@
         <v>86</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -2735,7 +2735,7 @@
       </c>
       <c r="C8" s="5">
         <f>SUM(C3:C7)</f>
-        <v>982.17000000000007</v>
+        <v>57.370000000000005</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -2821,13 +2821,13 @@
     </row>
     <row r="11" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="12" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A12" s="126" t="s">
+      <c r="A12" s="118" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="89"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="119"/>
+      <c r="E12" s="108"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
@@ -2855,10 +2855,10 @@
       <c r="B13" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="104" t="s">
+      <c r="C13" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="84"/>
+      <c r="D13" s="92"/>
       <c r="E13" s="17" t="s">
         <v>4</v>
       </c>
@@ -2870,10 +2870,10 @@
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="105" t="s">
+      <c r="C14" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="86"/>
+      <c r="D14" s="117"/>
       <c r="E14" s="18">
         <v>2405</v>
       </c>
@@ -2895,13 +2895,13 @@
       <c r="B16" s="11"/>
     </row>
     <row r="17" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A17" s="126" t="s">
+      <c r="A17" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="88"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="89"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="119"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="108"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
@@ -2929,10 +2929,10 @@
       <c r="B18" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="127" t="s">
+      <c r="C18" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="128"/>
+      <c r="D18" s="97"/>
       <c r="E18" s="74" t="s">
         <v>4</v>
       </c>
@@ -2944,10 +2944,10 @@
       <c r="B19" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="129" t="s">
+      <c r="C19" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="130"/>
+      <c r="D19" s="123"/>
       <c r="E19" s="67">
         <v>2405</v>
       </c>
@@ -2972,13 +2972,13 @@
       <c r="E21" s="51"/>
     </row>
     <row r="22" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A22" s="126" t="s">
+      <c r="A22" s="118" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="88"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="89"/>
+      <c r="B22" s="119"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="108"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
@@ -3006,10 +3006,10 @@
       <c r="B23" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="104" t="s">
+      <c r="C23" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="84"/>
+      <c r="D23" s="92"/>
       <c r="E23" s="17" t="s">
         <v>4</v>
       </c>
@@ -3021,10 +3021,10 @@
       <c r="B24" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="105" t="s">
+      <c r="C24" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="84"/>
+      <c r="D24" s="92"/>
       <c r="E24" s="27">
         <v>2405</v>
       </c>
@@ -3036,10 +3036,10 @@
       <c r="B25" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="C25" s="82" t="s">
+      <c r="C25" s="141" t="s">
         <v>163</v>
       </c>
-      <c r="D25" s="82"/>
+      <c r="D25" s="141"/>
       <c r="E25" s="67">
         <v>50</v>
       </c>
@@ -3051,10 +3051,10 @@
       <c r="B26" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="115" t="s">
+      <c r="C26" s="132" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="116"/>
+      <c r="D26" s="133"/>
       <c r="E26" s="67">
         <v>1035</v>
       </c>
@@ -3090,11 +3090,11 @@
       <c r="B30" s="11"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A31" s="112" t="s">
+      <c r="A31" s="131" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="113"/>
-      <c r="C31" s="84"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="92"/>
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="A32" s="20" t="s">
@@ -3109,11 +3109,11 @@
       <c r="D32" s="22"/>
     </row>
     <row r="33" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A33" s="114" t="s">
+      <c r="A33" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="113"/>
-      <c r="C33" s="84"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="92"/>
     </row>
     <row r="34" spans="1:3" ht="13.5" customHeight="1">
       <c r="A34" s="25" t="s">
@@ -3155,16 +3155,16 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A38" s="106" t="s">
+      <c r="A38" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="107"/>
-      <c r="C38" s="108"/>
+      <c r="B38" s="127"/>
+      <c r="C38" s="128"/>
     </row>
     <row r="39" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A39" s="109"/>
-      <c r="B39" s="110"/>
-      <c r="C39" s="111"/>
+      <c r="A39" s="129"/>
+      <c r="B39" s="107"/>
+      <c r="C39" s="130"/>
     </row>
     <row r="40" spans="1:3" ht="13.5" customHeight="1">
       <c r="A40" s="2" t="s">
@@ -3213,11 +3213,11 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A45" s="114" t="s">
+      <c r="A45" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="113"/>
-      <c r="C45" s="84"/>
+      <c r="B45" s="91"/>
+      <c r="C45" s="92"/>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
       <c r="A46" s="2" t="s">
@@ -3252,11 +3252,11 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A49" s="114" t="s">
+      <c r="A49" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="119"/>
-      <c r="C49" s="120"/>
+      <c r="B49" s="102"/>
+      <c r="C49" s="103"/>
     </row>
     <row r="50" spans="1:3" ht="13.5" customHeight="1">
       <c r="A50" s="2" t="s">
@@ -3298,11 +3298,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="114" t="s">
+      <c r="A54" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="B54" s="119"/>
-      <c r="C54" s="120"/>
+      <c r="B54" s="102"/>
+      <c r="C54" s="103"/>
     </row>
     <row r="55" spans="1:3" ht="13.5" customHeight="1">
       <c r="A55" s="2" t="s">
@@ -3326,11 +3326,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="133" t="s">
+      <c r="A57" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="134"/>
-      <c r="C57" s="128"/>
+      <c r="B57" s="96"/>
+      <c r="C57" s="97"/>
     </row>
     <row r="58" spans="1:3" ht="33" customHeight="1">
       <c r="A58" s="32" t="s">
@@ -3354,11 +3354,11 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A60" s="138" t="s">
+      <c r="A60" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="B60" s="110"/>
-      <c r="C60" s="89"/>
+      <c r="B60" s="107"/>
+      <c r="C60" s="108"/>
     </row>
     <row r="61" spans="1:3" ht="13.5" customHeight="1">
       <c r="A61" s="26" t="s">
@@ -3402,11 +3402,11 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A65" s="90" t="s">
+      <c r="A65" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="135"/>
-      <c r="C65" s="92"/>
+      <c r="B65" s="99"/>
+      <c r="C65" s="100"/>
     </row>
     <row r="66" spans="1:8" ht="13.5" customHeight="1">
       <c r="A66" s="58" t="s">
@@ -3462,11 +3462,11 @@
       </c>
     </row>
     <row r="71" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A71" s="90" t="s">
+      <c r="A71" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B71" s="91"/>
-      <c r="C71" s="92"/>
+      <c r="B71" s="144"/>
+      <c r="C71" s="100"/>
     </row>
     <row r="72" spans="1:8" ht="13.5" customHeight="1">
       <c r="A72" s="42" t="s">
@@ -3525,129 +3525,129 @@
       <c r="B78" s="11"/>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="95" t="s">
+      <c r="A79" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="B79" s="136"/>
-      <c r="C79" s="136"/>
-      <c r="D79" s="136"/>
-      <c r="E79" s="137"/>
+      <c r="B79" s="104"/>
+      <c r="C79" s="104"/>
+      <c r="D79" s="104"/>
+      <c r="E79" s="105"/>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="131" t="s">
+      <c r="A80" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="B80" s="132"/>
-      <c r="C80" s="131" t="s">
+      <c r="B80" s="94"/>
+      <c r="C80" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="D80" s="132"/>
+      <c r="D80" s="94"/>
       <c r="E80" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A81" s="139" t="s">
+      <c r="A81" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="B81" s="140"/>
-      <c r="C81" s="121"/>
-      <c r="D81" s="122"/>
+      <c r="B81" s="110"/>
+      <c r="C81" s="139"/>
+      <c r="D81" s="140"/>
       <c r="E81" s="44">
         <f>C76</f>
         <v>1503</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C82" s="141" t="s">
+      <c r="C82" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="D82" s="142"/>
+      <c r="D82" s="112"/>
       <c r="E82" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="95" t="s">
+      <c r="A84" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="B84" s="113"/>
-      <c r="C84" s="113"/>
-      <c r="D84" s="113"/>
-      <c r="E84" s="84"/>
+      <c r="B84" s="91"/>
+      <c r="C84" s="91"/>
+      <c r="D84" s="91"/>
+      <c r="E84" s="92"/>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="95" t="s">
+      <c r="A85" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B85" s="84"/>
-      <c r="C85" s="95" t="s">
+      <c r="B85" s="92"/>
+      <c r="C85" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D85" s="84"/>
+      <c r="D85" s="92"/>
       <c r="E85" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="85" t="s">
+      <c r="A86" s="142" t="s">
         <v>77</v>
       </c>
-      <c r="B86" s="96"/>
-      <c r="C86" s="93"/>
-      <c r="D86" s="94"/>
+      <c r="B86" s="146"/>
+      <c r="C86" s="134"/>
+      <c r="D86" s="145"/>
       <c r="E86" s="37">
         <f>E82</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="97" t="s">
+      <c r="A87" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="B87" s="98"/>
-      <c r="C87" s="101" t="s">
+      <c r="B87" s="85"/>
+      <c r="C87" s="124" t="s">
         <v>83</v>
       </c>
-      <c r="D87" s="102"/>
+      <c r="D87" s="138"/>
       <c r="E87" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A88" s="99"/>
-      <c r="B88" s="100"/>
-      <c r="C88" s="101" t="s">
+      <c r="A88" s="88"/>
+      <c r="B88" s="89"/>
+      <c r="C88" s="124" t="s">
         <v>91</v>
       </c>
-      <c r="D88" s="103"/>
+      <c r="D88" s="125"/>
       <c r="E88" s="52">
         <v>1000</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A89" s="85" t="s">
+      <c r="A89" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B89" s="86"/>
-      <c r="C89" s="117" t="s">
+      <c r="B89" s="117"/>
+      <c r="C89" s="135" t="s">
         <v>92</v>
       </c>
-      <c r="D89" s="118"/>
+      <c r="D89" s="136"/>
       <c r="E89" s="66">
         <f>C76</f>
         <v>1503</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C90" s="83" t="s">
+      <c r="C90" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="D90" s="84"/>
+      <c r="D90" s="92"/>
       <c r="E90" s="37">
         <f>SUM(C3:C7)</f>
-        <v>982.17000000000007</v>
+        <v>57.370000000000005</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
@@ -3665,90 +3665,90 @@
       <c r="E92" s="24"/>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="87" t="s">
+      <c r="A93" s="143" t="s">
         <v>64</v>
       </c>
-      <c r="B93" s="88"/>
-      <c r="C93" s="88"/>
-      <c r="D93" s="88"/>
-      <c r="E93" s="89"/>
+      <c r="B93" s="119"/>
+      <c r="C93" s="119"/>
+      <c r="D93" s="119"/>
+      <c r="E93" s="108"/>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="95" t="s">
+      <c r="A94" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B94" s="84"/>
-      <c r="C94" s="95" t="s">
+      <c r="B94" s="92"/>
+      <c r="C94" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D94" s="84"/>
+      <c r="D94" s="92"/>
       <c r="E94" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="85" t="s">
+      <c r="A95" s="142" t="s">
         <v>78</v>
       </c>
-      <c r="B95" s="86"/>
-      <c r="C95" s="93"/>
-      <c r="D95" s="84"/>
+      <c r="B95" s="117"/>
+      <c r="C95" s="134"/>
+      <c r="D95" s="92"/>
       <c r="E95" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A96" s="97" t="s">
+      <c r="A96" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="B96" s="98"/>
-      <c r="C96" s="101" t="s">
+      <c r="B96" s="85"/>
+      <c r="C96" s="124" t="s">
         <v>83</v>
       </c>
-      <c r="D96" s="102"/>
+      <c r="D96" s="138"/>
       <c r="E96" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A97" s="158"/>
-      <c r="B97" s="159"/>
-      <c r="C97" s="101" t="s">
+      <c r="A97" s="86"/>
+      <c r="B97" s="87"/>
+      <c r="C97" s="124" t="s">
         <v>169</v>
       </c>
-      <c r="D97" s="103"/>
+      <c r="D97" s="125"/>
       <c r="E97" s="52">
         <v>1500</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A98" s="99"/>
-      <c r="B98" s="100"/>
-      <c r="C98" s="160" t="s">
+      <c r="A98" s="88"/>
+      <c r="B98" s="89"/>
+      <c r="C98" s="82" t="s">
         <v>170</v>
       </c>
-      <c r="D98" s="161"/>
+      <c r="D98" s="83"/>
       <c r="E98" s="52">
         <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A99" s="85" t="s">
+      <c r="A99" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B99" s="96"/>
-      <c r="C99" s="117"/>
-      <c r="D99" s="118"/>
+      <c r="B99" s="146"/>
+      <c r="C99" s="135"/>
+      <c r="D99" s="136"/>
       <c r="E99" s="52">
         <f>C76</f>
         <v>1503</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C100" s="83" t="s">
+      <c r="C100" s="137" t="s">
         <v>29</v>
       </c>
-      <c r="D100" s="84"/>
+      <c r="D100" s="92"/>
       <c r="E100" s="52">
         <f>(E27+E95)-SUM(E96:E99)</f>
         <v>477</v>
@@ -7408,39 +7408,6 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="A96:B98"/>
-    <mergeCell ref="A84:E84"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A79:E79"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="A87:B88"/>
-    <mergeCell ref="C88:D88"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="A54:C54"/>
     <mergeCell ref="C81:D81"/>
@@ -7457,6 +7424,39 @@
     <mergeCell ref="A86:B86"/>
     <mergeCell ref="C96:D96"/>
     <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A79:E79"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="A96:B98"/>
+    <mergeCell ref="A84:E84"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="A87:B88"/>
+    <mergeCell ref="C88:D88"/>
     <mergeCell ref="C94:D94"/>
     <mergeCell ref="A94:B94"/>
   </mergeCells>
@@ -7515,7 +7515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5F3FA5-5013-4B35-A74B-6269617B858B}">
   <dimension ref="A1:Y1014"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -7533,13 +7533,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="113" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="125"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -7742,13 +7742,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="126" t="s">
+      <c r="A10" s="118" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="89"/>
+      <c r="B10" s="119"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="108"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -7776,10 +7776,10 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="104" t="s">
+      <c r="C11" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="84"/>
+      <c r="D11" s="92"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
@@ -7791,10 +7791,10 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="105" t="s">
+      <c r="C12" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="86"/>
+      <c r="D12" s="117"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -7816,13 +7816,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="126" t="s">
+      <c r="A15" s="118" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="88"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="89"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="108"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -7850,10 +7850,10 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="104" t="s">
+      <c r="C16" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="84"/>
+      <c r="D16" s="92"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
@@ -7865,10 +7865,10 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="105" t="s">
+      <c r="C17" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="84"/>
+      <c r="D17" s="92"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -7893,13 +7893,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="126" t="s">
+      <c r="A20" s="118" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="88"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="89"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="108"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -7927,10 +7927,10 @@
       <c r="B21" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="127" t="s">
+      <c r="C21" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="128"/>
+      <c r="D21" s="97"/>
       <c r="E21" s="74" t="s">
         <v>4</v>
       </c>
@@ -7942,10 +7942,10 @@
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="129" t="s">
+      <c r="C22" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="130"/>
+      <c r="D22" s="123"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -7955,8 +7955,8 @@
       <c r="B23" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="C23" s="129"/>
-      <c r="D23" s="129"/>
+      <c r="C23" s="122"/>
+      <c r="D23" s="122"/>
       <c r="E23" s="67">
         <v>204</v>
       </c>
@@ -7999,11 +7999,11 @@
       <c r="B28" s="11"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A29" s="143" t="s">
+      <c r="A29" s="156" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="113"/>
-      <c r="C29" s="84"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="92"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
       <c r="A30" s="20" t="s">
@@ -8018,11 +8018,11 @@
       <c r="D30" s="22"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A31" s="114" t="s">
+      <c r="A31" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="113"/>
-      <c r="C31" s="84"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="92"/>
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="A32" s="25" t="s">
@@ -8064,16 +8064,16 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="106" t="s">
+      <c r="A36" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="107"/>
-      <c r="C36" s="108"/>
+      <c r="B36" s="127"/>
+      <c r="C36" s="128"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A37" s="109"/>
-      <c r="B37" s="110"/>
-      <c r="C37" s="111"/>
+      <c r="A37" s="129"/>
+      <c r="B37" s="107"/>
+      <c r="C37" s="130"/>
     </row>
     <row r="38" spans="1:3" ht="13.5" customHeight="1">
       <c r="A38" s="2" t="s">
@@ -8122,11 +8122,11 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A43" s="114" t="s">
+      <c r="A43" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="113"/>
-      <c r="C43" s="84"/>
+      <c r="B43" s="91"/>
+      <c r="C43" s="92"/>
     </row>
     <row r="44" spans="1:3" ht="13.5" customHeight="1">
       <c r="A44" s="2" t="s">
@@ -8161,11 +8161,11 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A47" s="114" t="s">
+      <c r="A47" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="119"/>
-      <c r="C47" s="120"/>
+      <c r="B47" s="102"/>
+      <c r="C47" s="103"/>
     </row>
     <row r="48" spans="1:3" ht="13.5" customHeight="1">
       <c r="A48" s="2" t="s">
@@ -8207,11 +8207,11 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A52" s="114" t="s">
+      <c r="A52" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="B52" s="119"/>
-      <c r="C52" s="120"/>
+      <c r="B52" s="102"/>
+      <c r="C52" s="103"/>
     </row>
     <row r="53" spans="1:3" ht="13.5" customHeight="1">
       <c r="A53" s="2" t="s">
@@ -8235,11 +8235,11 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A55" s="133" t="s">
+      <c r="A55" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="134"/>
-      <c r="C55" s="128"/>
+      <c r="B55" s="96"/>
+      <c r="C55" s="97"/>
     </row>
     <row r="56" spans="1:3" ht="33" customHeight="1">
       <c r="A56" s="32" t="s">
@@ -8263,11 +8263,11 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A58" s="138" t="s">
+      <c r="A58" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="110"/>
-      <c r="C58" s="89"/>
+      <c r="B58" s="107"/>
+      <c r="C58" s="108"/>
     </row>
     <row r="59" spans="1:3" ht="13.5" customHeight="1">
       <c r="A59" s="26" t="s">
@@ -8311,11 +8311,11 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A63" s="90" t="s">
+      <c r="A63" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B63" s="135"/>
-      <c r="C63" s="92"/>
+      <c r="B63" s="99"/>
+      <c r="C63" s="100"/>
     </row>
     <row r="64" spans="1:3" ht="13.5" customHeight="1">
       <c r="A64" s="58" t="s">
@@ -8382,11 +8382,11 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A70" s="90" t="s">
+      <c r="A70" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B70" s="91"/>
-      <c r="C70" s="92"/>
+      <c r="B70" s="144"/>
+      <c r="C70" s="100"/>
     </row>
     <row r="71" spans="1:8" ht="13.5" customHeight="1">
       <c r="A71" s="42" t="s">
@@ -8446,68 +8446,68 @@
       <c r="B77" s="11"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="95" t="s">
+      <c r="A78" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="B78" s="113"/>
-      <c r="C78" s="113"/>
-      <c r="D78" s="113"/>
-      <c r="E78" s="84"/>
+      <c r="B78" s="91"/>
+      <c r="C78" s="91"/>
+      <c r="D78" s="91"/>
+      <c r="E78" s="92"/>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="131" t="s">
+      <c r="A79" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="B79" s="128"/>
-      <c r="C79" s="131" t="s">
+      <c r="B79" s="97"/>
+      <c r="C79" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="D79" s="128"/>
+      <c r="D79" s="97"/>
       <c r="E79" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="146" t="s">
+      <c r="A80" s="152" t="s">
         <v>82</v>
       </c>
-      <c r="B80" s="146"/>
-      <c r="C80" s="144" t="s">
+      <c r="B80" s="152"/>
+      <c r="C80" s="150" t="s">
         <v>83</v>
       </c>
-      <c r="D80" s="145"/>
+      <c r="D80" s="151"/>
       <c r="E80" s="75">
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A81" s="147"/>
-      <c r="B81" s="147"/>
-      <c r="C81" s="148" t="s">
+      <c r="A81" s="153"/>
+      <c r="B81" s="153"/>
+      <c r="C81" s="154" t="s">
         <v>119</v>
       </c>
-      <c r="D81" s="149"/>
+      <c r="D81" s="155"/>
       <c r="E81" s="52">
         <v>850</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A82" s="139" t="s">
+      <c r="A82" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="B82" s="140"/>
-      <c r="C82" s="121"/>
-      <c r="D82" s="122"/>
+      <c r="B82" s="110"/>
+      <c r="C82" s="139"/>
+      <c r="D82" s="140"/>
       <c r="E82" s="44">
         <f>C75</f>
         <v>1503</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C83" s="141" t="s">
+      <c r="C83" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="D83" s="113"/>
+      <c r="D83" s="91"/>
       <c r="E83" s="37">
         <f>(C6+E13)-SUM(E80:E82)</f>
         <v>555.19999999999982</v>
@@ -8515,91 +8515,91 @@
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="95" t="s">
+      <c r="A85" s="90" t="s">
         <v>101</v>
       </c>
-      <c r="B85" s="113"/>
-      <c r="C85" s="113"/>
-      <c r="D85" s="113"/>
-      <c r="E85" s="84"/>
+      <c r="B85" s="91"/>
+      <c r="C85" s="91"/>
+      <c r="D85" s="91"/>
+      <c r="E85" s="92"/>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="95" t="s">
+      <c r="A86" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B86" s="84"/>
-      <c r="C86" s="95" t="s">
+      <c r="B86" s="92"/>
+      <c r="C86" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D86" s="84"/>
+      <c r="D86" s="92"/>
       <c r="E86" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="85" t="s">
+      <c r="A87" s="142" t="s">
         <v>81</v>
       </c>
-      <c r="B87" s="86"/>
-      <c r="C87" s="117"/>
-      <c r="D87" s="152"/>
+      <c r="B87" s="117"/>
+      <c r="C87" s="135"/>
+      <c r="D87" s="149"/>
       <c r="E87" s="37">
         <f>E83</f>
         <v>555.19999999999982</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A88" s="97" t="s">
+      <c r="A88" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="B88" s="98"/>
-      <c r="C88" s="117" t="s">
+      <c r="B88" s="85"/>
+      <c r="C88" s="135" t="s">
         <v>83</v>
       </c>
-      <c r="D88" s="151"/>
+      <c r="D88" s="148"/>
       <c r="E88" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A89" s="158"/>
-      <c r="B89" s="159"/>
-      <c r="C89" s="101" t="s">
+      <c r="A89" s="86"/>
+      <c r="B89" s="87"/>
+      <c r="C89" s="124" t="s">
         <v>119</v>
       </c>
-      <c r="D89" s="150"/>
+      <c r="D89" s="147"/>
       <c r="E89" s="52">
         <v>850</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A90" s="99"/>
-      <c r="B90" s="100"/>
-      <c r="C90" s="101" t="s">
+      <c r="A90" s="88"/>
+      <c r="B90" s="89"/>
+      <c r="C90" s="124" t="s">
         <v>172</v>
       </c>
-      <c r="D90" s="150"/>
+      <c r="D90" s="147"/>
       <c r="E90" s="52">
         <v>187</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="85" t="s">
+      <c r="A91" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B91" s="86"/>
-      <c r="C91" s="93"/>
-      <c r="D91" s="84"/>
+      <c r="B91" s="117"/>
+      <c r="C91" s="134"/>
+      <c r="D91" s="92"/>
       <c r="E91" s="66">
         <f>C75</f>
         <v>1503</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C92" s="83" t="s">
+      <c r="C92" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="D92" s="84"/>
+      <c r="D92" s="92"/>
       <c r="E92" s="37">
         <f>(E18+E87)-SUM(E88:E91)</f>
         <v>420.19999999999982</v>
@@ -8620,48 +8620,48 @@
       <c r="E94" s="24"/>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="87" t="s">
+      <c r="A95" s="143" t="s">
         <v>102</v>
       </c>
-      <c r="B95" s="88"/>
-      <c r="C95" s="88"/>
-      <c r="D95" s="88"/>
-      <c r="E95" s="89"/>
+      <c r="B95" s="119"/>
+      <c r="C95" s="119"/>
+      <c r="D95" s="119"/>
+      <c r="E95" s="108"/>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A96" s="95" t="s">
+      <c r="A96" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B96" s="84"/>
-      <c r="C96" s="95" t="s">
+      <c r="B96" s="92"/>
+      <c r="C96" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D96" s="84"/>
+      <c r="D96" s="92"/>
       <c r="E96" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A97" s="85" t="s">
+      <c r="A97" s="142" t="s">
         <v>103</v>
       </c>
-      <c r="B97" s="86"/>
-      <c r="C97" s="93"/>
-      <c r="D97" s="84"/>
+      <c r="B97" s="117"/>
+      <c r="C97" s="134"/>
+      <c r="D97" s="92"/>
       <c r="E97" s="37">
         <f>E92</f>
         <v>420.19999999999982</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A98" s="85" t="s">
+      <c r="A98" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="B98" s="96"/>
-      <c r="C98" s="101" t="s">
+      <c r="B98" s="146"/>
+      <c r="C98" s="124" t="s">
         <v>83</v>
       </c>
-      <c r="D98" s="102"/>
+      <c r="D98" s="138"/>
       <c r="E98" s="52">
         <v>0</v>
       </c>
@@ -8669,31 +8669,31 @@
     <row r="99" spans="1:5" ht="13.5" customHeight="1">
       <c r="A99" s="76"/>
       <c r="B99" s="77"/>
-      <c r="C99" s="101" t="s">
+      <c r="C99" s="124" t="s">
         <v>171</v>
       </c>
-      <c r="D99" s="150"/>
+      <c r="D99" s="147"/>
       <c r="E99" s="52">
         <v>800</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A100" s="85" t="s">
+      <c r="A100" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B100" s="86"/>
-      <c r="C100" s="93"/>
-      <c r="D100" s="84"/>
+      <c r="B100" s="117"/>
+      <c r="C100" s="134"/>
+      <c r="D100" s="92"/>
       <c r="E100" s="66">
         <f>C75</f>
         <v>1503</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C101" s="83" t="s">
+      <c r="C101" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="D101" s="84"/>
+      <c r="D101" s="92"/>
       <c r="E101" s="52">
         <f>(E24+E97)-SUM(E98:E100)</f>
         <v>726.19999999999982</v>
@@ -12353,6 +12353,43 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="A95:E95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="A80:B81"/>
+    <mergeCell ref="C81:D81"/>
     <mergeCell ref="A88:B90"/>
     <mergeCell ref="C89:D89"/>
     <mergeCell ref="C23:D23"/>
@@ -12369,43 +12406,6 @@
     <mergeCell ref="C82:D82"/>
     <mergeCell ref="A36:C37"/>
     <mergeCell ref="A43:C43"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="A95:E95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="A80:B81"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A78:E78"/>
-    <mergeCell ref="A79:B79"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="59" priority="2" operator="lessThan">
@@ -12484,13 +12484,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="125"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -12693,13 +12693,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="126" t="s">
+      <c r="A10" s="118" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="89"/>
+      <c r="B10" s="119"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="108"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -12727,10 +12727,10 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="104" t="s">
+      <c r="C11" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="84"/>
+      <c r="D11" s="92"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
@@ -12742,10 +12742,10 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="105" t="s">
+      <c r="C12" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="86"/>
+      <c r="D12" s="117"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -12767,13 +12767,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="126" t="s">
+      <c r="A15" s="118" t="s">
         <v>113</v>
       </c>
-      <c r="B15" s="88"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="89"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="108"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -12801,10 +12801,10 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="104" t="s">
+      <c r="C16" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="84"/>
+      <c r="D16" s="92"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
@@ -12816,10 +12816,10 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="105" t="s">
+      <c r="C17" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="84"/>
+      <c r="D17" s="92"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -12844,13 +12844,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="126" t="s">
+      <c r="A20" s="118" t="s">
         <v>109</v>
       </c>
-      <c r="B20" s="88"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="89"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="108"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -12878,10 +12878,10 @@
       <c r="B21" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="127" t="s">
+      <c r="C21" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="128"/>
+      <c r="D21" s="97"/>
       <c r="E21" s="74" t="s">
         <v>4</v>
       </c>
@@ -12893,10 +12893,10 @@
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="129" t="s">
+      <c r="C22" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="130"/>
+      <c r="D22" s="123"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -12939,11 +12939,11 @@
       <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A28" s="143" t="s">
+      <c r="A28" s="156" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="113"/>
-      <c r="C28" s="84"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="92"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="20" t="s">
@@ -12958,11 +12958,11 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="114" t="s">
+      <c r="A30" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="113"/>
-      <c r="C30" s="84"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="92"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="25" t="s">
@@ -13004,16 +13004,16 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="106" t="s">
+      <c r="A35" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="107"/>
-      <c r="C35" s="108"/>
+      <c r="B35" s="127"/>
+      <c r="C35" s="128"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="109"/>
-      <c r="B36" s="110"/>
-      <c r="C36" s="111"/>
+      <c r="A36" s="129"/>
+      <c r="B36" s="107"/>
+      <c r="C36" s="130"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -13062,11 +13062,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A42" s="114" t="s">
+      <c r="A42" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="113"/>
-      <c r="C42" s="84"/>
+      <c r="B42" s="91"/>
+      <c r="C42" s="92"/>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
@@ -13101,11 +13101,11 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A46" s="114" t="s">
+      <c r="A46" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="119"/>
-      <c r="C46" s="120"/>
+      <c r="B46" s="102"/>
+      <c r="C46" s="103"/>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -13147,11 +13147,11 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="114" t="s">
+      <c r="A51" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="119"/>
-      <c r="C51" s="120"/>
+      <c r="B51" s="102"/>
+      <c r="C51" s="103"/>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="2" t="s">
@@ -13175,11 +13175,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="133" t="s">
+      <c r="A54" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="134"/>
-      <c r="C54" s="128"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="97"/>
     </row>
     <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="32" t="s">
@@ -13203,11 +13203,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="138" t="s">
+      <c r="A57" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="110"/>
-      <c r="C57" s="89"/>
+      <c r="B57" s="107"/>
+      <c r="C57" s="108"/>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
       <c r="A58" s="26" t="s">
@@ -13251,11 +13251,11 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A62" s="90" t="s">
+      <c r="A62" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="135"/>
-      <c r="C62" s="92"/>
+      <c r="B62" s="99"/>
+      <c r="C62" s="100"/>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
       <c r="A63" s="58" t="s">
@@ -13322,11 +13322,11 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A69" s="90" t="s">
+      <c r="A69" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="91"/>
-      <c r="C69" s="92"/>
+      <c r="B69" s="144"/>
+      <c r="C69" s="100"/>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
       <c r="A70" s="42" t="s">
@@ -13386,57 +13386,57 @@
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="95" t="s">
+      <c r="A77" s="90" t="s">
         <v>106</v>
       </c>
-      <c r="B77" s="113"/>
-      <c r="C77" s="113"/>
-      <c r="D77" s="113"/>
-      <c r="E77" s="84"/>
+      <c r="B77" s="91"/>
+      <c r="C77" s="91"/>
+      <c r="D77" s="91"/>
+      <c r="E77" s="92"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="131" t="s">
+      <c r="A78" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="B78" s="128"/>
-      <c r="C78" s="131" t="s">
+      <c r="B78" s="97"/>
+      <c r="C78" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="128"/>
+      <c r="D78" s="97"/>
       <c r="E78" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="146" t="s">
+      <c r="A79" s="152" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="98"/>
-      <c r="C79" s="144" t="s">
+      <c r="B79" s="85"/>
+      <c r="C79" s="150" t="s">
         <v>147</v>
       </c>
-      <c r="D79" s="145"/>
+      <c r="D79" s="151"/>
       <c r="E79" s="75">
         <v>1200</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="139" t="s">
+      <c r="A80" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="140"/>
-      <c r="C80" s="121"/>
-      <c r="D80" s="122"/>
+      <c r="B80" s="110"/>
+      <c r="C80" s="139"/>
+      <c r="D80" s="140"/>
       <c r="E80" s="44">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C81" s="141" t="s">
+      <c r="C81" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="D81" s="113"/>
+      <c r="D81" s="91"/>
       <c r="E81" s="37">
         <f>(C6+E13)-SUM(E79:E80)</f>
         <v>658.39999999999964</v>
@@ -13444,69 +13444,69 @@
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="95" t="s">
+      <c r="A83" s="90" t="s">
         <v>115</v>
       </c>
-      <c r="B83" s="113"/>
-      <c r="C83" s="113"/>
-      <c r="D83" s="113"/>
-      <c r="E83" s="84"/>
+      <c r="B83" s="91"/>
+      <c r="C83" s="91"/>
+      <c r="D83" s="91"/>
+      <c r="E83" s="92"/>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="95" t="s">
+      <c r="A84" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="84"/>
-      <c r="C84" s="95" t="s">
+      <c r="B84" s="92"/>
+      <c r="C84" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="84"/>
+      <c r="D84" s="92"/>
       <c r="E84" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="85" t="s">
+      <c r="A85" s="142" t="s">
         <v>107</v>
       </c>
-      <c r="B85" s="86"/>
-      <c r="C85" s="117"/>
-      <c r="D85" s="152"/>
+      <c r="B85" s="117"/>
+      <c r="C85" s="135"/>
+      <c r="D85" s="149"/>
       <c r="E85" s="37">
         <f>E81</f>
         <v>658.39999999999964</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="85" t="s">
+      <c r="A86" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="B86" s="96"/>
-      <c r="C86" s="101" t="s">
+      <c r="B86" s="146"/>
+      <c r="C86" s="124" t="s">
         <v>147</v>
       </c>
-      <c r="D86" s="151"/>
+      <c r="D86" s="148"/>
       <c r="E86" s="52">
         <v>1200</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="85" t="s">
+      <c r="A87" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="86"/>
-      <c r="C87" s="93"/>
-      <c r="D87" s="84"/>
+      <c r="B87" s="117"/>
+      <c r="C87" s="134"/>
+      <c r="D87" s="92"/>
       <c r="E87" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C88" s="83" t="s">
+      <c r="C88" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="84"/>
+      <c r="D88" s="92"/>
       <c r="E88" s="37">
         <f>(E18+E85)-SUM(E86:E87)</f>
         <v>564.39999999999964</v>
@@ -13527,69 +13527,69 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="87" t="s">
+      <c r="A91" s="143" t="s">
         <v>112</v>
       </c>
-      <c r="B91" s="88"/>
-      <c r="C91" s="88"/>
-      <c r="D91" s="88"/>
-      <c r="E91" s="89"/>
+      <c r="B91" s="119"/>
+      <c r="C91" s="119"/>
+      <c r="D91" s="119"/>
+      <c r="E91" s="108"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="95" t="s">
+      <c r="A92" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B92" s="84"/>
-      <c r="C92" s="95" t="s">
+      <c r="B92" s="92"/>
+      <c r="C92" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D92" s="84"/>
+      <c r="D92" s="92"/>
       <c r="E92" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="85" t="s">
+      <c r="A93" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="B93" s="86"/>
-      <c r="C93" s="93"/>
-      <c r="D93" s="84"/>
+      <c r="B93" s="117"/>
+      <c r="C93" s="134"/>
+      <c r="D93" s="92"/>
       <c r="E93" s="37">
         <f>E88</f>
         <v>564.39999999999964</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="85" t="s">
+      <c r="A94" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="96"/>
-      <c r="C94" s="101" t="s">
+      <c r="B94" s="146"/>
+      <c r="C94" s="124" t="s">
         <v>147</v>
       </c>
-      <c r="D94" s="102"/>
+      <c r="D94" s="138"/>
       <c r="E94" s="52">
         <v>1200</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="85" t="s">
+      <c r="A95" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B95" s="86"/>
-      <c r="C95" s="93"/>
-      <c r="D95" s="84"/>
+      <c r="B95" s="117"/>
+      <c r="C95" s="134"/>
+      <c r="D95" s="92"/>
       <c r="E95" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C96" s="83" t="s">
+      <c r="C96" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="D96" s="84"/>
+      <c r="D96" s="92"/>
       <c r="E96" s="52">
         <f>(E23+E93)-SUM(E94:E95)</f>
         <v>470.39999999999964</v>
@@ -17249,11 +17249,36 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A35:C36"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A77:E77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="A86:B86"/>
     <mergeCell ref="C88:D88"/>
@@ -17267,36 +17292,11 @@
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="C84:D84"/>
     <mergeCell ref="C79:D79"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="A77:E77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A35:C36"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="47" priority="2" operator="lessThan">
@@ -17374,13 +17374,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="113" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="125"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -17583,13 +17583,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="126" t="s">
+      <c r="A10" s="118" t="s">
         <v>122</v>
       </c>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="89"/>
+      <c r="B10" s="119"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="108"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -17617,10 +17617,10 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="104" t="s">
+      <c r="C11" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="84"/>
+      <c r="D11" s="92"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
@@ -17632,10 +17632,10 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="105" t="s">
+      <c r="C12" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="86"/>
+      <c r="D12" s="117"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -17657,13 +17657,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="126" t="s">
+      <c r="A15" s="118" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="88"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="89"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="108"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -17691,10 +17691,10 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="104" t="s">
+      <c r="C16" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="84"/>
+      <c r="D16" s="92"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
@@ -17706,10 +17706,10 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="105" t="s">
+      <c r="C17" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="84"/>
+      <c r="D17" s="92"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -17734,13 +17734,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="126" t="s">
+      <c r="A20" s="118" t="s">
         <v>124</v>
       </c>
-      <c r="B20" s="88"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="89"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="108"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -17768,10 +17768,10 @@
       <c r="B21" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="127" t="s">
+      <c r="C21" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="128"/>
+      <c r="D21" s="97"/>
       <c r="E21" s="74" t="s">
         <v>4</v>
       </c>
@@ -17783,10 +17783,10 @@
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="129" t="s">
+      <c r="C22" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="130"/>
+      <c r="D22" s="123"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -17829,11 +17829,11 @@
       <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A28" s="143" t="s">
+      <c r="A28" s="156" t="s">
         <v>126</v>
       </c>
-      <c r="B28" s="113"/>
-      <c r="C28" s="84"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="92"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="20" t="s">
@@ -17848,11 +17848,11 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="114" t="s">
+      <c r="A30" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="113"/>
-      <c r="C30" s="84"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="92"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="25" t="s">
@@ -17894,16 +17894,16 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="106" t="s">
+      <c r="A35" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="107"/>
-      <c r="C35" s="108"/>
+      <c r="B35" s="127"/>
+      <c r="C35" s="128"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="109"/>
-      <c r="B36" s="110"/>
-      <c r="C36" s="111"/>
+      <c r="A36" s="129"/>
+      <c r="B36" s="107"/>
+      <c r="C36" s="130"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -17952,11 +17952,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A42" s="114" t="s">
+      <c r="A42" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="113"/>
-      <c r="C42" s="84"/>
+      <c r="B42" s="91"/>
+      <c r="C42" s="92"/>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
@@ -17991,11 +17991,11 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A46" s="114" t="s">
+      <c r="A46" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="119"/>
-      <c r="C46" s="120"/>
+      <c r="B46" s="102"/>
+      <c r="C46" s="103"/>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -18037,11 +18037,11 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="114" t="s">
+      <c r="A51" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="119"/>
-      <c r="C51" s="120"/>
+      <c r="B51" s="102"/>
+      <c r="C51" s="103"/>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="2" t="s">
@@ -18065,11 +18065,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="133" t="s">
+      <c r="A54" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="134"/>
-      <c r="C54" s="128"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="97"/>
     </row>
     <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="32" t="s">
@@ -18093,11 +18093,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="138" t="s">
+      <c r="A57" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="110"/>
-      <c r="C57" s="89"/>
+      <c r="B57" s="107"/>
+      <c r="C57" s="108"/>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
       <c r="A58" s="26" t="s">
@@ -18141,11 +18141,11 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A62" s="90" t="s">
+      <c r="A62" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="135"/>
-      <c r="C62" s="92"/>
+      <c r="B62" s="99"/>
+      <c r="C62" s="100"/>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
       <c r="A63" s="58" t="s">
@@ -18212,11 +18212,11 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A69" s="90" t="s">
+      <c r="A69" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="91"/>
-      <c r="C69" s="92"/>
+      <c r="B69" s="144"/>
+      <c r="C69" s="100"/>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
       <c r="A70" s="42" t="s">
@@ -18276,57 +18276,57 @@
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="95" t="s">
+      <c r="A77" s="90" t="s">
         <v>127</v>
       </c>
-      <c r="B77" s="113"/>
-      <c r="C77" s="113"/>
-      <c r="D77" s="113"/>
-      <c r="E77" s="84"/>
+      <c r="B77" s="91"/>
+      <c r="C77" s="91"/>
+      <c r="D77" s="91"/>
+      <c r="E77" s="92"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="131" t="s">
+      <c r="A78" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="B78" s="128"/>
-      <c r="C78" s="131" t="s">
+      <c r="B78" s="97"/>
+      <c r="C78" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="128"/>
+      <c r="D78" s="97"/>
       <c r="E78" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="146" t="s">
+      <c r="A79" s="152" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="98"/>
-      <c r="C79" s="144" t="s">
+      <c r="B79" s="85"/>
+      <c r="C79" s="150" t="s">
         <v>147</v>
       </c>
-      <c r="D79" s="145"/>
+      <c r="D79" s="151"/>
       <c r="E79" s="75">
         <v>1200</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="139" t="s">
+      <c r="A80" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="140"/>
-      <c r="C80" s="121"/>
-      <c r="D80" s="122"/>
+      <c r="B80" s="110"/>
+      <c r="C80" s="139"/>
+      <c r="D80" s="140"/>
       <c r="E80" s="44">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C81" s="141" t="s">
+      <c r="C81" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="D81" s="113"/>
+      <c r="D81" s="91"/>
       <c r="E81" s="37">
         <f>(C6+E13)-SUM(E79:E80)</f>
         <v>402.59999999999945</v>
@@ -18334,69 +18334,69 @@
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="95" t="s">
+      <c r="A83" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="B83" s="113"/>
-      <c r="C83" s="113"/>
-      <c r="D83" s="113"/>
-      <c r="E83" s="84"/>
+      <c r="B83" s="91"/>
+      <c r="C83" s="91"/>
+      <c r="D83" s="91"/>
+      <c r="E83" s="92"/>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="95" t="s">
+      <c r="A84" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="84"/>
-      <c r="C84" s="95" t="s">
+      <c r="B84" s="92"/>
+      <c r="C84" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="84"/>
+      <c r="D84" s="92"/>
       <c r="E84" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="85" t="s">
+      <c r="A85" s="142" t="s">
         <v>145</v>
       </c>
-      <c r="B85" s="86"/>
-      <c r="C85" s="117"/>
-      <c r="D85" s="152"/>
+      <c r="B85" s="117"/>
+      <c r="C85" s="135"/>
+      <c r="D85" s="149"/>
       <c r="E85" s="37">
         <f>E81</f>
         <v>402.59999999999945</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="85" t="s">
+      <c r="A86" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="B86" s="96"/>
-      <c r="C86" s="101" t="s">
+      <c r="B86" s="146"/>
+      <c r="C86" s="124" t="s">
         <v>164</v>
       </c>
-      <c r="D86" s="151"/>
+      <c r="D86" s="148"/>
       <c r="E86" s="52">
         <v>1100</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="85" t="s">
+      <c r="A87" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="86"/>
-      <c r="C87" s="93"/>
-      <c r="D87" s="84"/>
+      <c r="B87" s="117"/>
+      <c r="C87" s="134"/>
+      <c r="D87" s="92"/>
       <c r="E87" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C88" s="83" t="s">
+      <c r="C88" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="84"/>
+      <c r="D88" s="92"/>
       <c r="E88" s="37">
         <f>(E18+E85)-SUM(E86:E87)</f>
         <v>408.59999999999945</v>
@@ -18417,69 +18417,69 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="87" t="s">
+      <c r="A91" s="143" t="s">
         <v>128</v>
       </c>
-      <c r="B91" s="88"/>
-      <c r="C91" s="88"/>
-      <c r="D91" s="88"/>
-      <c r="E91" s="89"/>
+      <c r="B91" s="119"/>
+      <c r="C91" s="119"/>
+      <c r="D91" s="119"/>
+      <c r="E91" s="108"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="95" t="s">
+      <c r="A92" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B92" s="84"/>
-      <c r="C92" s="95" t="s">
+      <c r="B92" s="92"/>
+      <c r="C92" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D92" s="84"/>
+      <c r="D92" s="92"/>
       <c r="E92" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="85" t="s">
+      <c r="A93" s="142" t="s">
         <v>146</v>
       </c>
-      <c r="B93" s="86"/>
-      <c r="C93" s="93"/>
-      <c r="D93" s="84"/>
+      <c r="B93" s="117"/>
+      <c r="C93" s="134"/>
+      <c r="D93" s="92"/>
       <c r="E93" s="37">
         <f>E88</f>
         <v>408.59999999999945</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="85" t="s">
+      <c r="A94" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="96"/>
-      <c r="C94" s="101" t="s">
+      <c r="B94" s="146"/>
+      <c r="C94" s="124" t="s">
         <v>164</v>
       </c>
-      <c r="D94" s="102"/>
+      <c r="D94" s="138"/>
       <c r="E94" s="52">
         <v>1100</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="85" t="s">
+      <c r="A95" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B95" s="86"/>
-      <c r="C95" s="93"/>
-      <c r="D95" s="84"/>
+      <c r="B95" s="117"/>
+      <c r="C95" s="134"/>
+      <c r="D95" s="92"/>
       <c r="E95" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C96" s="83" t="s">
+      <c r="C96" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="D96" s="84"/>
+      <c r="D96" s="92"/>
       <c r="E96" s="52">
         <f>(E23+E93)-SUM(E94:E95)</f>
         <v>414.59999999999945</v>
@@ -22139,18 +22139,29 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="A91:E91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="C84:D84"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="A35:C36"/>
@@ -22164,29 +22175,18 @@
     <mergeCell ref="A77:E77"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="A83:E83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="A91:E91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A28:C28"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="35" priority="2" operator="lessThan">
@@ -22246,8 +22246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A0D0F5D-D1BD-4315-A79D-5F8D7D39DF80}">
   <dimension ref="A1:Y1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -22264,13 +22264,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="113" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="125"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -22473,13 +22473,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="126" t="s">
+      <c r="A10" s="118" t="s">
         <v>132</v>
       </c>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="89"/>
+      <c r="B10" s="119"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="108"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -22507,10 +22507,10 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="104" t="s">
+      <c r="C11" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="84"/>
+      <c r="D11" s="92"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
@@ -22522,10 +22522,10 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="105" t="s">
+      <c r="C12" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="86"/>
+      <c r="D12" s="117"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -22547,13 +22547,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="126" t="s">
+      <c r="A15" s="118" t="s">
         <v>140</v>
       </c>
-      <c r="B15" s="88"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="89"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="108"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -22581,10 +22581,10 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="104" t="s">
+      <c r="C16" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="84"/>
+      <c r="D16" s="92"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
@@ -22596,10 +22596,10 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="105" t="s">
+      <c r="C17" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="84"/>
+      <c r="D17" s="92"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -22624,13 +22624,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="126" t="s">
+      <c r="A20" s="118" t="s">
         <v>136</v>
       </c>
-      <c r="B20" s="88"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="89"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="108"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -22658,10 +22658,10 @@
       <c r="B21" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="127" t="s">
+      <c r="C21" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="128"/>
+      <c r="D21" s="97"/>
       <c r="E21" s="74" t="s">
         <v>4</v>
       </c>
@@ -22673,10 +22673,10 @@
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="129" t="s">
+      <c r="C22" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="130"/>
+      <c r="D22" s="123"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -22719,11 +22719,11 @@
       <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A28" s="143" t="s">
+      <c r="A28" s="156" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="113"/>
-      <c r="C28" s="84"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="92"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="20" t="s">
@@ -22738,11 +22738,11 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="114" t="s">
+      <c r="A30" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="113"/>
-      <c r="C30" s="84"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="92"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="25" t="s">
@@ -22784,16 +22784,16 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="106" t="s">
+      <c r="A35" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="107"/>
-      <c r="C35" s="108"/>
+      <c r="B35" s="127"/>
+      <c r="C35" s="128"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="109"/>
-      <c r="B36" s="110"/>
-      <c r="C36" s="111"/>
+      <c r="A36" s="129"/>
+      <c r="B36" s="107"/>
+      <c r="C36" s="130"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -22842,11 +22842,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A42" s="114" t="s">
+      <c r="A42" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="113"/>
-      <c r="C42" s="84"/>
+      <c r="B42" s="91"/>
+      <c r="C42" s="92"/>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
@@ -22881,11 +22881,11 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A46" s="114" t="s">
+      <c r="A46" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="119"/>
-      <c r="C46" s="120"/>
+      <c r="B46" s="102"/>
+      <c r="C46" s="103"/>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -22927,11 +22927,11 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="114" t="s">
+      <c r="A51" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="119"/>
-      <c r="C51" s="120"/>
+      <c r="B51" s="102"/>
+      <c r="C51" s="103"/>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="2" t="s">
@@ -22955,11 +22955,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="133" t="s">
+      <c r="A54" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="134"/>
-      <c r="C54" s="128"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="97"/>
     </row>
     <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="32" t="s">
@@ -22983,11 +22983,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="138" t="s">
+      <c r="A57" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="110"/>
-      <c r="C57" s="89"/>
+      <c r="B57" s="107"/>
+      <c r="C57" s="108"/>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
       <c r="A58" s="26" t="s">
@@ -23031,11 +23031,11 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A62" s="90" t="s">
+      <c r="A62" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="135"/>
-      <c r="C62" s="92"/>
+      <c r="B62" s="99"/>
+      <c r="C62" s="100"/>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
       <c r="A63" s="58" t="s">
@@ -23102,11 +23102,11 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A69" s="90" t="s">
+      <c r="A69" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="91"/>
-      <c r="C69" s="92"/>
+      <c r="B69" s="144"/>
+      <c r="C69" s="100"/>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
       <c r="A70" s="42" t="s">
@@ -23166,57 +23166,57 @@
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="95" t="s">
+      <c r="A77" s="90" t="s">
         <v>134</v>
       </c>
-      <c r="B77" s="113"/>
-      <c r="C77" s="113"/>
-      <c r="D77" s="113"/>
-      <c r="E77" s="84"/>
+      <c r="B77" s="91"/>
+      <c r="C77" s="91"/>
+      <c r="D77" s="91"/>
+      <c r="E77" s="92"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="131" t="s">
+      <c r="A78" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="B78" s="128"/>
-      <c r="C78" s="131" t="s">
+      <c r="B78" s="97"/>
+      <c r="C78" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="128"/>
+      <c r="D78" s="97"/>
       <c r="E78" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="146" t="s">
+      <c r="A79" s="152" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="98"/>
-      <c r="C79" s="144" t="s">
+      <c r="B79" s="85"/>
+      <c r="C79" s="150" t="s">
         <v>164</v>
       </c>
-      <c r="D79" s="145"/>
+      <c r="D79" s="151"/>
       <c r="E79" s="75">
         <v>1100</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="139" t="s">
+      <c r="A80" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="140"/>
-      <c r="C80" s="121"/>
-      <c r="D80" s="122"/>
+      <c r="B80" s="110"/>
+      <c r="C80" s="139"/>
+      <c r="D80" s="140"/>
       <c r="E80" s="44">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C81" s="141" t="s">
+      <c r="C81" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="D81" s="113"/>
+      <c r="D81" s="91"/>
       <c r="E81" s="37">
         <f>(C6+E13)-SUM(E79:E80)</f>
         <v>446.79999999999927</v>
@@ -23224,69 +23224,69 @@
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="95" t="s">
+      <c r="A83" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="B83" s="113"/>
-      <c r="C83" s="113"/>
-      <c r="D83" s="113"/>
-      <c r="E83" s="84"/>
+      <c r="B83" s="91"/>
+      <c r="C83" s="91"/>
+      <c r="D83" s="91"/>
+      <c r="E83" s="92"/>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="95" t="s">
+      <c r="A84" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="84"/>
-      <c r="C84" s="95" t="s">
+      <c r="B84" s="92"/>
+      <c r="C84" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="84"/>
+      <c r="D84" s="92"/>
       <c r="E84" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="85" t="s">
+      <c r="A85" s="142" t="s">
         <v>143</v>
       </c>
-      <c r="B85" s="86"/>
-      <c r="C85" s="117"/>
-      <c r="D85" s="152"/>
+      <c r="B85" s="117"/>
+      <c r="C85" s="135"/>
+      <c r="D85" s="149"/>
       <c r="E85" s="37">
         <f>E81</f>
         <v>446.79999999999927</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="85" t="s">
+      <c r="A86" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="B86" s="96"/>
-      <c r="C86" s="101" t="s">
+      <c r="B86" s="146"/>
+      <c r="C86" s="124" t="s">
         <v>165</v>
       </c>
-      <c r="D86" s="151"/>
+      <c r="D86" s="148"/>
       <c r="E86" s="52">
         <v>1100</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="85" t="s">
+      <c r="A87" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="86"/>
-      <c r="C87" s="93"/>
-      <c r="D87" s="84"/>
+      <c r="B87" s="117"/>
+      <c r="C87" s="134"/>
+      <c r="D87" s="92"/>
       <c r="E87" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C88" s="83" t="s">
+      <c r="C88" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="84"/>
+      <c r="D88" s="92"/>
       <c r="E88" s="37">
         <f>(E18+E85)-SUM(E86:E87)</f>
         <v>452.79999999999927</v>
@@ -23307,69 +23307,69 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="87" t="s">
+      <c r="A91" s="143" t="s">
         <v>139</v>
       </c>
-      <c r="B91" s="88"/>
-      <c r="C91" s="88"/>
-      <c r="D91" s="88"/>
-      <c r="E91" s="89"/>
+      <c r="B91" s="119"/>
+      <c r="C91" s="119"/>
+      <c r="D91" s="119"/>
+      <c r="E91" s="108"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="95" t="s">
+      <c r="A92" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B92" s="84"/>
-      <c r="C92" s="95" t="s">
+      <c r="B92" s="92"/>
+      <c r="C92" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D92" s="84"/>
+      <c r="D92" s="92"/>
       <c r="E92" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="85" t="s">
+      <c r="A93" s="142" t="s">
         <v>144</v>
       </c>
-      <c r="B93" s="86"/>
-      <c r="C93" s="93"/>
-      <c r="D93" s="84"/>
+      <c r="B93" s="117"/>
+      <c r="C93" s="134"/>
+      <c r="D93" s="92"/>
       <c r="E93" s="37">
         <f>E88</f>
         <v>452.79999999999927</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="85" t="s">
+      <c r="A94" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="96"/>
-      <c r="C94" s="101" t="s">
+      <c r="B94" s="146"/>
+      <c r="C94" s="124" t="s">
         <v>166</v>
       </c>
-      <c r="D94" s="102"/>
+      <c r="D94" s="138"/>
       <c r="E94" s="52">
         <v>739</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="85" t="s">
+      <c r="A95" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B95" s="86"/>
-      <c r="C95" s="93"/>
-      <c r="D95" s="84"/>
+      <c r="B95" s="117"/>
+      <c r="C95" s="134"/>
+      <c r="D95" s="92"/>
       <c r="E95" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C96" s="83" t="s">
+      <c r="C96" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="D96" s="84"/>
+      <c r="D96" s="92"/>
       <c r="E96" s="52">
         <f>(E23+E93)-SUM(E94:E95)</f>
         <v>819.79999999999927</v>
@@ -27029,18 +27029,29 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="A91:E91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="C84:D84"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="A35:C36"/>
@@ -27054,29 +27065,18 @@
     <mergeCell ref="A77:E77"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="A83:E83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="A91:E91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A28:C28"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="23" priority="2" operator="lessThan">
@@ -27154,13 +27154,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="113" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="125"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="115"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -27363,13 +27363,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="126" t="s">
+      <c r="A10" s="118" t="s">
         <v>148</v>
       </c>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="89"/>
+      <c r="B10" s="119"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="108"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -27397,10 +27397,10 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="104" t="s">
+      <c r="C11" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="84"/>
+      <c r="D11" s="92"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
@@ -27412,10 +27412,10 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="105" t="s">
+      <c r="C12" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="86"/>
+      <c r="D12" s="117"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -27437,13 +27437,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="126" t="s">
+      <c r="A15" s="118" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="88"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="89"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="108"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -27471,10 +27471,10 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="104" t="s">
+      <c r="C16" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="84"/>
+      <c r="D16" s="92"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
@@ -27486,10 +27486,10 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="105" t="s">
+      <c r="C17" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="84"/>
+      <c r="D17" s="92"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -27514,13 +27514,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="126" t="s">
+      <c r="A20" s="118" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="88"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="89"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="108"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -27548,10 +27548,10 @@
       <c r="B21" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="127" t="s">
+      <c r="C21" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="128"/>
+      <c r="D21" s="97"/>
       <c r="E21" s="74" t="s">
         <v>4</v>
       </c>
@@ -27563,10 +27563,10 @@
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="129" t="s">
+      <c r="C22" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="130"/>
+      <c r="D22" s="123"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -27609,11 +27609,11 @@
       <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A28" s="143" t="s">
+      <c r="A28" s="156" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="113"/>
-      <c r="C28" s="84"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="92"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="20" t="s">
@@ -27628,11 +27628,11 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="114" t="s">
+      <c r="A30" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="113"/>
-      <c r="C30" s="84"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="92"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="25" t="s">
@@ -27674,16 +27674,16 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="106" t="s">
+      <c r="A35" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="107"/>
-      <c r="C35" s="108"/>
+      <c r="B35" s="127"/>
+      <c r="C35" s="128"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="109"/>
-      <c r="B36" s="110"/>
-      <c r="C36" s="111"/>
+      <c r="A36" s="129"/>
+      <c r="B36" s="107"/>
+      <c r="C36" s="130"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -27732,11 +27732,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A42" s="114" t="s">
+      <c r="A42" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="113"/>
-      <c r="C42" s="84"/>
+      <c r="B42" s="91"/>
+      <c r="C42" s="92"/>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
@@ -27771,11 +27771,11 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A46" s="114" t="s">
+      <c r="A46" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="119"/>
-      <c r="C46" s="120"/>
+      <c r="B46" s="102"/>
+      <c r="C46" s="103"/>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -27817,11 +27817,11 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="114" t="s">
+      <c r="A51" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="119"/>
-      <c r="C51" s="120"/>
+      <c r="B51" s="102"/>
+      <c r="C51" s="103"/>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="2" t="s">
@@ -27845,11 +27845,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="133" t="s">
+      <c r="A54" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="134"/>
-      <c r="C54" s="128"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="97"/>
     </row>
     <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="32" t="s">
@@ -27873,11 +27873,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="138" t="s">
+      <c r="A57" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="110"/>
-      <c r="C57" s="89"/>
+      <c r="B57" s="107"/>
+      <c r="C57" s="108"/>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
       <c r="A58" s="26" t="s">
@@ -27921,11 +27921,11 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A62" s="90" t="s">
+      <c r="A62" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="135"/>
-      <c r="C62" s="92"/>
+      <c r="B62" s="99"/>
+      <c r="C62" s="100"/>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
       <c r="A63" s="58" t="s">
@@ -27992,11 +27992,11 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A69" s="90" t="s">
+      <c r="A69" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="91"/>
-      <c r="C69" s="92"/>
+      <c r="B69" s="144"/>
+      <c r="C69" s="100"/>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
       <c r="A70" s="42" t="s">
@@ -28055,45 +28055,45 @@
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="95" t="s">
+      <c r="A77" s="90" t="s">
         <v>150</v>
       </c>
-      <c r="B77" s="113"/>
-      <c r="C77" s="113"/>
-      <c r="D77" s="113"/>
-      <c r="E77" s="84"/>
+      <c r="B77" s="91"/>
+      <c r="C77" s="91"/>
+      <c r="D77" s="91"/>
+      <c r="E77" s="92"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="131" t="s">
+      <c r="A78" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="B78" s="128"/>
-      <c r="C78" s="131" t="s">
+      <c r="B78" s="97"/>
+      <c r="C78" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="128"/>
+      <c r="D78" s="97"/>
       <c r="E78" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="153" t="s">
+      <c r="A79" s="157" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="153"/>
-      <c r="C79" s="154"/>
-      <c r="D79" s="155"/>
+      <c r="B79" s="157"/>
+      <c r="C79" s="160"/>
+      <c r="D79" s="161"/>
       <c r="E79" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="153" t="s">
+      <c r="A80" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="153"/>
-      <c r="C80" s="156"/>
-      <c r="D80" s="156"/>
+      <c r="B80" s="157"/>
+      <c r="C80" s="158"/>
+      <c r="D80" s="158"/>
       <c r="E80" s="80">
         <f>C74</f>
         <v>1299</v>
@@ -28102,10 +28102,10 @@
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
       <c r="A81" s="78"/>
       <c r="B81" s="78"/>
-      <c r="C81" s="157" t="s">
+      <c r="C81" s="159" t="s">
         <v>41</v>
       </c>
-      <c r="D81" s="110"/>
+      <c r="D81" s="107"/>
       <c r="E81" s="79">
         <f>(C6+E13)-SUM(E79:E80)</f>
         <v>1951.9999999999991</v>
@@ -28113,67 +28113,67 @@
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="95" t="s">
+      <c r="A83" s="90" t="s">
         <v>159</v>
       </c>
-      <c r="B83" s="113"/>
-      <c r="C83" s="113"/>
-      <c r="D83" s="113"/>
-      <c r="E83" s="84"/>
+      <c r="B83" s="91"/>
+      <c r="C83" s="91"/>
+      <c r="D83" s="91"/>
+      <c r="E83" s="92"/>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="95" t="s">
+      <c r="A84" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="84"/>
-      <c r="C84" s="95" t="s">
+      <c r="B84" s="92"/>
+      <c r="C84" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="84"/>
+      <c r="D84" s="92"/>
       <c r="E84" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="85" t="s">
+      <c r="A85" s="142" t="s">
         <v>151</v>
       </c>
-      <c r="B85" s="86"/>
-      <c r="C85" s="117"/>
-      <c r="D85" s="152"/>
+      <c r="B85" s="117"/>
+      <c r="C85" s="135"/>
+      <c r="D85" s="149"/>
       <c r="E85" s="37">
         <f>E81</f>
         <v>1951.9999999999991</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="85" t="s">
+      <c r="A86" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="B86" s="96"/>
-      <c r="C86" s="101"/>
-      <c r="D86" s="151"/>
+      <c r="B86" s="146"/>
+      <c r="C86" s="124"/>
+      <c r="D86" s="148"/>
       <c r="E86" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="85" t="s">
+      <c r="A87" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="86"/>
-      <c r="C87" s="93"/>
-      <c r="D87" s="84"/>
+      <c r="B87" s="117"/>
+      <c r="C87" s="134"/>
+      <c r="D87" s="92"/>
       <c r="E87" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C88" s="83" t="s">
+      <c r="C88" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="84"/>
+      <c r="D88" s="92"/>
       <c r="E88" s="37">
         <f>(E18+E85)-SUM(E86:E87)</f>
         <v>3057.9999999999991</v>
@@ -28194,67 +28194,67 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="87" t="s">
+      <c r="A91" s="143" t="s">
         <v>156</v>
       </c>
-      <c r="B91" s="88"/>
-      <c r="C91" s="88"/>
-      <c r="D91" s="88"/>
-      <c r="E91" s="89"/>
+      <c r="B91" s="119"/>
+      <c r="C91" s="119"/>
+      <c r="D91" s="119"/>
+      <c r="E91" s="108"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="95" t="s">
+      <c r="A92" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B92" s="84"/>
-      <c r="C92" s="95" t="s">
+      <c r="B92" s="92"/>
+      <c r="C92" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D92" s="84"/>
+      <c r="D92" s="92"/>
       <c r="E92" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="85" t="s">
+      <c r="A93" s="142" t="s">
         <v>160</v>
       </c>
-      <c r="B93" s="86"/>
-      <c r="C93" s="93"/>
-      <c r="D93" s="84"/>
+      <c r="B93" s="117"/>
+      <c r="C93" s="134"/>
+      <c r="D93" s="92"/>
       <c r="E93" s="37">
         <f>E88</f>
         <v>3057.9999999999991</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="85" t="s">
+      <c r="A94" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="96"/>
-      <c r="C94" s="101"/>
-      <c r="D94" s="102"/>
+      <c r="B94" s="146"/>
+      <c r="C94" s="124"/>
+      <c r="D94" s="138"/>
       <c r="E94" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="85" t="s">
+      <c r="A95" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B95" s="86"/>
-      <c r="C95" s="93"/>
-      <c r="D95" s="84"/>
+      <c r="B95" s="117"/>
+      <c r="C95" s="134"/>
+      <c r="D95" s="92"/>
       <c r="E95" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C96" s="83" t="s">
+      <c r="C96" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="D96" s="84"/>
+      <c r="D96" s="92"/>
       <c r="E96" s="52">
         <f>(E23+E93)-SUM(E94:E95)</f>
         <v>4163.9999999999991</v>
@@ -31914,29 +31914,18 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="A91:E91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="A83:E83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A28:C28"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="A35:C36"/>
@@ -31950,18 +31939,29 @@
     <mergeCell ref="A77:E77"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="A91:E91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
docs: Updated payback amount for Ng Wing Lam
</commit_message>
<xml_diff>
--- a/Alan Tang_s Income Expense Now.xlsx
+++ b/Alan Tang_s Income Expense Now.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Income-Expenditure-Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B727C8-FF4E-4F50-A43C-2083928310A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71361480-B48A-4C40-A4AB-07D4A57FDD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="171">
   <si>
     <t>Assets</t>
   </si>
@@ -459,9 +459,6 @@
     <t>30 Packets</t>
   </si>
   <si>
-    <t>2. Payback $850 to Ng Wing Lam</t>
-  </si>
-  <si>
     <t>HGC BroadBand End Of Service</t>
   </si>
   <si>
@@ -621,14 +618,14 @@
     <t>Net Debts:</t>
   </si>
   <si>
-    <t>2. Payback $1500 to Ng Wing Lam</t>
-  </si>
-  <si>
     <t>3. Additional Payment $10 for cigarette</t>
   </si>
   <si>
+    <t>3. Terminate the Fixed Line Phone 23290612 pay $187 remaining fees</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">2. Payback $800 to Ng Wing Lam - </t>
+      <t xml:space="preserve">2. Payback $1000 to Ng Wing Lam - </t>
     </r>
     <r>
       <rPr>
@@ -640,9 +637,6 @@
       </rPr>
       <t>Last Payment</t>
     </r>
-  </si>
-  <si>
-    <t>3. Terminate the Fixed Line Phone 23290612 pay $187 remaining fees</t>
   </si>
 </sst>
 </file>
@@ -1546,6 +1540,159 @@
     <xf numFmtId="0" fontId="25" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1570,68 +1717,14 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1639,115 +1732,13 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="22" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="22" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1768,23 +1759,26 @@
     <xf numFmtId="166" fontId="22" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2535,7 +2529,7 @@
   <dimension ref="A1:Y1013"/>
   <sheetViews>
     <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2552,13 +2546,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="120"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -2763,11 +2757,11 @@
     <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C9" s="57">
         <f>(-C75+SUM(E88,E97))</f>
-        <v>-12439</v>
+        <v>-12939</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -2821,13 +2815,13 @@
     </row>
     <row r="11" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="12" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A12" s="118" t="s">
+      <c r="A12" s="121" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="119"/>
-      <c r="C12" s="119"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="108"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="95"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
@@ -2855,10 +2849,10 @@
       <c r="B13" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="120" t="s">
+      <c r="C13" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="92"/>
+      <c r="D13" s="84"/>
       <c r="E13" s="17" t="s">
         <v>4</v>
       </c>
@@ -2870,10 +2864,10 @@
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="116" t="s">
+      <c r="C14" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="117"/>
+      <c r="D14" s="92"/>
       <c r="E14" s="18">
         <v>2405</v>
       </c>
@@ -2895,13 +2889,13 @@
       <c r="B16" s="11"/>
     </row>
     <row r="17" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A17" s="118" t="s">
+      <c r="A17" s="121" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="119"/>
-      <c r="C17" s="119"/>
-      <c r="D17" s="119"/>
-      <c r="E17" s="108"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="95"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
@@ -2929,10 +2923,10 @@
       <c r="B18" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="121" t="s">
+      <c r="C18" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="97"/>
+      <c r="D18" s="123"/>
       <c r="E18" s="74" t="s">
         <v>4</v>
       </c>
@@ -2944,10 +2938,10 @@
       <c r="B19" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="123"/>
+      <c r="D19" s="125"/>
       <c r="E19" s="67">
         <v>2405</v>
       </c>
@@ -2972,13 +2966,13 @@
       <c r="E21" s="51"/>
     </row>
     <row r="22" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A22" s="118" t="s">
+      <c r="A22" s="121" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="119"/>
-      <c r="C22" s="119"/>
-      <c r="D22" s="119"/>
-      <c r="E22" s="108"/>
+      <c r="B22" s="94"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="94"/>
+      <c r="E22" s="95"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
@@ -3006,10 +3000,10 @@
       <c r="B23" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="120" t="s">
+      <c r="C23" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="92"/>
+      <c r="D23" s="84"/>
       <c r="E23" s="17" t="s">
         <v>4</v>
       </c>
@@ -3021,40 +3015,40 @@
       <c r="B24" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="116" t="s">
+      <c r="C24" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="92"/>
+      <c r="D24" s="84"/>
       <c r="E24" s="27">
         <v>2405</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="13.15" customHeight="1">
       <c r="A25" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" s="89" t="s">
         <v>162</v>
       </c>
-      <c r="B25" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="C25" s="141" t="s">
-        <v>163</v>
-      </c>
-      <c r="D25" s="141"/>
+      <c r="D25" s="89"/>
       <c r="E25" s="67">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="13.15" customHeight="1">
       <c r="A26" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B26" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="132" t="s">
+      <c r="C26" s="116" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="133"/>
+      <c r="D26" s="117"/>
       <c r="E26" s="67">
         <v>1035</v>
       </c>
@@ -3090,11 +3084,11 @@
       <c r="B30" s="11"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A31" s="131" t="s">
+      <c r="A31" s="115" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="91"/>
-      <c r="C31" s="92"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="84"/>
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="A32" s="20" t="s">
@@ -3109,11 +3103,11 @@
       <c r="D32" s="22"/>
     </row>
     <row r="33" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A33" s="101" t="s">
+      <c r="A33" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="91"/>
-      <c r="C33" s="92"/>
+      <c r="B33" s="83"/>
+      <c r="C33" s="84"/>
     </row>
     <row r="34" spans="1:3" ht="13.5" customHeight="1">
       <c r="A34" s="25" t="s">
@@ -3126,7 +3120,7 @@
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
       <c r="A35" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="27">
@@ -3155,16 +3149,16 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A38" s="126" t="s">
+      <c r="A38" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="127"/>
-      <c r="C38" s="128"/>
+      <c r="B38" s="110"/>
+      <c r="C38" s="111"/>
     </row>
     <row r="39" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A39" s="129"/>
-      <c r="B39" s="107"/>
-      <c r="C39" s="130"/>
+      <c r="A39" s="112"/>
+      <c r="B39" s="113"/>
+      <c r="C39" s="114"/>
     </row>
     <row r="40" spans="1:3" ht="13.5" customHeight="1">
       <c r="A40" s="2" t="s">
@@ -3213,11 +3207,11 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A45" s="101" t="s">
+      <c r="A45" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="91"/>
-      <c r="C45" s="92"/>
+      <c r="B45" s="83"/>
+      <c r="C45" s="84"/>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
       <c r="A46" s="2" t="s">
@@ -3252,11 +3246,11 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A49" s="101" t="s">
+      <c r="A49" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="102"/>
-      <c r="C49" s="103"/>
+      <c r="B49" s="85"/>
+      <c r="C49" s="86"/>
     </row>
     <row r="50" spans="1:3" ht="13.5" customHeight="1">
       <c r="A50" s="2" t="s">
@@ -3298,11 +3292,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="101" t="s">
+      <c r="A54" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="B54" s="102"/>
-      <c r="C54" s="103"/>
+      <c r="B54" s="85"/>
+      <c r="C54" s="86"/>
     </row>
     <row r="55" spans="1:3" ht="13.5" customHeight="1">
       <c r="A55" s="2" t="s">
@@ -3326,11 +3320,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="95" t="s">
+      <c r="A57" s="141" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="96"/>
-      <c r="C57" s="97"/>
+      <c r="B57" s="142"/>
+      <c r="C57" s="123"/>
     </row>
     <row r="58" spans="1:3" ht="33" customHeight="1">
       <c r="A58" s="32" t="s">
@@ -3354,11 +3348,11 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A60" s="106" t="s">
+      <c r="A60" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="B60" s="107"/>
-      <c r="C60" s="108"/>
+      <c r="B60" s="113"/>
+      <c r="C60" s="95"/>
     </row>
     <row r="61" spans="1:3" ht="13.5" customHeight="1">
       <c r="A61" s="26" t="s">
@@ -3402,11 +3396,11 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A65" s="98" t="s">
+      <c r="A65" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="99"/>
-      <c r="C65" s="100"/>
+      <c r="B65" s="143"/>
+      <c r="C65" s="98"/>
     </row>
     <row r="66" spans="1:8" ht="13.5" customHeight="1">
       <c r="A66" s="58" t="s">
@@ -3462,11 +3456,11 @@
       </c>
     </row>
     <row r="71" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A71" s="98" t="s">
+      <c r="A71" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="B71" s="144"/>
-      <c r="C71" s="100"/>
+      <c r="B71" s="97"/>
+      <c r="C71" s="98"/>
     </row>
     <row r="72" spans="1:8" ht="13.5" customHeight="1">
       <c r="A72" s="42" t="s">
@@ -3525,126 +3519,126 @@
       <c r="B78" s="11"/>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="90" t="s">
+      <c r="A79" s="104" t="s">
         <v>62</v>
       </c>
-      <c r="B79" s="104"/>
-      <c r="C79" s="104"/>
-      <c r="D79" s="104"/>
-      <c r="E79" s="105"/>
+      <c r="B79" s="128"/>
+      <c r="C79" s="128"/>
+      <c r="D79" s="128"/>
+      <c r="E79" s="129"/>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="93" t="s">
+      <c r="A80" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="B80" s="94"/>
-      <c r="C80" s="93" t="s">
+      <c r="B80" s="127"/>
+      <c r="C80" s="126" t="s">
         <v>37</v>
       </c>
-      <c r="D80" s="94"/>
+      <c r="D80" s="127"/>
       <c r="E80" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A81" s="109" t="s">
+      <c r="A81" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="B81" s="110"/>
-      <c r="C81" s="139"/>
-      <c r="D81" s="140"/>
+      <c r="B81" s="132"/>
+      <c r="C81" s="87"/>
+      <c r="D81" s="88"/>
       <c r="E81" s="44">
         <f>C76</f>
         <v>1503</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C82" s="111" t="s">
+      <c r="C82" s="144" t="s">
         <v>41</v>
       </c>
-      <c r="D82" s="112"/>
+      <c r="D82" s="145"/>
       <c r="E82" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="90" t="s">
+      <c r="A84" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="B84" s="91"/>
-      <c r="C84" s="91"/>
-      <c r="D84" s="91"/>
-      <c r="E84" s="92"/>
+      <c r="B84" s="83"/>
+      <c r="C84" s="83"/>
+      <c r="D84" s="83"/>
+      <c r="E84" s="84"/>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="90" t="s">
+      <c r="A85" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B85" s="92"/>
-      <c r="C85" s="90" t="s">
+      <c r="B85" s="84"/>
+      <c r="C85" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="D85" s="92"/>
+      <c r="D85" s="84"/>
       <c r="E85" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="142" t="s">
+      <c r="A86" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="B86" s="146"/>
-      <c r="C86" s="134"/>
-      <c r="D86" s="145"/>
+      <c r="B86" s="101"/>
+      <c r="C86" s="99"/>
+      <c r="D86" s="100"/>
       <c r="E86" s="37">
         <f>E82</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="84" t="s">
+      <c r="A87" s="135" t="s">
         <v>82</v>
       </c>
-      <c r="B87" s="85"/>
-      <c r="C87" s="124" t="s">
+      <c r="B87" s="136"/>
+      <c r="C87" s="105" t="s">
         <v>83</v>
       </c>
-      <c r="D87" s="138"/>
+      <c r="D87" s="106"/>
       <c r="E87" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A88" s="88"/>
-      <c r="B88" s="89"/>
-      <c r="C88" s="124" t="s">
+      <c r="A88" s="139"/>
+      <c r="B88" s="140"/>
+      <c r="C88" s="105" t="s">
         <v>91</v>
       </c>
-      <c r="D88" s="125"/>
+      <c r="D88" s="146"/>
       <c r="E88" s="52">
         <v>1000</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A89" s="142" t="s">
+      <c r="A89" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B89" s="117"/>
-      <c r="C89" s="135" t="s">
+      <c r="B89" s="92"/>
+      <c r="C89" s="102" t="s">
         <v>92</v>
       </c>
-      <c r="D89" s="136"/>
+      <c r="D89" s="103"/>
       <c r="E89" s="66">
         <f>C76</f>
         <v>1503</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C90" s="137" t="s">
+      <c r="C90" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="D90" s="92"/>
+      <c r="D90" s="84"/>
       <c r="E90" s="37">
         <f>SUM(C3:C7)</f>
         <v>57.370000000000005</v>
@@ -3665,93 +3659,93 @@
       <c r="E92" s="24"/>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="143" t="s">
+      <c r="A93" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="B93" s="119"/>
-      <c r="C93" s="119"/>
-      <c r="D93" s="119"/>
-      <c r="E93" s="108"/>
+      <c r="B93" s="94"/>
+      <c r="C93" s="94"/>
+      <c r="D93" s="94"/>
+      <c r="E93" s="95"/>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="90" t="s">
+      <c r="A94" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B94" s="92"/>
-      <c r="C94" s="90" t="s">
+      <c r="B94" s="84"/>
+      <c r="C94" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="D94" s="92"/>
+      <c r="D94" s="84"/>
       <c r="E94" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="142" t="s">
+      <c r="A95" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="B95" s="117"/>
-      <c r="C95" s="134"/>
-      <c r="D95" s="92"/>
+      <c r="B95" s="92"/>
+      <c r="C95" s="99"/>
+      <c r="D95" s="84"/>
       <c r="E95" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A96" s="84" t="s">
+      <c r="A96" s="135" t="s">
         <v>82</v>
       </c>
-      <c r="B96" s="85"/>
-      <c r="C96" s="124" t="s">
+      <c r="B96" s="136"/>
+      <c r="C96" s="105" t="s">
         <v>83</v>
       </c>
-      <c r="D96" s="138"/>
+      <c r="D96" s="106"/>
       <c r="E96" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A97" s="86"/>
-      <c r="B97" s="87"/>
-      <c r="C97" s="124" t="s">
-        <v>169</v>
-      </c>
-      <c r="D97" s="125"/>
+      <c r="A97" s="137"/>
+      <c r="B97" s="138"/>
+      <c r="C97" s="105" t="s">
+        <v>91</v>
+      </c>
+      <c r="D97" s="146"/>
       <c r="E97" s="52">
-        <v>1500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A98" s="88"/>
-      <c r="B98" s="89"/>
-      <c r="C98" s="82" t="s">
-        <v>170</v>
-      </c>
-      <c r="D98" s="83"/>
+      <c r="A98" s="139"/>
+      <c r="B98" s="140"/>
+      <c r="C98" s="133" t="s">
+        <v>168</v>
+      </c>
+      <c r="D98" s="134"/>
       <c r="E98" s="52">
         <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A99" s="142" t="s">
+      <c r="A99" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B99" s="146"/>
-      <c r="C99" s="135"/>
-      <c r="D99" s="136"/>
+      <c r="B99" s="101"/>
+      <c r="C99" s="102"/>
+      <c r="D99" s="103"/>
       <c r="E99" s="52">
         <f>C76</f>
         <v>1503</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C100" s="137" t="s">
+      <c r="C100" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="D100" s="92"/>
+      <c r="D100" s="84"/>
       <c r="E100" s="52">
         <f>(E27+E95)-SUM(E96:E99)</f>
-        <v>477</v>
+        <v>977</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="13.5" customHeight="1">
@@ -7408,6 +7402,41 @@
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="A96:B98"/>
+    <mergeCell ref="A84:E84"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="A87:B88"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A79:E79"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="C26:D26"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="A54:C54"/>
     <mergeCell ref="C81:D81"/>
@@ -7424,41 +7453,6 @@
     <mergeCell ref="A86:B86"/>
     <mergeCell ref="C96:D96"/>
     <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A79:E79"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="A96:B98"/>
-    <mergeCell ref="A84:E84"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="A87:B88"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="A94:B94"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="C9">
@@ -7515,8 +7509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5F3FA5-5013-4B35-A74B-6269617B858B}">
   <dimension ref="A1:Y1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -7533,13 +7527,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="118" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="120"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -7561,7 +7555,7 @@
       </c>
       <c r="C3" s="5">
         <f>'April 2024 - June 2024'!E100</f>
-        <v>477</v>
+        <v>977</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7656,7 +7650,7 @@
       </c>
       <c r="C6" s="5">
         <f>SUM(C3:C5)</f>
-        <v>503.2</v>
+        <v>1003.2</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -7684,7 +7678,7 @@
     <row r="7" spans="1:25" ht="13.5" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="57">
         <f>('April 2024 - June 2024'!C9)+SUM(E81,E89,E99)</f>
@@ -7742,13 +7736,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="118" t="s">
+      <c r="A10" s="121" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="119"/>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="108"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="95"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -7776,10 +7770,10 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="120" t="s">
+      <c r="C11" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="92"/>
+      <c r="D11" s="84"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
@@ -7791,10 +7785,10 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="116" t="s">
+      <c r="C12" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="117"/>
+      <c r="D12" s="92"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -7816,13 +7810,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="121" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="119"/>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="108"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="95"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -7850,10 +7844,10 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="120" t="s">
+      <c r="C16" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="92"/>
+      <c r="D16" s="84"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
@@ -7865,10 +7859,10 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="92"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -7893,13 +7887,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="118" t="s">
+      <c r="A20" s="121" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="119"/>
-      <c r="C20" s="119"/>
-      <c r="D20" s="119"/>
-      <c r="E20" s="108"/>
+      <c r="B20" s="94"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="95"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -7927,10 +7921,10 @@
       <c r="B21" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="121" t="s">
+      <c r="C21" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="97"/>
+      <c r="D21" s="123"/>
       <c r="E21" s="74" t="s">
         <v>4</v>
       </c>
@@ -7942,10 +7936,10 @@
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="122" t="s">
+      <c r="C22" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="123"/>
+      <c r="D22" s="125"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -7953,10 +7947,10 @@
     <row r="23" spans="1:25" ht="13.15" customHeight="1">
       <c r="A23" s="33"/>
       <c r="B23" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="C23" s="122"/>
-      <c r="D23" s="122"/>
+        <v>119</v>
+      </c>
+      <c r="C23" s="124"/>
+      <c r="D23" s="124"/>
       <c r="E23" s="67">
         <v>204</v>
       </c>
@@ -7999,11 +7993,11 @@
       <c r="B28" s="11"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A29" s="156" t="s">
+      <c r="A29" s="147" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="91"/>
-      <c r="C29" s="92"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="84"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
       <c r="A30" s="20" t="s">
@@ -8018,11 +8012,11 @@
       <c r="D30" s="22"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A31" s="101" t="s">
+      <c r="A31" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="91"/>
-      <c r="C31" s="92"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="84"/>
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="A32" s="25" t="s">
@@ -8035,7 +8029,7 @@
     </row>
     <row r="33" spans="1:3" ht="13.5" customHeight="1">
       <c r="A33" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B33" s="26"/>
       <c r="C33" s="27">
@@ -8064,16 +8058,16 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="126" t="s">
+      <c r="A36" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="127"/>
-      <c r="C36" s="128"/>
+      <c r="B36" s="110"/>
+      <c r="C36" s="111"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A37" s="129"/>
-      <c r="B37" s="107"/>
-      <c r="C37" s="130"/>
+      <c r="A37" s="112"/>
+      <c r="B37" s="113"/>
+      <c r="C37" s="114"/>
     </row>
     <row r="38" spans="1:3" ht="13.5" customHeight="1">
       <c r="A38" s="2" t="s">
@@ -8122,11 +8116,11 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A43" s="101" t="s">
+      <c r="A43" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="91"/>
-      <c r="C43" s="92"/>
+      <c r="B43" s="83"/>
+      <c r="C43" s="84"/>
     </row>
     <row r="44" spans="1:3" ht="13.5" customHeight="1">
       <c r="A44" s="2" t="s">
@@ -8161,11 +8155,11 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A47" s="101" t="s">
+      <c r="A47" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="102"/>
-      <c r="C47" s="103"/>
+      <c r="B47" s="85"/>
+      <c r="C47" s="86"/>
     </row>
     <row r="48" spans="1:3" ht="13.5" customHeight="1">
       <c r="A48" s="2" t="s">
@@ -8207,11 +8201,11 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A52" s="101" t="s">
+      <c r="A52" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="B52" s="102"/>
-      <c r="C52" s="103"/>
+      <c r="B52" s="85"/>
+      <c r="C52" s="86"/>
     </row>
     <row r="53" spans="1:3" ht="13.5" customHeight="1">
       <c r="A53" s="2" t="s">
@@ -8235,11 +8229,11 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A55" s="95" t="s">
+      <c r="A55" s="141" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="96"/>
-      <c r="C55" s="97"/>
+      <c r="B55" s="142"/>
+      <c r="C55" s="123"/>
     </row>
     <row r="56" spans="1:3" ht="33" customHeight="1">
       <c r="A56" s="32" t="s">
@@ -8263,11 +8257,11 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A58" s="106" t="s">
+      <c r="A58" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="107"/>
-      <c r="C58" s="108"/>
+      <c r="B58" s="113"/>
+      <c r="C58" s="95"/>
     </row>
     <row r="59" spans="1:3" ht="13.5" customHeight="1">
       <c r="A59" s="26" t="s">
@@ -8311,11 +8305,11 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A63" s="98" t="s">
+      <c r="A63" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="B63" s="99"/>
-      <c r="C63" s="100"/>
+      <c r="B63" s="143"/>
+      <c r="C63" s="98"/>
     </row>
     <row r="64" spans="1:3" ht="13.5" customHeight="1">
       <c r="A64" s="58" t="s">
@@ -8382,11 +8376,11 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A70" s="98" t="s">
+      <c r="A70" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="B70" s="144"/>
-      <c r="C70" s="100"/>
+      <c r="B70" s="97"/>
+      <c r="C70" s="98"/>
     </row>
     <row r="71" spans="1:8" ht="13.5" customHeight="1">
       <c r="A71" s="42" t="s">
@@ -8446,163 +8440,163 @@
       <c r="B77" s="11"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="90" t="s">
+      <c r="A78" s="104" t="s">
         <v>100</v>
       </c>
-      <c r="B78" s="91"/>
-      <c r="C78" s="91"/>
-      <c r="D78" s="91"/>
-      <c r="E78" s="92"/>
+      <c r="B78" s="83"/>
+      <c r="C78" s="83"/>
+      <c r="D78" s="83"/>
+      <c r="E78" s="84"/>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="93" t="s">
+      <c r="A79" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="B79" s="97"/>
-      <c r="C79" s="93" t="s">
+      <c r="B79" s="123"/>
+      <c r="C79" s="126" t="s">
         <v>37</v>
       </c>
-      <c r="D79" s="97"/>
+      <c r="D79" s="123"/>
       <c r="E79" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="152" t="s">
+      <c r="A80" s="151" t="s">
         <v>82</v>
       </c>
-      <c r="B80" s="152"/>
-      <c r="C80" s="150" t="s">
+      <c r="B80" s="151"/>
+      <c r="C80" s="149" t="s">
         <v>83</v>
       </c>
-      <c r="D80" s="151"/>
+      <c r="D80" s="150"/>
       <c r="E80" s="75">
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A81" s="153"/>
-      <c r="B81" s="153"/>
-      <c r="C81" s="154" t="s">
-        <v>119</v>
-      </c>
-      <c r="D81" s="155"/>
+      <c r="A81" s="152"/>
+      <c r="B81" s="152"/>
+      <c r="C81" s="153" t="s">
+        <v>91</v>
+      </c>
+      <c r="D81" s="154"/>
       <c r="E81" s="52">
-        <v>850</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A82" s="109" t="s">
+      <c r="A82" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="B82" s="110"/>
-      <c r="C82" s="139"/>
-      <c r="D82" s="140"/>
+      <c r="B82" s="132"/>
+      <c r="C82" s="87"/>
+      <c r="D82" s="88"/>
       <c r="E82" s="44">
         <f>C75</f>
         <v>1503</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C83" s="111" t="s">
+      <c r="C83" s="144" t="s">
         <v>41</v>
       </c>
-      <c r="D83" s="91"/>
+      <c r="D83" s="83"/>
       <c r="E83" s="37">
         <f>(C6+E13)-SUM(E80:E82)</f>
-        <v>555.19999999999982</v>
+        <v>905.19999999999982</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="90" t="s">
+      <c r="A85" s="104" t="s">
         <v>101</v>
       </c>
-      <c r="B85" s="91"/>
-      <c r="C85" s="91"/>
-      <c r="D85" s="91"/>
-      <c r="E85" s="92"/>
+      <c r="B85" s="83"/>
+      <c r="C85" s="83"/>
+      <c r="D85" s="83"/>
+      <c r="E85" s="84"/>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="90" t="s">
+      <c r="A86" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B86" s="92"/>
-      <c r="C86" s="90" t="s">
+      <c r="B86" s="84"/>
+      <c r="C86" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="D86" s="92"/>
+      <c r="D86" s="84"/>
       <c r="E86" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="142" t="s">
+      <c r="A87" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="B87" s="117"/>
-      <c r="C87" s="135"/>
-      <c r="D87" s="149"/>
+      <c r="B87" s="92"/>
+      <c r="C87" s="102"/>
+      <c r="D87" s="156"/>
       <c r="E87" s="37">
         <f>E83</f>
-        <v>555.19999999999982</v>
+        <v>905.19999999999982</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A88" s="84" t="s">
+      <c r="A88" s="135" t="s">
         <v>82</v>
       </c>
-      <c r="B88" s="85"/>
-      <c r="C88" s="135" t="s">
+      <c r="B88" s="136"/>
+      <c r="C88" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="D88" s="148"/>
+      <c r="D88" s="155"/>
       <c r="E88" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A89" s="86"/>
-      <c r="B89" s="87"/>
-      <c r="C89" s="124" t="s">
-        <v>119</v>
-      </c>
-      <c r="D89" s="147"/>
+      <c r="A89" s="137"/>
+      <c r="B89" s="138"/>
+      <c r="C89" s="105" t="s">
+        <v>91</v>
+      </c>
+      <c r="D89" s="148"/>
       <c r="E89" s="52">
-        <v>850</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A90" s="88"/>
-      <c r="B90" s="89"/>
-      <c r="C90" s="124" t="s">
-        <v>172</v>
-      </c>
-      <c r="D90" s="147"/>
+      <c r="A90" s="139"/>
+      <c r="B90" s="140"/>
+      <c r="C90" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="D90" s="148"/>
       <c r="E90" s="52">
         <v>187</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="142" t="s">
+      <c r="A91" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B91" s="117"/>
-      <c r="C91" s="134"/>
-      <c r="D91" s="92"/>
+      <c r="B91" s="92"/>
+      <c r="C91" s="99"/>
+      <c r="D91" s="84"/>
       <c r="E91" s="66">
         <f>C75</f>
         <v>1503</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C92" s="137" t="s">
+      <c r="C92" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="D92" s="92"/>
+      <c r="D92" s="84"/>
       <c r="E92" s="37">
         <f>(E18+E87)-SUM(E88:E91)</f>
-        <v>420.19999999999982</v>
+        <v>620.19999999999982</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
@@ -8620,48 +8614,48 @@
       <c r="E94" s="24"/>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="143" t="s">
+      <c r="A95" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="B95" s="119"/>
-      <c r="C95" s="119"/>
-      <c r="D95" s="119"/>
-      <c r="E95" s="108"/>
+      <c r="B95" s="94"/>
+      <c r="C95" s="94"/>
+      <c r="D95" s="94"/>
+      <c r="E95" s="95"/>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A96" s="90" t="s">
+      <c r="A96" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B96" s="92"/>
-      <c r="C96" s="90" t="s">
+      <c r="B96" s="84"/>
+      <c r="C96" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="D96" s="92"/>
+      <c r="D96" s="84"/>
       <c r="E96" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A97" s="142" t="s">
+      <c r="A97" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="B97" s="117"/>
-      <c r="C97" s="134"/>
-      <c r="D97" s="92"/>
+      <c r="B97" s="92"/>
+      <c r="C97" s="99"/>
+      <c r="D97" s="84"/>
       <c r="E97" s="37">
         <f>E92</f>
-        <v>420.19999999999982</v>
+        <v>620.19999999999982</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A98" s="142" t="s">
+      <c r="A98" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="B98" s="146"/>
-      <c r="C98" s="124" t="s">
+      <c r="B98" s="101"/>
+      <c r="C98" s="105" t="s">
         <v>83</v>
       </c>
-      <c r="D98" s="138"/>
+      <c r="D98" s="106"/>
       <c r="E98" s="52">
         <v>0</v>
       </c>
@@ -8669,31 +8663,31 @@
     <row r="99" spans="1:5" ht="13.5" customHeight="1">
       <c r="A99" s="76"/>
       <c r="B99" s="77"/>
-      <c r="C99" s="124" t="s">
-        <v>171</v>
-      </c>
-      <c r="D99" s="147"/>
+      <c r="C99" s="105" t="s">
+        <v>170</v>
+      </c>
+      <c r="D99" s="148"/>
       <c r="E99" s="52">
-        <v>800</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A100" s="142" t="s">
+      <c r="A100" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B100" s="117"/>
-      <c r="C100" s="134"/>
-      <c r="D100" s="92"/>
+      <c r="B100" s="92"/>
+      <c r="C100" s="99"/>
+      <c r="D100" s="84"/>
       <c r="E100" s="66">
         <f>C75</f>
         <v>1503</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C101" s="137" t="s">
+      <c r="C101" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="D101" s="92"/>
+      <c r="D101" s="84"/>
       <c r="E101" s="52">
         <f>(E24+E97)-SUM(E98:E100)</f>
         <v>726.19999999999982</v>
@@ -12353,6 +12347,43 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="A88:B90"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="A85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="A36:C37"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="A95:E95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="A80:B81"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A63:C63"/>
     <mergeCell ref="A82:B82"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A1:E1"/>
@@ -12369,43 +12400,6 @@
     <mergeCell ref="A70:C70"/>
     <mergeCell ref="A78:E78"/>
     <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="A95:E95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="A80:B81"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="A88:B90"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="A85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="A36:C37"/>
-    <mergeCell ref="A43:C43"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="59" priority="2" operator="lessThan">
@@ -12466,7 +12460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1EAFDB-34A9-4E8B-8792-A6B6BA3CC3A2}">
   <dimension ref="A1:Y1009"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -12484,13 +12478,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="118" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="120"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -12635,7 +12629,7 @@
     <row r="7" spans="1:25" ht="13.5" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="57">
         <f>('July 2024 - September 2024'!C7)+SUM(E79,E86,E94)</f>
@@ -12693,13 +12687,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="118" t="s">
+      <c r="A10" s="121" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="119"/>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="108"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="95"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -12727,10 +12721,10 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="120" t="s">
+      <c r="C11" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="92"/>
+      <c r="D11" s="84"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
@@ -12742,10 +12736,10 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="116" t="s">
+      <c r="C12" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="117"/>
+      <c r="D12" s="92"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -12767,13 +12761,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="121" t="s">
         <v>113</v>
       </c>
-      <c r="B15" s="119"/>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="108"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="95"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -12801,10 +12795,10 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="120" t="s">
+      <c r="C16" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="92"/>
+      <c r="D16" s="84"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
@@ -12816,10 +12810,10 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="92"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -12844,13 +12838,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="118" t="s">
+      <c r="A20" s="121" t="s">
         <v>109</v>
       </c>
-      <c r="B20" s="119"/>
-      <c r="C20" s="119"/>
-      <c r="D20" s="119"/>
-      <c r="E20" s="108"/>
+      <c r="B20" s="94"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="95"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -12878,10 +12872,10 @@
       <c r="B21" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="121" t="s">
+      <c r="C21" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="97"/>
+      <c r="D21" s="123"/>
       <c r="E21" s="74" t="s">
         <v>4</v>
       </c>
@@ -12893,10 +12887,10 @@
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="122" t="s">
+      <c r="C22" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="123"/>
+      <c r="D22" s="125"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -12939,11 +12933,11 @@
       <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A28" s="156" t="s">
+      <c r="A28" s="147" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="91"/>
-      <c r="C28" s="92"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="84"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="20" t="s">
@@ -12958,11 +12952,11 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="101" t="s">
+      <c r="A30" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="91"/>
-      <c r="C30" s="92"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="84"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="25" t="s">
@@ -12975,7 +12969,7 @@
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="A32" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="27">
@@ -13004,16 +12998,16 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="126" t="s">
+      <c r="A35" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="127"/>
-      <c r="C35" s="128"/>
+      <c r="B35" s="110"/>
+      <c r="C35" s="111"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="129"/>
-      <c r="B36" s="107"/>
-      <c r="C36" s="130"/>
+      <c r="A36" s="112"/>
+      <c r="B36" s="113"/>
+      <c r="C36" s="114"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -13062,11 +13056,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A42" s="101" t="s">
+      <c r="A42" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="91"/>
-      <c r="C42" s="92"/>
+      <c r="B42" s="83"/>
+      <c r="C42" s="84"/>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
@@ -13101,11 +13095,11 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A46" s="101" t="s">
+      <c r="A46" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="102"/>
-      <c r="C46" s="103"/>
+      <c r="B46" s="85"/>
+      <c r="C46" s="86"/>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -13147,11 +13141,11 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="101" t="s">
+      <c r="A51" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="102"/>
-      <c r="C51" s="103"/>
+      <c r="B51" s="85"/>
+      <c r="C51" s="86"/>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="2" t="s">
@@ -13175,11 +13169,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="95" t="s">
+      <c r="A54" s="141" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="96"/>
-      <c r="C54" s="97"/>
+      <c r="B54" s="142"/>
+      <c r="C54" s="123"/>
     </row>
     <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="32" t="s">
@@ -13203,11 +13197,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="106" t="s">
+      <c r="A57" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="107"/>
-      <c r="C57" s="108"/>
+      <c r="B57" s="113"/>
+      <c r="C57" s="95"/>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
       <c r="A58" s="26" t="s">
@@ -13251,11 +13245,11 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A62" s="98" t="s">
+      <c r="A62" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="99"/>
-      <c r="C62" s="100"/>
+      <c r="B62" s="143"/>
+      <c r="C62" s="98"/>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
       <c r="A63" s="58" t="s">
@@ -13322,11 +13316,11 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A69" s="98" t="s">
+      <c r="A69" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="144"/>
-      <c r="C69" s="100"/>
+      <c r="B69" s="97"/>
+      <c r="C69" s="98"/>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
       <c r="A70" s="42" t="s">
@@ -13386,57 +13380,57 @@
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="90" t="s">
+      <c r="A77" s="104" t="s">
         <v>106</v>
       </c>
-      <c r="B77" s="91"/>
-      <c r="C77" s="91"/>
-      <c r="D77" s="91"/>
-      <c r="E77" s="92"/>
+      <c r="B77" s="83"/>
+      <c r="C77" s="83"/>
+      <c r="D77" s="83"/>
+      <c r="E77" s="84"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="93" t="s">
+      <c r="A78" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="B78" s="97"/>
-      <c r="C78" s="93" t="s">
+      <c r="B78" s="123"/>
+      <c r="C78" s="126" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="97"/>
+      <c r="D78" s="123"/>
       <c r="E78" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="152" t="s">
+      <c r="A79" s="151" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="85"/>
-      <c r="C79" s="150" t="s">
-        <v>147</v>
-      </c>
-      <c r="D79" s="151"/>
+      <c r="B79" s="136"/>
+      <c r="C79" s="149" t="s">
+        <v>146</v>
+      </c>
+      <c r="D79" s="150"/>
       <c r="E79" s="75">
         <v>1200</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="109" t="s">
+      <c r="A80" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="110"/>
-      <c r="C80" s="139"/>
-      <c r="D80" s="140"/>
+      <c r="B80" s="132"/>
+      <c r="C80" s="87"/>
+      <c r="D80" s="88"/>
       <c r="E80" s="44">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C81" s="111" t="s">
+      <c r="C81" s="144" t="s">
         <v>41</v>
       </c>
-      <c r="D81" s="91"/>
+      <c r="D81" s="83"/>
       <c r="E81" s="37">
         <f>(C6+E13)-SUM(E79:E80)</f>
         <v>658.39999999999964</v>
@@ -13444,69 +13438,69 @@
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="90" t="s">
+      <c r="A83" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="B83" s="91"/>
-      <c r="C83" s="91"/>
-      <c r="D83" s="91"/>
-      <c r="E83" s="92"/>
+      <c r="B83" s="83"/>
+      <c r="C83" s="83"/>
+      <c r="D83" s="83"/>
+      <c r="E83" s="84"/>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="90" t="s">
+      <c r="A84" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="92"/>
-      <c r="C84" s="90" t="s">
+      <c r="B84" s="84"/>
+      <c r="C84" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="92"/>
+      <c r="D84" s="84"/>
       <c r="E84" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="142" t="s">
+      <c r="A85" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="B85" s="117"/>
-      <c r="C85" s="135"/>
-      <c r="D85" s="149"/>
+      <c r="B85" s="92"/>
+      <c r="C85" s="102"/>
+      <c r="D85" s="156"/>
       <c r="E85" s="37">
         <f>E81</f>
         <v>658.39999999999964</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="142" t="s">
+      <c r="A86" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="B86" s="146"/>
-      <c r="C86" s="124" t="s">
-        <v>147</v>
-      </c>
-      <c r="D86" s="148"/>
+      <c r="B86" s="101"/>
+      <c r="C86" s="105" t="s">
+        <v>146</v>
+      </c>
+      <c r="D86" s="155"/>
       <c r="E86" s="52">
         <v>1200</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="142" t="s">
+      <c r="A87" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="117"/>
-      <c r="C87" s="134"/>
-      <c r="D87" s="92"/>
+      <c r="B87" s="92"/>
+      <c r="C87" s="99"/>
+      <c r="D87" s="84"/>
       <c r="E87" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C88" s="137" t="s">
+      <c r="C88" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="92"/>
+      <c r="D88" s="84"/>
       <c r="E88" s="37">
         <f>(E18+E85)-SUM(E86:E87)</f>
         <v>564.39999999999964</v>
@@ -13527,69 +13521,69 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="143" t="s">
+      <c r="A91" s="93" t="s">
         <v>112</v>
       </c>
-      <c r="B91" s="119"/>
-      <c r="C91" s="119"/>
-      <c r="D91" s="119"/>
-      <c r="E91" s="108"/>
+      <c r="B91" s="94"/>
+      <c r="C91" s="94"/>
+      <c r="D91" s="94"/>
+      <c r="E91" s="95"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="90" t="s">
+      <c r="A92" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B92" s="92"/>
-      <c r="C92" s="90" t="s">
+      <c r="B92" s="84"/>
+      <c r="C92" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="D92" s="92"/>
+      <c r="D92" s="84"/>
       <c r="E92" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="142" t="s">
+      <c r="A93" s="91" t="s">
         <v>116</v>
       </c>
-      <c r="B93" s="117"/>
-      <c r="C93" s="134"/>
-      <c r="D93" s="92"/>
+      <c r="B93" s="92"/>
+      <c r="C93" s="99"/>
+      <c r="D93" s="84"/>
       <c r="E93" s="37">
         <f>E88</f>
         <v>564.39999999999964</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="142" t="s">
+      <c r="A94" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="146"/>
-      <c r="C94" s="124" t="s">
-        <v>147</v>
-      </c>
-      <c r="D94" s="138"/>
+      <c r="B94" s="101"/>
+      <c r="C94" s="105" t="s">
+        <v>146</v>
+      </c>
+      <c r="D94" s="106"/>
       <c r="E94" s="52">
         <v>1200</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="142" t="s">
+      <c r="A95" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B95" s="117"/>
-      <c r="C95" s="134"/>
-      <c r="D95" s="92"/>
+      <c r="B95" s="92"/>
+      <c r="C95" s="99"/>
+      <c r="D95" s="84"/>
       <c r="E95" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C96" s="137" t="s">
+      <c r="C96" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="D96" s="92"/>
+      <c r="D96" s="84"/>
       <c r="E96" s="52">
         <f>(E23+E93)-SUM(E94:E95)</f>
         <v>470.39999999999964</v>
@@ -17249,36 +17243,11 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A35:C36"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="A77:E77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="A86:B86"/>
     <mergeCell ref="C88:D88"/>
@@ -17292,11 +17261,36 @@
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="C84:D84"/>
     <mergeCell ref="C79:D79"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A77:E77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A35:C36"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A15:E15"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="47" priority="2" operator="lessThan">
@@ -17374,13 +17368,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="113" t="s">
-        <v>121</v>
-      </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="115"/>
+      <c r="A1" s="118" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="120"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -17525,7 +17519,7 @@
     <row r="7" spans="1:25" ht="13.5" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="57">
         <f>('October 2024 - December 2024'!C7)+SUM(E79,E86,E94)</f>
@@ -17583,13 +17577,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="118" t="s">
-        <v>122</v>
-      </c>
-      <c r="B10" s="119"/>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="108"/>
+      <c r="A10" s="121" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="94"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="95"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -17617,25 +17611,25 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="120" t="s">
+      <c r="C11" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="92"/>
+      <c r="D11" s="84"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="13.5" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="116" t="s">
+      <c r="C12" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="117"/>
+      <c r="D12" s="92"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -17657,13 +17651,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="118" t="s">
-        <v>129</v>
-      </c>
-      <c r="B15" s="119"/>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="108"/>
+      <c r="A15" s="121" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="95"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -17691,25 +17685,25 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="120" t="s">
+      <c r="C16" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="92"/>
+      <c r="D16" s="84"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="13.15" customHeight="1">
       <c r="A17" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="92"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -17734,13 +17728,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="118" t="s">
-        <v>124</v>
-      </c>
-      <c r="B20" s="119"/>
-      <c r="C20" s="119"/>
-      <c r="D20" s="119"/>
-      <c r="E20" s="108"/>
+      <c r="A20" s="121" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="94"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="95"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -17768,25 +17762,25 @@
       <c r="B21" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="121" t="s">
+      <c r="C21" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="97"/>
+      <c r="D21" s="123"/>
       <c r="E21" s="74" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="13.15" customHeight="1">
       <c r="A22" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="122" t="s">
+      <c r="C22" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="123"/>
+      <c r="D22" s="125"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -17829,11 +17823,11 @@
       <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A28" s="156" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="91"/>
-      <c r="C28" s="92"/>
+      <c r="A28" s="147" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="83"/>
+      <c r="C28" s="84"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="20" t="s">
@@ -17848,11 +17842,11 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="101" t="s">
+      <c r="A30" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="91"/>
-      <c r="C30" s="92"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="84"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="25" t="s">
@@ -17865,7 +17859,7 @@
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="A32" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="27">
@@ -17894,16 +17888,16 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="126" t="s">
+      <c r="A35" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="127"/>
-      <c r="C35" s="128"/>
+      <c r="B35" s="110"/>
+      <c r="C35" s="111"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="129"/>
-      <c r="B36" s="107"/>
-      <c r="C36" s="130"/>
+      <c r="A36" s="112"/>
+      <c r="B36" s="113"/>
+      <c r="C36" s="114"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -17952,11 +17946,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A42" s="101" t="s">
+      <c r="A42" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="91"/>
-      <c r="C42" s="92"/>
+      <c r="B42" s="83"/>
+      <c r="C42" s="84"/>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
@@ -17991,11 +17985,11 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A46" s="101" t="s">
+      <c r="A46" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="102"/>
-      <c r="C46" s="103"/>
+      <c r="B46" s="85"/>
+      <c r="C46" s="86"/>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -18037,11 +18031,11 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="101" t="s">
+      <c r="A51" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="102"/>
-      <c r="C51" s="103"/>
+      <c r="B51" s="85"/>
+      <c r="C51" s="86"/>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="2" t="s">
@@ -18065,11 +18059,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="95" t="s">
+      <c r="A54" s="141" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="96"/>
-      <c r="C54" s="97"/>
+      <c r="B54" s="142"/>
+      <c r="C54" s="123"/>
     </row>
     <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="32" t="s">
@@ -18093,11 +18087,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="106" t="s">
+      <c r="A57" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="107"/>
-      <c r="C57" s="108"/>
+      <c r="B57" s="113"/>
+      <c r="C57" s="95"/>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
       <c r="A58" s="26" t="s">
@@ -18141,11 +18135,11 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A62" s="98" t="s">
+      <c r="A62" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="99"/>
-      <c r="C62" s="100"/>
+      <c r="B62" s="143"/>
+      <c r="C62" s="98"/>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
       <c r="A63" s="58" t="s">
@@ -18212,11 +18206,11 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A69" s="98" t="s">
+      <c r="A69" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="144"/>
-      <c r="C69" s="100"/>
+      <c r="B69" s="97"/>
+      <c r="C69" s="98"/>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
       <c r="A70" s="42" t="s">
@@ -18276,57 +18270,57 @@
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="90" t="s">
-        <v>127</v>
-      </c>
-      <c r="B77" s="91"/>
-      <c r="C77" s="91"/>
-      <c r="D77" s="91"/>
-      <c r="E77" s="92"/>
+      <c r="A77" s="104" t="s">
+        <v>126</v>
+      </c>
+      <c r="B77" s="83"/>
+      <c r="C77" s="83"/>
+      <c r="D77" s="83"/>
+      <c r="E77" s="84"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="93" t="s">
+      <c r="A78" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="B78" s="97"/>
-      <c r="C78" s="93" t="s">
+      <c r="B78" s="123"/>
+      <c r="C78" s="126" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="97"/>
+      <c r="D78" s="123"/>
       <c r="E78" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="152" t="s">
+      <c r="A79" s="151" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="85"/>
-      <c r="C79" s="150" t="s">
-        <v>147</v>
-      </c>
-      <c r="D79" s="151"/>
+      <c r="B79" s="136"/>
+      <c r="C79" s="149" t="s">
+        <v>146</v>
+      </c>
+      <c r="D79" s="150"/>
       <c r="E79" s="75">
         <v>1200</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="109" t="s">
+      <c r="A80" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="110"/>
-      <c r="C80" s="139"/>
-      <c r="D80" s="140"/>
+      <c r="B80" s="132"/>
+      <c r="C80" s="87"/>
+      <c r="D80" s="88"/>
       <c r="E80" s="44">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C81" s="111" t="s">
+      <c r="C81" s="144" t="s">
         <v>41</v>
       </c>
-      <c r="D81" s="91"/>
+      <c r="D81" s="83"/>
       <c r="E81" s="37">
         <f>(C6+E13)-SUM(E79:E80)</f>
         <v>402.59999999999945</v>
@@ -18334,69 +18328,69 @@
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="90" t="s">
-        <v>131</v>
-      </c>
-      <c r="B83" s="91"/>
-      <c r="C83" s="91"/>
-      <c r="D83" s="91"/>
-      <c r="E83" s="92"/>
+      <c r="A83" s="104" t="s">
+        <v>130</v>
+      </c>
+      <c r="B83" s="83"/>
+      <c r="C83" s="83"/>
+      <c r="D83" s="83"/>
+      <c r="E83" s="84"/>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="90" t="s">
+      <c r="A84" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="92"/>
-      <c r="C84" s="90" t="s">
+      <c r="B84" s="84"/>
+      <c r="C84" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="92"/>
+      <c r="D84" s="84"/>
       <c r="E84" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="142" t="s">
-        <v>145</v>
-      </c>
-      <c r="B85" s="117"/>
-      <c r="C85" s="135"/>
-      <c r="D85" s="149"/>
+      <c r="A85" s="91" t="s">
+        <v>144</v>
+      </c>
+      <c r="B85" s="92"/>
+      <c r="C85" s="102"/>
+      <c r="D85" s="156"/>
       <c r="E85" s="37">
         <f>E81</f>
         <v>402.59999999999945</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="142" t="s">
+      <c r="A86" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="B86" s="146"/>
-      <c r="C86" s="124" t="s">
-        <v>164</v>
-      </c>
-      <c r="D86" s="148"/>
+      <c r="B86" s="101"/>
+      <c r="C86" s="105" t="s">
+        <v>163</v>
+      </c>
+      <c r="D86" s="155"/>
       <c r="E86" s="52">
         <v>1100</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="142" t="s">
+      <c r="A87" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="117"/>
-      <c r="C87" s="134"/>
-      <c r="D87" s="92"/>
+      <c r="B87" s="92"/>
+      <c r="C87" s="99"/>
+      <c r="D87" s="84"/>
       <c r="E87" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C88" s="137" t="s">
+      <c r="C88" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="92"/>
+      <c r="D88" s="84"/>
       <c r="E88" s="37">
         <f>(E18+E85)-SUM(E86:E87)</f>
         <v>408.59999999999945</v>
@@ -18417,69 +18411,69 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="143" t="s">
-        <v>128</v>
-      </c>
-      <c r="B91" s="119"/>
-      <c r="C91" s="119"/>
-      <c r="D91" s="119"/>
-      <c r="E91" s="108"/>
+      <c r="A91" s="93" t="s">
+        <v>127</v>
+      </c>
+      <c r="B91" s="94"/>
+      <c r="C91" s="94"/>
+      <c r="D91" s="94"/>
+      <c r="E91" s="95"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="90" t="s">
+      <c r="A92" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B92" s="92"/>
-      <c r="C92" s="90" t="s">
+      <c r="B92" s="84"/>
+      <c r="C92" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="D92" s="92"/>
+      <c r="D92" s="84"/>
       <c r="E92" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="142" t="s">
-        <v>146</v>
-      </c>
-      <c r="B93" s="117"/>
-      <c r="C93" s="134"/>
-      <c r="D93" s="92"/>
+      <c r="A93" s="91" t="s">
+        <v>145</v>
+      </c>
+      <c r="B93" s="92"/>
+      <c r="C93" s="99"/>
+      <c r="D93" s="84"/>
       <c r="E93" s="37">
         <f>E88</f>
         <v>408.59999999999945</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="142" t="s">
+      <c r="A94" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="146"/>
-      <c r="C94" s="124" t="s">
-        <v>164</v>
-      </c>
-      <c r="D94" s="138"/>
+      <c r="B94" s="101"/>
+      <c r="C94" s="105" t="s">
+        <v>163</v>
+      </c>
+      <c r="D94" s="106"/>
       <c r="E94" s="52">
         <v>1100</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="142" t="s">
+      <c r="A95" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B95" s="117"/>
-      <c r="C95" s="134"/>
-      <c r="D95" s="92"/>
+      <c r="B95" s="92"/>
+      <c r="C95" s="99"/>
+      <c r="D95" s="84"/>
       <c r="E95" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C96" s="137" t="s">
+      <c r="C96" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="D96" s="92"/>
+      <c r="D96" s="84"/>
       <c r="E96" s="52">
         <f>(E23+E93)-SUM(E94:E95)</f>
         <v>414.59999999999945</v>
@@ -22139,29 +22133,18 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="A91:E91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="A83:E83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A28:C28"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="A35:C36"/>
@@ -22175,18 +22158,29 @@
     <mergeCell ref="A77:E77"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="A91:E91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="35" priority="2" operator="lessThan">
@@ -22264,13 +22258,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="113" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="115"/>
+      <c r="A1" s="118" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="120"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -22415,7 +22409,7 @@
     <row r="7" spans="1:25" ht="13.5" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="57">
         <f>('January 2025 - March 2025'!C7)+SUM(E79,E86,E94)</f>
@@ -22473,13 +22467,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="118" t="s">
-        <v>132</v>
-      </c>
-      <c r="B10" s="119"/>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="108"/>
+      <c r="A10" s="121" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="94"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="95"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -22507,25 +22501,25 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="120" t="s">
+      <c r="C11" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="92"/>
+      <c r="D11" s="84"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="13.5" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="116" t="s">
+      <c r="C12" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="117"/>
+      <c r="D12" s="92"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -22547,13 +22541,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="118" t="s">
-        <v>140</v>
-      </c>
-      <c r="B15" s="119"/>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="108"/>
+      <c r="A15" s="121" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="95"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -22581,25 +22575,25 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="120" t="s">
+      <c r="C16" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="92"/>
+      <c r="D16" s="84"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="13.15" customHeight="1">
       <c r="A17" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="92"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -22624,13 +22618,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="118" t="s">
-        <v>136</v>
-      </c>
-      <c r="B20" s="119"/>
-      <c r="C20" s="119"/>
-      <c r="D20" s="119"/>
-      <c r="E20" s="108"/>
+      <c r="A20" s="121" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="94"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="95"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -22658,25 +22652,25 @@
       <c r="B21" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="121" t="s">
+      <c r="C21" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="97"/>
+      <c r="D21" s="123"/>
       <c r="E21" s="74" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="13.15" customHeight="1">
       <c r="A22" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="122" t="s">
+      <c r="C22" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="123"/>
+      <c r="D22" s="125"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -22719,11 +22713,11 @@
       <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A28" s="156" t="s">
-        <v>138</v>
-      </c>
-      <c r="B28" s="91"/>
-      <c r="C28" s="92"/>
+      <c r="A28" s="147" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" s="83"/>
+      <c r="C28" s="84"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="20" t="s">
@@ -22738,11 +22732,11 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="101" t="s">
+      <c r="A30" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="91"/>
-      <c r="C30" s="92"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="84"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="25" t="s">
@@ -22755,7 +22749,7 @@
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="A32" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="27">
@@ -22784,16 +22778,16 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="126" t="s">
+      <c r="A35" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="127"/>
-      <c r="C35" s="128"/>
+      <c r="B35" s="110"/>
+      <c r="C35" s="111"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="129"/>
-      <c r="B36" s="107"/>
-      <c r="C36" s="130"/>
+      <c r="A36" s="112"/>
+      <c r="B36" s="113"/>
+      <c r="C36" s="114"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -22842,11 +22836,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A42" s="101" t="s">
+      <c r="A42" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="91"/>
-      <c r="C42" s="92"/>
+      <c r="B42" s="83"/>
+      <c r="C42" s="84"/>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
@@ -22881,11 +22875,11 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A46" s="101" t="s">
+      <c r="A46" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="102"/>
-      <c r="C46" s="103"/>
+      <c r="B46" s="85"/>
+      <c r="C46" s="86"/>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -22927,11 +22921,11 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="101" t="s">
+      <c r="A51" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="102"/>
-      <c r="C51" s="103"/>
+      <c r="B51" s="85"/>
+      <c r="C51" s="86"/>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="2" t="s">
@@ -22955,11 +22949,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="95" t="s">
+      <c r="A54" s="141" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="96"/>
-      <c r="C54" s="97"/>
+      <c r="B54" s="142"/>
+      <c r="C54" s="123"/>
     </row>
     <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="32" t="s">
@@ -22983,11 +22977,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="106" t="s">
+      <c r="A57" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="107"/>
-      <c r="C57" s="108"/>
+      <c r="B57" s="113"/>
+      <c r="C57" s="95"/>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
       <c r="A58" s="26" t="s">
@@ -23031,11 +23025,11 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A62" s="98" t="s">
+      <c r="A62" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="99"/>
-      <c r="C62" s="100"/>
+      <c r="B62" s="143"/>
+      <c r="C62" s="98"/>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
       <c r="A63" s="58" t="s">
@@ -23102,11 +23096,11 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A69" s="98" t="s">
+      <c r="A69" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="144"/>
-      <c r="C69" s="100"/>
+      <c r="B69" s="97"/>
+      <c r="C69" s="98"/>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
       <c r="A70" s="42" t="s">
@@ -23166,57 +23160,57 @@
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="90" t="s">
-        <v>134</v>
-      </c>
-      <c r="B77" s="91"/>
-      <c r="C77" s="91"/>
-      <c r="D77" s="91"/>
-      <c r="E77" s="92"/>
+      <c r="A77" s="104" t="s">
+        <v>133</v>
+      </c>
+      <c r="B77" s="83"/>
+      <c r="C77" s="83"/>
+      <c r="D77" s="83"/>
+      <c r="E77" s="84"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="93" t="s">
+      <c r="A78" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="B78" s="97"/>
-      <c r="C78" s="93" t="s">
+      <c r="B78" s="123"/>
+      <c r="C78" s="126" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="97"/>
+      <c r="D78" s="123"/>
       <c r="E78" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="152" t="s">
+      <c r="A79" s="151" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="85"/>
-      <c r="C79" s="150" t="s">
-        <v>164</v>
-      </c>
-      <c r="D79" s="151"/>
+      <c r="B79" s="136"/>
+      <c r="C79" s="149" t="s">
+        <v>163</v>
+      </c>
+      <c r="D79" s="150"/>
       <c r="E79" s="75">
         <v>1100</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="109" t="s">
+      <c r="A80" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="110"/>
-      <c r="C80" s="139"/>
-      <c r="D80" s="140"/>
+      <c r="B80" s="132"/>
+      <c r="C80" s="87"/>
+      <c r="D80" s="88"/>
       <c r="E80" s="44">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C81" s="111" t="s">
+      <c r="C81" s="144" t="s">
         <v>41</v>
       </c>
-      <c r="D81" s="91"/>
+      <c r="D81" s="83"/>
       <c r="E81" s="37">
         <f>(C6+E13)-SUM(E79:E80)</f>
         <v>446.79999999999927</v>
@@ -23224,69 +23218,69 @@
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="90" t="s">
-        <v>142</v>
-      </c>
-      <c r="B83" s="91"/>
-      <c r="C83" s="91"/>
-      <c r="D83" s="91"/>
-      <c r="E83" s="92"/>
+      <c r="A83" s="104" t="s">
+        <v>141</v>
+      </c>
+      <c r="B83" s="83"/>
+      <c r="C83" s="83"/>
+      <c r="D83" s="83"/>
+      <c r="E83" s="84"/>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="90" t="s">
+      <c r="A84" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="92"/>
-      <c r="C84" s="90" t="s">
+      <c r="B84" s="84"/>
+      <c r="C84" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="92"/>
+      <c r="D84" s="84"/>
       <c r="E84" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="142" t="s">
-        <v>143</v>
-      </c>
-      <c r="B85" s="117"/>
-      <c r="C85" s="135"/>
-      <c r="D85" s="149"/>
+      <c r="A85" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="B85" s="92"/>
+      <c r="C85" s="102"/>
+      <c r="D85" s="156"/>
       <c r="E85" s="37">
         <f>E81</f>
         <v>446.79999999999927</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="142" t="s">
+      <c r="A86" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="B86" s="146"/>
-      <c r="C86" s="124" t="s">
-        <v>165</v>
-      </c>
-      <c r="D86" s="148"/>
+      <c r="B86" s="101"/>
+      <c r="C86" s="105" t="s">
+        <v>164</v>
+      </c>
+      <c r="D86" s="155"/>
       <c r="E86" s="52">
         <v>1100</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="142" t="s">
+      <c r="A87" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="117"/>
-      <c r="C87" s="134"/>
-      <c r="D87" s="92"/>
+      <c r="B87" s="92"/>
+      <c r="C87" s="99"/>
+      <c r="D87" s="84"/>
       <c r="E87" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C88" s="137" t="s">
+      <c r="C88" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="92"/>
+      <c r="D88" s="84"/>
       <c r="E88" s="37">
         <f>(E18+E85)-SUM(E86:E87)</f>
         <v>452.79999999999927</v>
@@ -23307,69 +23301,69 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="143" t="s">
-        <v>139</v>
-      </c>
-      <c r="B91" s="119"/>
-      <c r="C91" s="119"/>
-      <c r="D91" s="119"/>
-      <c r="E91" s="108"/>
+      <c r="A91" s="93" t="s">
+        <v>138</v>
+      </c>
+      <c r="B91" s="94"/>
+      <c r="C91" s="94"/>
+      <c r="D91" s="94"/>
+      <c r="E91" s="95"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="90" t="s">
+      <c r="A92" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B92" s="92"/>
-      <c r="C92" s="90" t="s">
+      <c r="B92" s="84"/>
+      <c r="C92" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="D92" s="92"/>
+      <c r="D92" s="84"/>
       <c r="E92" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="142" t="s">
-        <v>144</v>
-      </c>
-      <c r="B93" s="117"/>
-      <c r="C93" s="134"/>
-      <c r="D93" s="92"/>
+      <c r="A93" s="91" t="s">
+        <v>143</v>
+      </c>
+      <c r="B93" s="92"/>
+      <c r="C93" s="99"/>
+      <c r="D93" s="84"/>
       <c r="E93" s="37">
         <f>E88</f>
         <v>452.79999999999927</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="142" t="s">
+      <c r="A94" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="146"/>
-      <c r="C94" s="124" t="s">
-        <v>166</v>
-      </c>
-      <c r="D94" s="138"/>
+      <c r="B94" s="101"/>
+      <c r="C94" s="105" t="s">
+        <v>165</v>
+      </c>
+      <c r="D94" s="106"/>
       <c r="E94" s="52">
         <v>739</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="142" t="s">
+      <c r="A95" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B95" s="117"/>
-      <c r="C95" s="134"/>
-      <c r="D95" s="92"/>
+      <c r="B95" s="92"/>
+      <c r="C95" s="99"/>
+      <c r="D95" s="84"/>
       <c r="E95" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C96" s="137" t="s">
+      <c r="C96" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="D96" s="92"/>
+      <c r="D96" s="84"/>
       <c r="E96" s="52">
         <f>(E23+E93)-SUM(E94:E95)</f>
         <v>819.79999999999927</v>
@@ -27029,29 +27023,18 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="A91:E91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="A83:E83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A28:C28"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="A35:C36"/>
@@ -27065,18 +27048,29 @@
     <mergeCell ref="A77:E77"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="A91:E91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="23" priority="2" operator="lessThan">
@@ -27154,13 +27148,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="113" t="s">
-        <v>152</v>
-      </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="115"/>
+      <c r="A1" s="118" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="120"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -27305,7 +27299,7 @@
     <row r="7" spans="1:25" ht="13.5" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="57">
         <f>('April 2025 - June 2025'!C7)</f>
@@ -27363,13 +27357,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="118" t="s">
-        <v>148</v>
-      </c>
-      <c r="B10" s="119"/>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="108"/>
+      <c r="A10" s="121" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="94"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="95"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -27397,25 +27391,25 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="120" t="s">
+      <c r="C11" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="92"/>
+      <c r="D11" s="84"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="13.5" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="116" t="s">
+      <c r="C12" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="117"/>
+      <c r="D12" s="92"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -27437,13 +27431,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="118" t="s">
-        <v>157</v>
-      </c>
-      <c r="B15" s="119"/>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="108"/>
+      <c r="A15" s="121" t="s">
+        <v>156</v>
+      </c>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="95"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -27471,25 +27465,25 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="120" t="s">
+      <c r="C16" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="92"/>
+      <c r="D16" s="84"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="13.15" customHeight="1">
       <c r="A17" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="92"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -27514,13 +27508,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="118" t="s">
-        <v>153</v>
-      </c>
-      <c r="B20" s="119"/>
-      <c r="C20" s="119"/>
-      <c r="D20" s="119"/>
-      <c r="E20" s="108"/>
+      <c r="A20" s="121" t="s">
+        <v>152</v>
+      </c>
+      <c r="B20" s="94"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="95"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -27548,25 +27542,25 @@
       <c r="B21" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="121" t="s">
+      <c r="C21" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="97"/>
+      <c r="D21" s="123"/>
       <c r="E21" s="74" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="13.15" customHeight="1">
       <c r="A22" s="33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="122" t="s">
+      <c r="C22" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="123"/>
+      <c r="D22" s="125"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -27609,11 +27603,11 @@
       <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A28" s="156" t="s">
-        <v>155</v>
-      </c>
-      <c r="B28" s="91"/>
-      <c r="C28" s="92"/>
+      <c r="A28" s="147" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" s="83"/>
+      <c r="C28" s="84"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="20" t="s">
@@ -27628,11 +27622,11 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="101" t="s">
+      <c r="A30" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="91"/>
-      <c r="C30" s="92"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="84"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="25" t="s">
@@ -27645,7 +27639,7 @@
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="A32" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="27">
@@ -27674,16 +27668,16 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="126" t="s">
+      <c r="A35" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="127"/>
-      <c r="C35" s="128"/>
+      <c r="B35" s="110"/>
+      <c r="C35" s="111"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="129"/>
-      <c r="B36" s="107"/>
-      <c r="C36" s="130"/>
+      <c r="A36" s="112"/>
+      <c r="B36" s="113"/>
+      <c r="C36" s="114"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -27732,11 +27726,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A42" s="101" t="s">
+      <c r="A42" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="91"/>
-      <c r="C42" s="92"/>
+      <c r="B42" s="83"/>
+      <c r="C42" s="84"/>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
@@ -27771,11 +27765,11 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A46" s="101" t="s">
+      <c r="A46" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="102"/>
-      <c r="C46" s="103"/>
+      <c r="B46" s="85"/>
+      <c r="C46" s="86"/>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -27817,11 +27811,11 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="101" t="s">
+      <c r="A51" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="102"/>
-      <c r="C51" s="103"/>
+      <c r="B51" s="85"/>
+      <c r="C51" s="86"/>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="2" t="s">
@@ -27845,11 +27839,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="95" t="s">
+      <c r="A54" s="141" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="96"/>
-      <c r="C54" s="97"/>
+      <c r="B54" s="142"/>
+      <c r="C54" s="123"/>
     </row>
     <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="32" t="s">
@@ -27873,11 +27867,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="106" t="s">
+      <c r="A57" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="107"/>
-      <c r="C57" s="108"/>
+      <c r="B57" s="113"/>
+      <c r="C57" s="95"/>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
       <c r="A58" s="26" t="s">
@@ -27921,11 +27915,11 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A62" s="98" t="s">
+      <c r="A62" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="99"/>
-      <c r="C62" s="100"/>
+      <c r="B62" s="143"/>
+      <c r="C62" s="98"/>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
       <c r="A63" s="58" t="s">
@@ -27992,11 +27986,11 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A69" s="98" t="s">
+      <c r="A69" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="144"/>
-      <c r="C69" s="100"/>
+      <c r="B69" s="97"/>
+      <c r="C69" s="98"/>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
       <c r="A70" s="42" t="s">
@@ -28055,23 +28049,23 @@
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="90" t="s">
-        <v>150</v>
-      </c>
-      <c r="B77" s="91"/>
-      <c r="C77" s="91"/>
-      <c r="D77" s="91"/>
-      <c r="E77" s="92"/>
+      <c r="A77" s="104" t="s">
+        <v>149</v>
+      </c>
+      <c r="B77" s="83"/>
+      <c r="C77" s="83"/>
+      <c r="D77" s="83"/>
+      <c r="E77" s="84"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="93" t="s">
+      <c r="A78" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="B78" s="97"/>
-      <c r="C78" s="93" t="s">
+      <c r="B78" s="123"/>
+      <c r="C78" s="126" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="97"/>
+      <c r="D78" s="123"/>
       <c r="E78" s="43" t="s">
         <v>4</v>
       </c>
@@ -28081,8 +28075,8 @@
         <v>82</v>
       </c>
       <c r="B79" s="157"/>
-      <c r="C79" s="160"/>
-      <c r="D79" s="161"/>
+      <c r="C79" s="158"/>
+      <c r="D79" s="159"/>
       <c r="E79" s="52">
         <v>0</v>
       </c>
@@ -28092,8 +28086,8 @@
         <v>40</v>
       </c>
       <c r="B80" s="157"/>
-      <c r="C80" s="158"/>
-      <c r="D80" s="158"/>
+      <c r="C80" s="160"/>
+      <c r="D80" s="160"/>
       <c r="E80" s="80">
         <f>C74</f>
         <v>1299</v>
@@ -28102,10 +28096,10 @@
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
       <c r="A81" s="78"/>
       <c r="B81" s="78"/>
-      <c r="C81" s="159" t="s">
+      <c r="C81" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="D81" s="107"/>
+      <c r="D81" s="113"/>
       <c r="E81" s="79">
         <f>(C6+E13)-SUM(E79:E80)</f>
         <v>1951.9999999999991</v>
@@ -28113,67 +28107,67 @@
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="90" t="s">
-        <v>159</v>
-      </c>
-      <c r="B83" s="91"/>
-      <c r="C83" s="91"/>
-      <c r="D83" s="91"/>
-      <c r="E83" s="92"/>
+      <c r="A83" s="104" t="s">
+        <v>158</v>
+      </c>
+      <c r="B83" s="83"/>
+      <c r="C83" s="83"/>
+      <c r="D83" s="83"/>
+      <c r="E83" s="84"/>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="90" t="s">
+      <c r="A84" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="92"/>
-      <c r="C84" s="90" t="s">
+      <c r="B84" s="84"/>
+      <c r="C84" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="92"/>
+      <c r="D84" s="84"/>
       <c r="E84" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="142" t="s">
-        <v>151</v>
-      </c>
-      <c r="B85" s="117"/>
-      <c r="C85" s="135"/>
-      <c r="D85" s="149"/>
+      <c r="A85" s="91" t="s">
+        <v>150</v>
+      </c>
+      <c r="B85" s="92"/>
+      <c r="C85" s="102"/>
+      <c r="D85" s="156"/>
       <c r="E85" s="37">
         <f>E81</f>
         <v>1951.9999999999991</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="142" t="s">
+      <c r="A86" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="B86" s="146"/>
-      <c r="C86" s="124"/>
-      <c r="D86" s="148"/>
+      <c r="B86" s="101"/>
+      <c r="C86" s="105"/>
+      <c r="D86" s="155"/>
       <c r="E86" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="142" t="s">
+      <c r="A87" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="117"/>
-      <c r="C87" s="134"/>
-      <c r="D87" s="92"/>
+      <c r="B87" s="92"/>
+      <c r="C87" s="99"/>
+      <c r="D87" s="84"/>
       <c r="E87" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C88" s="137" t="s">
+      <c r="C88" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="92"/>
+      <c r="D88" s="84"/>
       <c r="E88" s="37">
         <f>(E18+E85)-SUM(E86:E87)</f>
         <v>3057.9999999999991</v>
@@ -28194,67 +28188,67 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="143" t="s">
-        <v>156</v>
-      </c>
-      <c r="B91" s="119"/>
-      <c r="C91" s="119"/>
-      <c r="D91" s="119"/>
-      <c r="E91" s="108"/>
+      <c r="A91" s="93" t="s">
+        <v>155</v>
+      </c>
+      <c r="B91" s="94"/>
+      <c r="C91" s="94"/>
+      <c r="D91" s="94"/>
+      <c r="E91" s="95"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="90" t="s">
+      <c r="A92" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B92" s="92"/>
-      <c r="C92" s="90" t="s">
+      <c r="B92" s="84"/>
+      <c r="C92" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="D92" s="92"/>
+      <c r="D92" s="84"/>
       <c r="E92" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="142" t="s">
-        <v>160</v>
-      </c>
-      <c r="B93" s="117"/>
-      <c r="C93" s="134"/>
-      <c r="D93" s="92"/>
+      <c r="A93" s="91" t="s">
+        <v>159</v>
+      </c>
+      <c r="B93" s="92"/>
+      <c r="C93" s="99"/>
+      <c r="D93" s="84"/>
       <c r="E93" s="37">
         <f>E88</f>
         <v>3057.9999999999991</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="142" t="s">
+      <c r="A94" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="146"/>
-      <c r="C94" s="124"/>
-      <c r="D94" s="138"/>
+      <c r="B94" s="101"/>
+      <c r="C94" s="105"/>
+      <c r="D94" s="106"/>
       <c r="E94" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="142" t="s">
+      <c r="A95" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B95" s="117"/>
-      <c r="C95" s="134"/>
-      <c r="D95" s="92"/>
+      <c r="B95" s="92"/>
+      <c r="C95" s="99"/>
+      <c r="D95" s="84"/>
       <c r="E95" s="66">
         <f>C74</f>
         <v>1299</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C96" s="137" t="s">
+      <c r="C96" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="D96" s="92"/>
+      <c r="D96" s="84"/>
       <c r="E96" s="52">
         <f>(E23+E93)-SUM(E94:E95)</f>
         <v>4163.9999999999991</v>
@@ -31914,18 +31908,29 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="A91:E91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="C84:D84"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="A35:C36"/>
@@ -31939,29 +31944,18 @@
     <mergeCell ref="A77:E77"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="A83:E83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="A91:E91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A28:C28"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
docs: Updated Income and Expense
</commit_message>
<xml_diff>
--- a/Alan Tang_s Income Expense Now.xlsx
+++ b/Alan Tang_s Income Expense Now.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Income-Expenditure-Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB63850-F6F8-4609-BF92-E67A22509A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6619958-8F1E-4CCB-826D-5D0B227E1E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="April 2024 - June 2024" sheetId="1" r:id="rId1"/>
@@ -1534,29 +1534,20 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1567,17 +1558,50 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1591,10 +1615,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1612,17 +1639,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1634,18 +1652,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1669,6 +1675,9 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1679,9 +1688,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1696,35 +1702,29 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1778,7 +1778,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="71">
+  <dxfs count="73">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -2309,6 +2314,11 @@
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2523,7 +2533,7 @@
   <dimension ref="A1:Y1014"/>
   <sheetViews>
     <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+      <selection activeCell="C99" sqref="C99:D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2540,13 +2550,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="120"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="122"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -2567,7 +2577,7 @@
         <v>87</v>
       </c>
       <c r="C3" s="5">
-        <v>9.9700000000000006</v>
+        <v>0</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2598,7 +2608,7 @@
         <v>85</v>
       </c>
       <c r="C4" s="5">
-        <v>10.199999999999999</v>
+        <v>0</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -2629,7 +2639,7 @@
         <v>86</v>
       </c>
       <c r="C5" s="5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -2690,8 +2700,8 @@
       <c r="B7" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="5">
-        <v>26.2</v>
+      <c r="C7" s="57">
+        <v>-22.9</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -2721,9 +2731,9 @@
       <c r="B8" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="57">
         <f>SUM(C3:C7)</f>
-        <v>57.370000000000005</v>
+        <v>-22.9</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -2809,13 +2819,13 @@
     </row>
     <row r="11" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="12" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A12" s="122" t="s">
+      <c r="A12" s="124" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="98"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="99"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="92"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
@@ -2843,10 +2853,10 @@
       <c r="B13" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="123" t="s">
+      <c r="C13" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="94"/>
+      <c r="D13" s="83"/>
       <c r="E13" s="17" t="s">
         <v>4</v>
       </c>
@@ -2858,10 +2868,10 @@
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="121" t="s">
+      <c r="C14" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="96"/>
+      <c r="D14" s="104"/>
       <c r="E14" s="18">
         <v>2405</v>
       </c>
@@ -2883,13 +2893,13 @@
       <c r="B16" s="11"/>
     </row>
     <row r="17" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A17" s="122" t="s">
+      <c r="A17" s="124" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="98"/>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="99"/>
+      <c r="B17" s="106"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="92"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
@@ -2917,10 +2927,10 @@
       <c r="B18" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="124" t="s">
+      <c r="C18" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="82"/>
+      <c r="D18" s="127"/>
       <c r="E18" s="73" t="s">
         <v>4</v>
       </c>
@@ -2932,10 +2942,10 @@
       <c r="B19" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="125" t="s">
+      <c r="C19" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="126"/>
+      <c r="D19" s="129"/>
       <c r="E19" s="67">
         <v>2405</v>
       </c>
@@ -2947,10 +2957,10 @@
       <c r="B20" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="127" t="s">
+      <c r="C20" s="130" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="128"/>
+      <c r="D20" s="131"/>
       <c r="E20" s="67">
         <v>1035</v>
       </c>
@@ -2975,13 +2985,13 @@
       <c r="E22" s="51"/>
     </row>
     <row r="23" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A23" s="122" t="s">
+      <c r="A23" s="124" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="98"/>
-      <c r="C23" s="98"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="99"/>
+      <c r="B23" s="106"/>
+      <c r="C23" s="106"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="92"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
@@ -3009,10 +3019,10 @@
       <c r="B24" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="123" t="s">
+      <c r="C24" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="94"/>
+      <c r="D24" s="83"/>
       <c r="E24" s="17" t="s">
         <v>4</v>
       </c>
@@ -3024,10 +3034,10 @@
       <c r="B25" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="121" t="s">
+      <c r="C25" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="94"/>
+      <c r="D25" s="83"/>
       <c r="E25" s="27">
         <v>2405</v>
       </c>
@@ -3039,10 +3049,10 @@
       <c r="B26" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="C26" s="140" t="s">
+      <c r="C26" s="138" t="s">
         <v>160</v>
       </c>
-      <c r="D26" s="140"/>
+      <c r="D26" s="138"/>
       <c r="E26" s="67">
         <v>50</v>
       </c>
@@ -3078,11 +3088,11 @@
       <c r="B30" s="11"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A31" s="136" t="s">
+      <c r="A31" s="137" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="137"/>
-      <c r="C31" s="94"/>
+      <c r="B31" s="93"/>
+      <c r="C31" s="83"/>
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="A32" s="20" t="s">
@@ -3097,11 +3107,11 @@
       <c r="D32" s="22"/>
     </row>
     <row r="33" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A33" s="88" t="s">
+      <c r="A33" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="137"/>
-      <c r="C33" s="94"/>
+      <c r="B33" s="93"/>
+      <c r="C33" s="83"/>
     </row>
     <row r="34" spans="1:3" ht="13.5" customHeight="1">
       <c r="A34" s="25" t="s">
@@ -3143,16 +3153,16 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A38" s="130" t="s">
+      <c r="A38" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="131"/>
-      <c r="C38" s="132"/>
+      <c r="B38" s="133"/>
+      <c r="C38" s="134"/>
     </row>
     <row r="39" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A39" s="133"/>
-      <c r="B39" s="134"/>
-      <c r="C39" s="135"/>
+      <c r="A39" s="135"/>
+      <c r="B39" s="91"/>
+      <c r="C39" s="136"/>
     </row>
     <row r="40" spans="1:3" ht="13.5" customHeight="1">
       <c r="A40" s="2" t="s">
@@ -3201,11 +3211,11 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A45" s="88" t="s">
+      <c r="A45" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="137"/>
-      <c r="C45" s="94"/>
+      <c r="B45" s="93"/>
+      <c r="C45" s="83"/>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
       <c r="A46" s="2" t="s">
@@ -3240,11 +3250,11 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A49" s="88" t="s">
+      <c r="A49" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="89"/>
-      <c r="C49" s="90"/>
+      <c r="B49" s="86"/>
+      <c r="C49" s="87"/>
     </row>
     <row r="50" spans="1:3" ht="13.5" customHeight="1">
       <c r="A50" s="2" t="s">
@@ -3286,11 +3296,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="88" t="s">
+      <c r="A54" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="B54" s="89"/>
-      <c r="C54" s="90"/>
+      <c r="B54" s="86"/>
+      <c r="C54" s="87"/>
     </row>
     <row r="55" spans="1:3" ht="13.5" customHeight="1">
       <c r="A55" s="2" t="s">
@@ -3314,11 +3324,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="80" t="s">
+      <c r="A57" s="139" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="81"/>
-      <c r="C57" s="82"/>
+      <c r="B57" s="140"/>
+      <c r="C57" s="127"/>
     </row>
     <row r="58" spans="1:3" ht="33" customHeight="1">
       <c r="A58" s="32" t="s">
@@ -3342,11 +3352,11 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A60" s="141" t="s">
+      <c r="A60" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="B60" s="134"/>
-      <c r="C60" s="99"/>
+      <c r="B60" s="91"/>
+      <c r="C60" s="92"/>
     </row>
     <row r="61" spans="1:3" ht="13.5" customHeight="1">
       <c r="A61" s="26" t="s">
@@ -3390,11 +3400,11 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A65" s="83" t="s">
+      <c r="A65" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="84"/>
-      <c r="C65" s="85"/>
+      <c r="B65" s="141"/>
+      <c r="C65" s="109"/>
     </row>
     <row r="66" spans="1:8" ht="13.5" customHeight="1">
       <c r="A66" s="58" t="s">
@@ -3450,11 +3460,11 @@
       </c>
     </row>
     <row r="71" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A71" s="83" t="s">
+      <c r="A71" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="B71" s="100"/>
-      <c r="C71" s="85"/>
+      <c r="B71" s="108"/>
+      <c r="C71" s="109"/>
     </row>
     <row r="72" spans="1:8" ht="13.5" customHeight="1">
       <c r="A72" s="42" t="s">
@@ -3513,129 +3523,129 @@
       <c r="B78" s="11"/>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="106" t="s">
+      <c r="A79" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="B79" s="110"/>
-      <c r="C79" s="110"/>
-      <c r="D79" s="110"/>
-      <c r="E79" s="111"/>
+      <c r="B79" s="116"/>
+      <c r="C79" s="116"/>
+      <c r="D79" s="116"/>
+      <c r="E79" s="117"/>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="108" t="s">
+      <c r="A80" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B80" s="109"/>
-      <c r="C80" s="108" t="s">
+      <c r="B80" s="95"/>
+      <c r="C80" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="D80" s="109"/>
+      <c r="D80" s="95"/>
       <c r="E80" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A81" s="112" t="s">
+      <c r="A81" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="B81" s="113"/>
-      <c r="C81" s="138"/>
-      <c r="D81" s="139"/>
+      <c r="B81" s="119"/>
+      <c r="C81" s="88"/>
+      <c r="D81" s="89"/>
       <c r="E81" s="44">
         <f>C76</f>
         <v>1503</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C82" s="86" t="s">
+      <c r="C82" s="142" t="s">
         <v>41</v>
       </c>
-      <c r="D82" s="87"/>
+      <c r="D82" s="143"/>
       <c r="E82" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="106" t="s">
+      <c r="A84" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="B84" s="137"/>
-      <c r="C84" s="137"/>
-      <c r="D84" s="137"/>
-      <c r="E84" s="94"/>
+      <c r="B84" s="93"/>
+      <c r="C84" s="93"/>
+      <c r="D84" s="93"/>
+      <c r="E84" s="83"/>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="106" t="s">
+      <c r="A85" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B85" s="94"/>
-      <c r="C85" s="106" t="s">
+      <c r="B85" s="83"/>
+      <c r="C85" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D85" s="94"/>
+      <c r="D85" s="83"/>
       <c r="E85" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="95" t="s">
+      <c r="A86" s="103" t="s">
         <v>77</v>
       </c>
-      <c r="B86" s="103"/>
-      <c r="C86" s="101"/>
-      <c r="D86" s="102"/>
+      <c r="B86" s="112"/>
+      <c r="C86" s="110"/>
+      <c r="D86" s="111"/>
       <c r="E86" s="37">
         <f>E82</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="114" t="s">
+      <c r="A87" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="B87" s="115"/>
-      <c r="C87" s="91" t="s">
+      <c r="B87" s="97"/>
+      <c r="C87" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="D87" s="107"/>
+      <c r="D87" s="115"/>
       <c r="E87" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A88" s="116"/>
-      <c r="B88" s="117"/>
-      <c r="C88" s="91" t="s">
+      <c r="A88" s="100"/>
+      <c r="B88" s="101"/>
+      <c r="C88" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="D88" s="129"/>
+      <c r="D88" s="81"/>
       <c r="E88" s="52">
         <v>1000</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A89" s="95" t="s">
+      <c r="A89" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B89" s="96"/>
-      <c r="C89" s="104" t="s">
+      <c r="B89" s="104"/>
+      <c r="C89" s="113" t="s">
         <v>91</v>
       </c>
-      <c r="D89" s="105"/>
+      <c r="D89" s="114"/>
       <c r="E89" s="66">
         <f>C76</f>
         <v>1503</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C90" s="93" t="s">
+      <c r="C90" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="D90" s="94"/>
+      <c r="D90" s="83"/>
       <c r="E90" s="37">
         <f>SUM(C3:C7)</f>
-        <v>57.370000000000005</v>
+        <v>-22.9</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
@@ -3653,105 +3663,105 @@
       <c r="E92" s="24"/>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="97" t="s">
+      <c r="A93" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="B93" s="98"/>
-      <c r="C93" s="98"/>
-      <c r="D93" s="98"/>
-      <c r="E93" s="99"/>
+      <c r="B93" s="106"/>
+      <c r="C93" s="106"/>
+      <c r="D93" s="106"/>
+      <c r="E93" s="92"/>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="106" t="s">
+      <c r="A94" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B94" s="94"/>
-      <c r="C94" s="106" t="s">
+      <c r="B94" s="83"/>
+      <c r="C94" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D94" s="94"/>
+      <c r="D94" s="83"/>
       <c r="E94" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="95" t="s">
+      <c r="A95" s="103" t="s">
         <v>78</v>
       </c>
-      <c r="B95" s="96"/>
-      <c r="C95" s="101"/>
-      <c r="D95" s="94"/>
+      <c r="B95" s="104"/>
+      <c r="C95" s="110"/>
+      <c r="D95" s="83"/>
       <c r="E95" s="37">
         <f>E90</f>
-        <v>57.370000000000005</v>
+        <v>-22.9</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A96" s="114" t="s">
+      <c r="A96" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="B96" s="115"/>
-      <c r="C96" s="91" t="s">
+      <c r="B96" s="97"/>
+      <c r="C96" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="D96" s="107"/>
+      <c r="D96" s="115"/>
       <c r="E96" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A97" s="142"/>
-      <c r="B97" s="143"/>
-      <c r="C97" s="91" t="s">
+      <c r="A97" s="98"/>
+      <c r="B97" s="99"/>
+      <c r="C97" s="80" t="s">
         <v>166</v>
       </c>
-      <c r="D97" s="92"/>
+      <c r="D97" s="84"/>
       <c r="E97" s="52">
         <v>500</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A98" s="142"/>
-      <c r="B98" s="143"/>
-      <c r="C98" s="91" t="s">
+      <c r="A98" s="98"/>
+      <c r="B98" s="99"/>
+      <c r="C98" s="80" t="s">
         <v>172</v>
       </c>
-      <c r="D98" s="92"/>
+      <c r="D98" s="84"/>
       <c r="E98" s="52">
         <v>56</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A99" s="116"/>
-      <c r="B99" s="117"/>
-      <c r="C99" s="91" t="s">
+      <c r="A99" s="100"/>
+      <c r="B99" s="101"/>
+      <c r="C99" s="80" t="s">
         <v>165</v>
       </c>
-      <c r="D99" s="129"/>
+      <c r="D99" s="81"/>
       <c r="E99" s="52">
-        <v>9.9700000000000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A100" s="95" t="s">
+      <c r="A100" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B100" s="103"/>
-      <c r="C100" s="104"/>
-      <c r="D100" s="105"/>
+      <c r="B100" s="112"/>
+      <c r="C100" s="113"/>
+      <c r="D100" s="114"/>
       <c r="E100" s="52">
         <f>C76</f>
         <v>1503</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C101" s="93" t="s">
+      <c r="C101" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="D101" s="94"/>
+      <c r="D101" s="83"/>
       <c r="E101" s="52">
         <f>(E27+E95)-SUM(E96:E100)</f>
-        <v>443.39999999999964</v>
+        <v>373.09999999999991</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="13.5" customHeight="1">
@@ -7408,10 +7418,10 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C87:D87"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="A38:C39"/>
     <mergeCell ref="A31:C31"/>
@@ -7444,12 +7454,6 @@
     <mergeCell ref="A79:E79"/>
     <mergeCell ref="A81:B81"/>
     <mergeCell ref="A87:B88"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C87:D87"/>
     <mergeCell ref="C88:D88"/>
     <mergeCell ref="C94:D94"/>
     <mergeCell ref="C97:D97"/>
@@ -7460,50 +7464,61 @@
     <mergeCell ref="A84:E84"/>
     <mergeCell ref="C80:D80"/>
     <mergeCell ref="A96:B99"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A65:C65"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
+  <conditionalFormatting sqref="C7:C8">
+    <cfRule type="cellIs" dxfId="72" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="70" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E82">
-    <cfRule type="cellIs" dxfId="69" priority="26" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="70" priority="27" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="28" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86">
-    <cfRule type="cellIs" dxfId="67" priority="22" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="68" priority="23" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="24" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E90">
-    <cfRule type="cellIs" dxfId="65" priority="24" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="66" priority="25" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="26" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E95">
-    <cfRule type="cellIs" dxfId="63" priority="20" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="64" priority="21" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="63" priority="22" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E101">
-    <cfRule type="cellIs" dxfId="61" priority="18" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="62" priority="19" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="20" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7516,8 +7531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5F3FA5-5013-4B35-A74B-6269617B858B}">
   <dimension ref="A1:Y1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -7534,13 +7549,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="120"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="122"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -7562,7 +7577,7 @@
       </c>
       <c r="C3" s="5">
         <f>'April 2024 - June 2024'!E101</f>
-        <v>443.39999999999964</v>
+        <v>373.09999999999991</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7623,9 +7638,9 @@
       <c r="B5" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="57">
         <f>'April 2024 - June 2024'!C7</f>
-        <v>26.2</v>
+        <v>-22.9</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -7657,7 +7672,7 @@
       </c>
       <c r="C6" s="5">
         <f>SUM(C3:C5)</f>
-        <v>469.59999999999962</v>
+        <v>350.19999999999993</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -7743,13 +7758,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="122" t="s">
+      <c r="A10" s="124" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="98"/>
-      <c r="C10" s="98"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="99"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="92"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -7777,10 +7792,10 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="123" t="s">
+      <c r="C11" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="94"/>
+      <c r="D11" s="83"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
@@ -7792,10 +7807,10 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="121" t="s">
+      <c r="C12" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="96"/>
+      <c r="D12" s="104"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -7817,13 +7832,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="122" t="s">
+      <c r="A15" s="124" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="98"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="99"/>
+      <c r="B15" s="106"/>
+      <c r="C15" s="106"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="92"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -7851,10 +7866,10 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="123" t="s">
+      <c r="C16" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="94"/>
+      <c r="D16" s="83"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
@@ -7866,10 +7881,10 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="121" t="s">
+      <c r="C17" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="94"/>
+      <c r="D17" s="83"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -7894,13 +7909,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="122" t="s">
+      <c r="A20" s="124" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="98"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="99"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="92"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -7928,10 +7943,10 @@
       <c r="B21" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="124" t="s">
+      <c r="C21" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="82"/>
+      <c r="D21" s="127"/>
       <c r="E21" s="73" t="s">
         <v>4</v>
       </c>
@@ -7943,10 +7958,10 @@
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="126"/>
+      <c r="D22" s="129"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -8003,8 +8018,8 @@
       <c r="A29" s="146" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="137"/>
-      <c r="C29" s="94"/>
+      <c r="B29" s="93"/>
+      <c r="C29" s="83"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
       <c r="A30" s="20" t="s">
@@ -8019,11 +8034,11 @@
       <c r="D30" s="22"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A31" s="88" t="s">
+      <c r="A31" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="137"/>
-      <c r="C31" s="94"/>
+      <c r="B31" s="93"/>
+      <c r="C31" s="83"/>
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="A32" s="25" t="s">
@@ -8065,16 +8080,16 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="130" t="s">
+      <c r="A36" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="131"/>
-      <c r="C36" s="132"/>
+      <c r="B36" s="133"/>
+      <c r="C36" s="134"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A37" s="133"/>
-      <c r="B37" s="134"/>
-      <c r="C37" s="135"/>
+      <c r="A37" s="135"/>
+      <c r="B37" s="91"/>
+      <c r="C37" s="136"/>
     </row>
     <row r="38" spans="1:3" ht="13.5" customHeight="1">
       <c r="A38" s="2" t="s">
@@ -8123,11 +8138,11 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A43" s="88" t="s">
+      <c r="A43" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="137"/>
-      <c r="C43" s="94"/>
+      <c r="B43" s="93"/>
+      <c r="C43" s="83"/>
     </row>
     <row r="44" spans="1:3" ht="13.5" customHeight="1">
       <c r="A44" s="2" t="s">
@@ -8162,11 +8177,11 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A47" s="88" t="s">
+      <c r="A47" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="89"/>
-      <c r="C47" s="90"/>
+      <c r="B47" s="86"/>
+      <c r="C47" s="87"/>
     </row>
     <row r="48" spans="1:3" ht="13.5" customHeight="1">
       <c r="A48" s="2" t="s">
@@ -8208,11 +8223,11 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A52" s="88" t="s">
+      <c r="A52" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="B52" s="89"/>
-      <c r="C52" s="90"/>
+      <c r="B52" s="86"/>
+      <c r="C52" s="87"/>
     </row>
     <row r="53" spans="1:3" ht="13.5" customHeight="1">
       <c r="A53" s="2" t="s">
@@ -8236,11 +8251,11 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A55" s="80" t="s">
+      <c r="A55" s="139" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="81"/>
-      <c r="C55" s="82"/>
+      <c r="B55" s="140"/>
+      <c r="C55" s="127"/>
     </row>
     <row r="56" spans="1:3" ht="33" customHeight="1">
       <c r="A56" s="32" t="s">
@@ -8264,11 +8279,11 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A58" s="141" t="s">
+      <c r="A58" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="134"/>
-      <c r="C58" s="99"/>
+      <c r="B58" s="91"/>
+      <c r="C58" s="92"/>
     </row>
     <row r="59" spans="1:3" ht="13.5" customHeight="1">
       <c r="A59" s="26" t="s">
@@ -8312,11 +8327,11 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A63" s="83" t="s">
+      <c r="A63" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B63" s="84"/>
-      <c r="C63" s="85"/>
+      <c r="B63" s="141"/>
+      <c r="C63" s="109"/>
     </row>
     <row r="64" spans="1:3" ht="13.5" customHeight="1">
       <c r="A64" s="58" t="s">
@@ -8383,11 +8398,11 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A70" s="83" t="s">
+      <c r="A70" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="B70" s="100"/>
-      <c r="C70" s="85"/>
+      <c r="B70" s="108"/>
+      <c r="C70" s="109"/>
     </row>
     <row r="71" spans="1:8" ht="13.5" customHeight="1">
       <c r="A71" s="42" t="s">
@@ -8447,23 +8462,23 @@
       <c r="B77" s="11"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="106" t="s">
+      <c r="A78" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="B78" s="137"/>
-      <c r="C78" s="137"/>
-      <c r="D78" s="137"/>
-      <c r="E78" s="94"/>
+      <c r="B78" s="93"/>
+      <c r="C78" s="93"/>
+      <c r="D78" s="93"/>
+      <c r="E78" s="83"/>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A79" s="108" t="s">
+      <c r="A79" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B79" s="82"/>
-      <c r="C79" s="108" t="s">
+      <c r="B79" s="127"/>
+      <c r="C79" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="D79" s="82"/>
+      <c r="D79" s="127"/>
       <c r="E79" s="43" t="s">
         <v>4</v>
       </c>
@@ -8493,68 +8508,68 @@
       </c>
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A82" s="112" t="s">
+      <c r="A82" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="B82" s="113"/>
-      <c r="C82" s="138"/>
-      <c r="D82" s="139"/>
+      <c r="B82" s="119"/>
+      <c r="C82" s="88"/>
+      <c r="D82" s="89"/>
       <c r="E82" s="44">
         <f>C75</f>
         <v>1559</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C83" s="86" t="s">
+      <c r="C83" s="142" t="s">
         <v>41</v>
       </c>
-      <c r="D83" s="137"/>
+      <c r="D83" s="93"/>
       <c r="E83" s="37">
         <f>(C6+E13)-SUM(E80:E82)</f>
-        <v>515.59999999999945</v>
+        <v>396.19999999999982</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="106" t="s">
+      <c r="A85" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="B85" s="137"/>
-      <c r="C85" s="137"/>
-      <c r="D85" s="137"/>
-      <c r="E85" s="94"/>
+      <c r="B85" s="93"/>
+      <c r="C85" s="93"/>
+      <c r="D85" s="93"/>
+      <c r="E85" s="83"/>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="106" t="s">
+      <c r="A86" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B86" s="94"/>
-      <c r="C86" s="106" t="s">
+      <c r="B86" s="83"/>
+      <c r="C86" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D86" s="94"/>
+      <c r="D86" s="83"/>
       <c r="E86" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="95" t="s">
+      <c r="A87" s="103" t="s">
         <v>81</v>
       </c>
-      <c r="B87" s="96"/>
-      <c r="C87" s="104"/>
+      <c r="B87" s="104"/>
+      <c r="C87" s="113"/>
       <c r="D87" s="145"/>
       <c r="E87" s="37">
         <f>E83</f>
-        <v>515.59999999999945</v>
+        <v>396.19999999999982</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A88" s="114" t="s">
+      <c r="A88" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="B88" s="115"/>
-      <c r="C88" s="104" t="s">
+      <c r="B88" s="97"/>
+      <c r="C88" s="113" t="s">
         <v>83</v>
       </c>
       <c r="D88" s="144"/>
@@ -8563,47 +8578,47 @@
       </c>
     </row>
     <row r="89" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A89" s="142"/>
-      <c r="B89" s="143"/>
-      <c r="C89" s="91" t="s">
+      <c r="A89" s="98"/>
+      <c r="B89" s="99"/>
+      <c r="C89" s="80" t="s">
         <v>164</v>
       </c>
-      <c r="D89" s="92"/>
+      <c r="D89" s="84"/>
       <c r="E89" s="52">
         <v>800</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A90" s="116"/>
-      <c r="B90" s="117"/>
-      <c r="C90" s="91" t="s">
+      <c r="A90" s="100"/>
+      <c r="B90" s="101"/>
+      <c r="C90" s="80" t="s">
         <v>163</v>
       </c>
-      <c r="D90" s="92"/>
+      <c r="D90" s="84"/>
       <c r="E90" s="52">
         <v>187</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="95" t="s">
+      <c r="A91" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B91" s="96"/>
-      <c r="C91" s="101"/>
-      <c r="D91" s="94"/>
+      <c r="B91" s="104"/>
+      <c r="C91" s="110"/>
+      <c r="D91" s="83"/>
       <c r="E91" s="66">
         <f>C75</f>
         <v>1559</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C92" s="93" t="s">
+      <c r="C92" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="D92" s="94"/>
+      <c r="D92" s="83"/>
       <c r="E92" s="37">
         <f>(E18+E87)-SUM(E88:E91)</f>
-        <v>374.59999999999945</v>
+        <v>255.19999999999982</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
@@ -8621,94 +8636,94 @@
       <c r="E94" s="24"/>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="97" t="s">
+      <c r="A95" s="105" t="s">
         <v>101</v>
       </c>
-      <c r="B95" s="98"/>
-      <c r="C95" s="98"/>
-      <c r="D95" s="98"/>
-      <c r="E95" s="99"/>
+      <c r="B95" s="106"/>
+      <c r="C95" s="106"/>
+      <c r="D95" s="106"/>
+      <c r="E95" s="92"/>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A96" s="106" t="s">
+      <c r="A96" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B96" s="94"/>
-      <c r="C96" s="106" t="s">
+      <c r="B96" s="83"/>
+      <c r="C96" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D96" s="94"/>
+      <c r="D96" s="83"/>
       <c r="E96" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A97" s="95" t="s">
+      <c r="A97" s="103" t="s">
         <v>102</v>
       </c>
-      <c r="B97" s="96"/>
-      <c r="C97" s="101"/>
-      <c r="D97" s="94"/>
+      <c r="B97" s="104"/>
+      <c r="C97" s="110"/>
+      <c r="D97" s="83"/>
       <c r="E97" s="37">
         <f>E92</f>
-        <v>374.59999999999945</v>
+        <v>255.19999999999982</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A98" s="114" t="s">
+      <c r="A98" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="B98" s="115"/>
-      <c r="C98" s="91" t="s">
+      <c r="B98" s="97"/>
+      <c r="C98" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="D98" s="107"/>
+      <c r="D98" s="115"/>
       <c r="E98" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A99" s="142"/>
-      <c r="B99" s="143"/>
-      <c r="C99" s="91" t="s">
+      <c r="A99" s="98"/>
+      <c r="B99" s="99"/>
+      <c r="C99" s="80" t="s">
         <v>168</v>
       </c>
-      <c r="D99" s="92"/>
+      <c r="D99" s="84"/>
       <c r="E99" s="52">
         <v>88</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A100" s="116"/>
-      <c r="B100" s="117"/>
-      <c r="C100" s="91" t="s">
+      <c r="A100" s="100"/>
+      <c r="B100" s="101"/>
+      <c r="C100" s="80" t="s">
         <v>164</v>
       </c>
-      <c r="D100" s="92"/>
+      <c r="D100" s="84"/>
       <c r="E100" s="52">
         <v>800</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A101" s="95" t="s">
+      <c r="A101" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B101" s="96"/>
-      <c r="C101" s="101"/>
-      <c r="D101" s="94"/>
+      <c r="B101" s="104"/>
+      <c r="C101" s="110"/>
+      <c r="D101" s="83"/>
       <c r="E101" s="66">
         <f>C75</f>
         <v>1559</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C102" s="93" t="s">
+      <c r="C102" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="D102" s="94"/>
+      <c r="D102" s="83"/>
       <c r="E102" s="52">
         <f>(E24+E97)-SUM(E98:E101)</f>
-        <v>536.59999999999945</v>
+        <v>417.19999999999982</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="13.5" customHeight="1">
@@ -12378,6 +12393,7 @@
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="A63:C63"/>
     <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A78:E78"/>
     <mergeCell ref="C102:D102"/>
     <mergeCell ref="C98:D98"/>
     <mergeCell ref="A91:B91"/>
@@ -12406,7 +12422,8 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="A29:C29"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="A82:B82"/>
     <mergeCell ref="C88:D88"/>
     <mergeCell ref="C83:D83"/>
     <mergeCell ref="A85:E85"/>
@@ -12417,56 +12434,54 @@
     <mergeCell ref="A88:B90"/>
     <mergeCell ref="C89:D89"/>
     <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="A82:B82"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="59" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="60" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C7">
-    <cfRule type="cellIs" dxfId="58" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="C5:C7">
+    <cfRule type="cellIs" dxfId="59" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83">
-    <cfRule type="cellIs" dxfId="57" priority="12" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="58" priority="12" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="cellIs" dxfId="55" priority="8" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="56" priority="8" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="cellIs" dxfId="53" priority="10" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="54" priority="10" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="53" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="cellIs" dxfId="51" priority="6" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="52" priority="6" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="51" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E102">
-    <cfRule type="cellIs" dxfId="49" priority="4" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="50" priority="4" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12479,8 +12494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1EAFDB-34A9-4E8B-8792-A6B6BA3CC3A2}">
   <dimension ref="A1:Y1009"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -12497,13 +12512,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="120"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="122"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -12525,7 +12540,7 @@
       </c>
       <c r="C3" s="5">
         <f>'July 2024 - September 2024'!E102</f>
-        <v>536.59999999999945</v>
+        <v>417.19999999999982</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -12586,9 +12601,9 @@
       <c r="B5" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="57">
         <f>'July 2024 - September 2024'!C5</f>
-        <v>26.2</v>
+        <v>-22.9</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -12620,7 +12635,7 @@
       </c>
       <c r="C6" s="5">
         <f>SUM(C3:C5)</f>
-        <v>562.7999999999995</v>
+        <v>394.29999999999984</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -12706,13 +12721,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="122" t="s">
+      <c r="A10" s="124" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="98"/>
-      <c r="C10" s="98"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="99"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="92"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -12740,10 +12755,10 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="123" t="s">
+      <c r="C11" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="94"/>
+      <c r="D11" s="83"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
@@ -12755,10 +12770,10 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="121" t="s">
+      <c r="C12" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="96"/>
+      <c r="D12" s="104"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -12780,13 +12795,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="122" t="s">
+      <c r="A15" s="124" t="s">
         <v>112</v>
       </c>
-      <c r="B15" s="98"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="99"/>
+      <c r="B15" s="106"/>
+      <c r="C15" s="106"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="92"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -12814,10 +12829,10 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="123" t="s">
+      <c r="C16" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="94"/>
+      <c r="D16" s="83"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
@@ -12829,10 +12844,10 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="121" t="s">
+      <c r="C17" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="94"/>
+      <c r="D17" s="83"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -12857,13 +12872,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="122" t="s">
+      <c r="A20" s="124" t="s">
         <v>108</v>
       </c>
-      <c r="B20" s="98"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="99"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="92"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -12891,10 +12906,10 @@
       <c r="B21" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="124" t="s">
+      <c r="C21" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="82"/>
+      <c r="D21" s="127"/>
       <c r="E21" s="73" t="s">
         <v>4</v>
       </c>
@@ -12906,10 +12921,10 @@
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="126"/>
+      <c r="D22" s="129"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -12955,8 +12970,8 @@
       <c r="A28" s="146" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="137"/>
-      <c r="C28" s="94"/>
+      <c r="B28" s="93"/>
+      <c r="C28" s="83"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="20" t="s">
@@ -12971,11 +12986,11 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="88" t="s">
+      <c r="A30" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="137"/>
-      <c r="C30" s="94"/>
+      <c r="B30" s="93"/>
+      <c r="C30" s="83"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="25" t="s">
@@ -13017,16 +13032,16 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="130" t="s">
+      <c r="A35" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="131"/>
-      <c r="C35" s="132"/>
+      <c r="B35" s="133"/>
+      <c r="C35" s="134"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="133"/>
-      <c r="B36" s="134"/>
-      <c r="C36" s="135"/>
+      <c r="A36" s="135"/>
+      <c r="B36" s="91"/>
+      <c r="C36" s="136"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -13075,11 +13090,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A42" s="88" t="s">
+      <c r="A42" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="137"/>
-      <c r="C42" s="94"/>
+      <c r="B42" s="93"/>
+      <c r="C42" s="83"/>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
@@ -13114,11 +13129,11 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A46" s="88" t="s">
+      <c r="A46" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="89"/>
-      <c r="C46" s="90"/>
+      <c r="B46" s="86"/>
+      <c r="C46" s="87"/>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -13160,11 +13175,11 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="88" t="s">
+      <c r="A51" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="89"/>
-      <c r="C51" s="90"/>
+      <c r="B51" s="86"/>
+      <c r="C51" s="87"/>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="2" t="s">
@@ -13188,11 +13203,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="80" t="s">
+      <c r="A54" s="139" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="81"/>
-      <c r="C54" s="82"/>
+      <c r="B54" s="140"/>
+      <c r="C54" s="127"/>
     </row>
     <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="32" t="s">
@@ -13216,11 +13231,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="141" t="s">
+      <c r="A57" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="134"/>
-      <c r="C57" s="99"/>
+      <c r="B57" s="91"/>
+      <c r="C57" s="92"/>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
       <c r="A58" s="26" t="s">
@@ -13264,11 +13279,11 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A62" s="83" t="s">
+      <c r="A62" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="84"/>
-      <c r="C62" s="85"/>
+      <c r="B62" s="141"/>
+      <c r="C62" s="109"/>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
       <c r="A63" s="58" t="s">
@@ -13335,11 +13350,11 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A69" s="83" t="s">
+      <c r="A69" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="100"/>
-      <c r="C69" s="85"/>
+      <c r="B69" s="108"/>
+      <c r="C69" s="109"/>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
       <c r="A70" s="42" t="s">
@@ -13399,23 +13414,23 @@
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="106" t="s">
+      <c r="A77" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="B77" s="137"/>
-      <c r="C77" s="137"/>
-      <c r="D77" s="137"/>
-      <c r="E77" s="94"/>
+      <c r="B77" s="93"/>
+      <c r="C77" s="93"/>
+      <c r="D77" s="93"/>
+      <c r="E77" s="83"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="108" t="s">
+      <c r="A78" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B78" s="82"/>
-      <c r="C78" s="108" t="s">
+      <c r="B78" s="127"/>
+      <c r="C78" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="82"/>
+      <c r="D78" s="127"/>
       <c r="E78" s="43" t="s">
         <v>4</v>
       </c>
@@ -13424,7 +13439,7 @@
       <c r="A79" s="151" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="115"/>
+      <c r="B79" s="97"/>
       <c r="C79" s="149" t="s">
         <v>173</v>
       </c>
@@ -13434,68 +13449,68 @@
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="112" t="s">
+      <c r="A80" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="113"/>
-      <c r="C80" s="138"/>
-      <c r="D80" s="139"/>
+      <c r="B80" s="119"/>
+      <c r="C80" s="88"/>
+      <c r="D80" s="89"/>
       <c r="E80" s="44">
         <f>C74</f>
         <v>1443</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C81" s="86" t="s">
+      <c r="C81" s="142" t="s">
         <v>41</v>
       </c>
-      <c r="D81" s="137"/>
+      <c r="D81" s="93"/>
       <c r="E81" s="37">
         <f>(C6+E13)-SUM(E79:E80)</f>
-        <v>424.79999999999927</v>
+        <v>256.29999999999973</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="106" t="s">
+      <c r="A83" s="82" t="s">
         <v>114</v>
       </c>
-      <c r="B83" s="137"/>
-      <c r="C83" s="137"/>
-      <c r="D83" s="137"/>
-      <c r="E83" s="94"/>
+      <c r="B83" s="93"/>
+      <c r="C83" s="93"/>
+      <c r="D83" s="93"/>
+      <c r="E83" s="83"/>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="106" t="s">
+      <c r="A84" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="94"/>
-      <c r="C84" s="106" t="s">
+      <c r="B84" s="83"/>
+      <c r="C84" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="94"/>
+      <c r="D84" s="83"/>
       <c r="E84" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="95" t="s">
+      <c r="A85" s="103" t="s">
         <v>106</v>
       </c>
-      <c r="B85" s="96"/>
-      <c r="C85" s="104"/>
+      <c r="B85" s="104"/>
+      <c r="C85" s="113"/>
       <c r="D85" s="145"/>
       <c r="E85" s="37">
         <f>E81</f>
-        <v>424.79999999999927</v>
+        <v>256.29999999999973</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="95" t="s">
+      <c r="A86" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="B86" s="103"/>
-      <c r="C86" s="91" t="s">
+      <c r="B86" s="112"/>
+      <c r="C86" s="80" t="s">
         <v>170</v>
       </c>
       <c r="D86" s="144"/>
@@ -13504,25 +13519,25 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="95" t="s">
+      <c r="A87" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="96"/>
-      <c r="C87" s="101"/>
-      <c r="D87" s="94"/>
+      <c r="B87" s="104"/>
+      <c r="C87" s="110"/>
+      <c r="D87" s="83"/>
       <c r="E87" s="66">
         <f>C74</f>
         <v>1443</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C88" s="93" t="s">
+      <c r="C88" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="94"/>
+      <c r="D88" s="83"/>
       <c r="E88" s="37">
         <f>(E18+E85)-SUM(E86:E87)</f>
-        <v>486.79999999999927</v>
+        <v>318.29999999999973</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="13.5" customHeight="1">
@@ -13540,72 +13555,72 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="97" t="s">
+      <c r="A91" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="B91" s="98"/>
-      <c r="C91" s="98"/>
-      <c r="D91" s="98"/>
-      <c r="E91" s="99"/>
+      <c r="B91" s="106"/>
+      <c r="C91" s="106"/>
+      <c r="D91" s="106"/>
+      <c r="E91" s="92"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="106" t="s">
+      <c r="A92" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B92" s="94"/>
-      <c r="C92" s="106" t="s">
+      <c r="B92" s="83"/>
+      <c r="C92" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D92" s="94"/>
+      <c r="D92" s="83"/>
       <c r="E92" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="95" t="s">
+      <c r="A93" s="103" t="s">
         <v>115</v>
       </c>
-      <c r="B93" s="96"/>
-      <c r="C93" s="101"/>
-      <c r="D93" s="94"/>
+      <c r="B93" s="104"/>
+      <c r="C93" s="110"/>
+      <c r="D93" s="83"/>
       <c r="E93" s="37">
         <f>E88</f>
-        <v>486.79999999999927</v>
+        <v>318.29999999999973</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="95" t="s">
+      <c r="A94" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="103"/>
-      <c r="C94" s="91" t="s">
+      <c r="B94" s="112"/>
+      <c r="C94" s="80" t="s">
         <v>170</v>
       </c>
-      <c r="D94" s="107"/>
+      <c r="D94" s="115"/>
       <c r="E94" s="52">
         <v>900</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="95" t="s">
+      <c r="A95" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B95" s="96"/>
-      <c r="C95" s="101"/>
-      <c r="D95" s="94"/>
+      <c r="B95" s="104"/>
+      <c r="C95" s="110"/>
+      <c r="D95" s="83"/>
       <c r="E95" s="66">
         <f>C74</f>
         <v>1443</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C96" s="93" t="s">
+      <c r="C96" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="D96" s="94"/>
+      <c r="D96" s="83"/>
       <c r="E96" s="52">
         <f>(E23+E93)-SUM(E94:E95)</f>
-        <v>548.79999999999927</v>
+        <v>380.29999999999973</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="13.5" customHeight="1">
@@ -17312,52 +17327,52 @@
     <mergeCell ref="A15:E15"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="47" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C7">
-    <cfRule type="cellIs" dxfId="46" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="C5:C7">
+    <cfRule type="cellIs" dxfId="47" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="cellIs" dxfId="45" priority="11" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="46" priority="11" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="cellIs" dxfId="43" priority="7" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="44" priority="7" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88">
-    <cfRule type="cellIs" dxfId="41" priority="9" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="42" priority="9" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="cellIs" dxfId="39" priority="5" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="40" priority="5" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E96">
-    <cfRule type="cellIs" dxfId="37" priority="3" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="38" priority="3" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17369,8 +17384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5AAEA1-C3EE-4B36-938E-0F583AF15471}">
   <dimension ref="A1:Y1009"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -17387,13 +17402,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="120"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="122"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -17415,7 +17430,7 @@
       </c>
       <c r="C3" s="5">
         <f>'October 2024 - December 2024'!E96</f>
-        <v>548.79999999999927</v>
+        <v>380.29999999999973</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -17476,9 +17491,9 @@
       <c r="B5" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="57">
         <f>'October 2024 - December 2024'!C5</f>
-        <v>26.2</v>
+        <v>-22.9</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -17510,7 +17525,7 @@
       </c>
       <c r="C6" s="5">
         <f>SUM(C3:C5)</f>
-        <v>574.99999999999932</v>
+        <v>357.39999999999975</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -17596,13 +17611,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="122" t="s">
+      <c r="A10" s="124" t="s">
         <v>120</v>
       </c>
-      <c r="B10" s="98"/>
-      <c r="C10" s="98"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="99"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="92"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -17630,10 +17645,10 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="123" t="s">
+      <c r="C11" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="94"/>
+      <c r="D11" s="83"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
@@ -17645,10 +17660,10 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="121" t="s">
+      <c r="C12" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="96"/>
+      <c r="D12" s="104"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -17670,13 +17685,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="122" t="s">
+      <c r="A15" s="124" t="s">
         <v>127</v>
       </c>
-      <c r="B15" s="98"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="99"/>
+      <c r="B15" s="106"/>
+      <c r="C15" s="106"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="92"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -17704,10 +17719,10 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="123" t="s">
+      <c r="C16" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="94"/>
+      <c r="D16" s="83"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
@@ -17719,10 +17734,10 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="121" t="s">
+      <c r="C17" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="94"/>
+      <c r="D17" s="83"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -17747,13 +17762,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="122" t="s">
+      <c r="A20" s="124" t="s">
         <v>122</v>
       </c>
-      <c r="B20" s="98"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="99"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="92"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -17781,10 +17796,10 @@
       <c r="B21" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="124" t="s">
+      <c r="C21" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="82"/>
+      <c r="D21" s="127"/>
       <c r="E21" s="73" t="s">
         <v>4</v>
       </c>
@@ -17796,10 +17811,10 @@
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="126"/>
+      <c r="D22" s="129"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -17845,8 +17860,8 @@
       <c r="A28" s="146" t="s">
         <v>124</v>
       </c>
-      <c r="B28" s="137"/>
-      <c r="C28" s="94"/>
+      <c r="B28" s="93"/>
+      <c r="C28" s="83"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="20" t="s">
@@ -17861,11 +17876,11 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="88" t="s">
+      <c r="A30" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="137"/>
-      <c r="C30" s="94"/>
+      <c r="B30" s="93"/>
+      <c r="C30" s="83"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="25" t="s">
@@ -17907,16 +17922,16 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="130" t="s">
+      <c r="A35" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="131"/>
-      <c r="C35" s="132"/>
+      <c r="B35" s="133"/>
+      <c r="C35" s="134"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="133"/>
-      <c r="B36" s="134"/>
-      <c r="C36" s="135"/>
+      <c r="A36" s="135"/>
+      <c r="B36" s="91"/>
+      <c r="C36" s="136"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -17965,11 +17980,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A42" s="88" t="s">
+      <c r="A42" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="137"/>
-      <c r="C42" s="94"/>
+      <c r="B42" s="93"/>
+      <c r="C42" s="83"/>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
@@ -18004,11 +18019,11 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A46" s="88" t="s">
+      <c r="A46" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="89"/>
-      <c r="C46" s="90"/>
+      <c r="B46" s="86"/>
+      <c r="C46" s="87"/>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -18050,11 +18065,11 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="88" t="s">
+      <c r="A51" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="89"/>
-      <c r="C51" s="90"/>
+      <c r="B51" s="86"/>
+      <c r="C51" s="87"/>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="2" t="s">
@@ -18078,11 +18093,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="80" t="s">
+      <c r="A54" s="139" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="81"/>
-      <c r="C54" s="82"/>
+      <c r="B54" s="140"/>
+      <c r="C54" s="127"/>
     </row>
     <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="32" t="s">
@@ -18106,11 +18121,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="141" t="s">
+      <c r="A57" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="134"/>
-      <c r="C57" s="99"/>
+      <c r="B57" s="91"/>
+      <c r="C57" s="92"/>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
       <c r="A58" s="26" t="s">
@@ -18154,11 +18169,11 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A62" s="83" t="s">
+      <c r="A62" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="84"/>
-      <c r="C62" s="85"/>
+      <c r="B62" s="141"/>
+      <c r="C62" s="109"/>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
       <c r="A63" s="58" t="s">
@@ -18225,11 +18240,11 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A69" s="83" t="s">
+      <c r="A69" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="100"/>
-      <c r="C69" s="85"/>
+      <c r="B69" s="108"/>
+      <c r="C69" s="109"/>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
       <c r="A70" s="42" t="s">
@@ -18289,23 +18304,23 @@
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="106" t="s">
+      <c r="A77" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="B77" s="137"/>
-      <c r="C77" s="137"/>
-      <c r="D77" s="137"/>
-      <c r="E77" s="94"/>
+      <c r="B77" s="93"/>
+      <c r="C77" s="93"/>
+      <c r="D77" s="93"/>
+      <c r="E77" s="83"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="108" t="s">
+      <c r="A78" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B78" s="82"/>
-      <c r="C78" s="108" t="s">
+      <c r="B78" s="127"/>
+      <c r="C78" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="82"/>
+      <c r="D78" s="127"/>
       <c r="E78" s="43" t="s">
         <v>4</v>
       </c>
@@ -18314,7 +18329,7 @@
       <c r="A79" s="151" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="115"/>
+      <c r="B79" s="97"/>
       <c r="C79" s="149" t="s">
         <v>170</v>
       </c>
@@ -18324,68 +18339,68 @@
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="112" t="s">
+      <c r="A80" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="113"/>
-      <c r="C80" s="138"/>
-      <c r="D80" s="139"/>
+      <c r="B80" s="119"/>
+      <c r="C80" s="88"/>
+      <c r="D80" s="89"/>
       <c r="E80" s="44">
         <f>C74</f>
         <v>1443</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C81" s="86" t="s">
+      <c r="C81" s="142" t="s">
         <v>41</v>
       </c>
-      <c r="D81" s="137"/>
+      <c r="D81" s="93"/>
       <c r="E81" s="37">
         <f>(C6+E13)-SUM(E79:E80)</f>
-        <v>636.99999999999909</v>
+        <v>419.39999999999964</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="106" t="s">
+      <c r="A83" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="B83" s="137"/>
-      <c r="C83" s="137"/>
-      <c r="D83" s="137"/>
-      <c r="E83" s="94"/>
+      <c r="B83" s="93"/>
+      <c r="C83" s="93"/>
+      <c r="D83" s="93"/>
+      <c r="E83" s="83"/>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="106" t="s">
+      <c r="A84" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="94"/>
-      <c r="C84" s="106" t="s">
+      <c r="B84" s="83"/>
+      <c r="C84" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="94"/>
+      <c r="D84" s="83"/>
       <c r="E84" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="95" t="s">
+      <c r="A85" s="103" t="s">
         <v>143</v>
       </c>
-      <c r="B85" s="96"/>
-      <c r="C85" s="104"/>
+      <c r="B85" s="104"/>
+      <c r="C85" s="113"/>
       <c r="D85" s="145"/>
       <c r="E85" s="37">
         <f>E81</f>
-        <v>636.99999999999909</v>
+        <v>419.39999999999964</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="95" t="s">
+      <c r="A86" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="B86" s="103"/>
-      <c r="C86" s="91" t="s">
+      <c r="B86" s="112"/>
+      <c r="C86" s="80" t="s">
         <v>170</v>
       </c>
       <c r="D86" s="144"/>
@@ -18394,25 +18409,25 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="95" t="s">
+      <c r="A87" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="96"/>
-      <c r="C87" s="101"/>
-      <c r="D87" s="94"/>
+      <c r="B87" s="104"/>
+      <c r="C87" s="110"/>
+      <c r="D87" s="83"/>
       <c r="E87" s="66">
         <f>C74</f>
         <v>1443</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C88" s="93" t="s">
+      <c r="C88" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="94"/>
+      <c r="D88" s="83"/>
       <c r="E88" s="37">
         <f>(E18+E85)-SUM(E86:E87)</f>
-        <v>698.99999999999909</v>
+        <v>481.39999999999964</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="13.5" customHeight="1">
@@ -18430,72 +18445,72 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="97" t="s">
+      <c r="A91" s="105" t="s">
         <v>126</v>
       </c>
-      <c r="B91" s="98"/>
-      <c r="C91" s="98"/>
-      <c r="D91" s="98"/>
-      <c r="E91" s="99"/>
+      <c r="B91" s="106"/>
+      <c r="C91" s="106"/>
+      <c r="D91" s="106"/>
+      <c r="E91" s="92"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="106" t="s">
+      <c r="A92" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B92" s="94"/>
-      <c r="C92" s="106" t="s">
+      <c r="B92" s="83"/>
+      <c r="C92" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D92" s="94"/>
+      <c r="D92" s="83"/>
       <c r="E92" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="95" t="s">
+      <c r="A93" s="103" t="s">
         <v>144</v>
       </c>
-      <c r="B93" s="96"/>
-      <c r="C93" s="101"/>
-      <c r="D93" s="94"/>
+      <c r="B93" s="104"/>
+      <c r="C93" s="110"/>
+      <c r="D93" s="83"/>
       <c r="E93" s="37">
         <f>E88</f>
-        <v>698.99999999999909</v>
+        <v>481.39999999999964</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="95" t="s">
+      <c r="A94" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="103"/>
-      <c r="C94" s="91" t="s">
+      <c r="B94" s="112"/>
+      <c r="C94" s="80" t="s">
         <v>170</v>
       </c>
-      <c r="D94" s="107"/>
+      <c r="D94" s="115"/>
       <c r="E94" s="52">
         <v>900</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="95" t="s">
+      <c r="A95" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B95" s="96"/>
-      <c r="C95" s="101"/>
-      <c r="D95" s="94"/>
+      <c r="B95" s="104"/>
+      <c r="C95" s="110"/>
+      <c r="D95" s="83"/>
       <c r="E95" s="66">
         <f>C74</f>
         <v>1443</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C96" s="93" t="s">
+      <c r="C96" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="D96" s="94"/>
+      <c r="D96" s="83"/>
       <c r="E96" s="52">
         <f>(E23+E93)-SUM(E94:E95)</f>
-        <v>760.99999999999909</v>
+        <v>543.39999999999964</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="13.5" customHeight="1">
@@ -22202,52 +22217,52 @@
     <mergeCell ref="C96:D96"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="35" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C7">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="C5:C7">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="cellIs" dxfId="33" priority="11" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="11" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="cellIs" dxfId="31" priority="7" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="7" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88">
-    <cfRule type="cellIs" dxfId="29" priority="9" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="9" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="cellIs" dxfId="27" priority="5" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="5" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E96">
-    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="3" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22259,8 +22274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A0D0F5D-D1BD-4315-A79D-5F8D7D39DF80}">
   <dimension ref="A1:Y1009"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -22277,13 +22292,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="120"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="122"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -22305,7 +22320,7 @@
       </c>
       <c r="C3" s="5">
         <f>'January 2025 - March 2025'!E96</f>
-        <v>760.99999999999909</v>
+        <v>543.39999999999964</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -22366,9 +22381,9 @@
       <c r="B5" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="57">
         <f>'January 2025 - March 2025'!C5</f>
-        <v>26.2</v>
+        <v>-22.9</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -22400,7 +22415,7 @@
       </c>
       <c r="C6" s="5">
         <f>SUM(C3:C5)</f>
-        <v>787.19999999999914</v>
+        <v>520.49999999999966</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -22486,13 +22501,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="122" t="s">
+      <c r="A10" s="124" t="s">
         <v>130</v>
       </c>
-      <c r="B10" s="98"/>
-      <c r="C10" s="98"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="99"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="92"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -22520,10 +22535,10 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="123" t="s">
+      <c r="C11" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="94"/>
+      <c r="D11" s="83"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
@@ -22535,10 +22550,10 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="121" t="s">
+      <c r="C12" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="96"/>
+      <c r="D12" s="104"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -22560,13 +22575,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="122" t="s">
+      <c r="A15" s="124" t="s">
         <v>138</v>
       </c>
-      <c r="B15" s="98"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="99"/>
+      <c r="B15" s="106"/>
+      <c r="C15" s="106"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="92"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -22594,10 +22609,10 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="123" t="s">
+      <c r="C16" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="94"/>
+      <c r="D16" s="83"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
@@ -22609,10 +22624,10 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="121" t="s">
+      <c r="C17" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="94"/>
+      <c r="D17" s="83"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -22637,13 +22652,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="122" t="s">
+      <c r="A20" s="124" t="s">
         <v>134</v>
       </c>
-      <c r="B20" s="98"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="99"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="92"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -22671,10 +22686,10 @@
       <c r="B21" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="124" t="s">
+      <c r="C21" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="82"/>
+      <c r="D21" s="127"/>
       <c r="E21" s="73" t="s">
         <v>4</v>
       </c>
@@ -22686,10 +22701,10 @@
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="126"/>
+      <c r="D22" s="129"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -22735,8 +22750,8 @@
       <c r="A28" s="146" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="137"/>
-      <c r="C28" s="94"/>
+      <c r="B28" s="93"/>
+      <c r="C28" s="83"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="20" t="s">
@@ -22751,11 +22766,11 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="88" t="s">
+      <c r="A30" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="137"/>
-      <c r="C30" s="94"/>
+      <c r="B30" s="93"/>
+      <c r="C30" s="83"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="25" t="s">
@@ -22797,16 +22812,16 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="130" t="s">
+      <c r="A35" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="131"/>
-      <c r="C35" s="132"/>
+      <c r="B35" s="133"/>
+      <c r="C35" s="134"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="133"/>
-      <c r="B36" s="134"/>
-      <c r="C36" s="135"/>
+      <c r="A36" s="135"/>
+      <c r="B36" s="91"/>
+      <c r="C36" s="136"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -22855,11 +22870,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A42" s="88" t="s">
+      <c r="A42" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="137"/>
-      <c r="C42" s="94"/>
+      <c r="B42" s="93"/>
+      <c r="C42" s="83"/>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
@@ -22894,11 +22909,11 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A46" s="88" t="s">
+      <c r="A46" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="89"/>
-      <c r="C46" s="90"/>
+      <c r="B46" s="86"/>
+      <c r="C46" s="87"/>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -22940,11 +22955,11 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="88" t="s">
+      <c r="A51" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="89"/>
-      <c r="C51" s="90"/>
+      <c r="B51" s="86"/>
+      <c r="C51" s="87"/>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="2" t="s">
@@ -22968,11 +22983,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="80" t="s">
+      <c r="A54" s="139" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="81"/>
-      <c r="C54" s="82"/>
+      <c r="B54" s="140"/>
+      <c r="C54" s="127"/>
     </row>
     <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="32" t="s">
@@ -22996,11 +23011,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="141" t="s">
+      <c r="A57" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="134"/>
-      <c r="C57" s="99"/>
+      <c r="B57" s="91"/>
+      <c r="C57" s="92"/>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
       <c r="A58" s="26" t="s">
@@ -23044,11 +23059,11 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A62" s="83" t="s">
+      <c r="A62" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="84"/>
-      <c r="C62" s="85"/>
+      <c r="B62" s="141"/>
+      <c r="C62" s="109"/>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
       <c r="A63" s="58" t="s">
@@ -23115,11 +23130,11 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A69" s="83" t="s">
+      <c r="A69" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="100"/>
-      <c r="C69" s="85"/>
+      <c r="B69" s="108"/>
+      <c r="C69" s="109"/>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
       <c r="A70" s="42" t="s">
@@ -23179,23 +23194,23 @@
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="106" t="s">
+      <c r="A77" s="82" t="s">
         <v>132</v>
       </c>
-      <c r="B77" s="137"/>
-      <c r="C77" s="137"/>
-      <c r="D77" s="137"/>
-      <c r="E77" s="94"/>
+      <c r="B77" s="93"/>
+      <c r="C77" s="93"/>
+      <c r="D77" s="93"/>
+      <c r="E77" s="83"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="108" t="s">
+      <c r="A78" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B78" s="82"/>
-      <c r="C78" s="108" t="s">
+      <c r="B78" s="127"/>
+      <c r="C78" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="82"/>
+      <c r="D78" s="127"/>
       <c r="E78" s="43" t="s">
         <v>4</v>
       </c>
@@ -23204,7 +23219,7 @@
       <c r="A79" s="151" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="115"/>
+      <c r="B79" s="97"/>
       <c r="C79" s="149" t="s">
         <v>170</v>
       </c>
@@ -23214,68 +23229,68 @@
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A80" s="112" t="s">
+      <c r="A80" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="113"/>
-      <c r="C80" s="138"/>
-      <c r="D80" s="139"/>
+      <c r="B80" s="119"/>
+      <c r="C80" s="88"/>
+      <c r="D80" s="89"/>
       <c r="E80" s="44">
         <f>C74</f>
         <v>1443</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C81" s="86" t="s">
+      <c r="C81" s="142" t="s">
         <v>41</v>
       </c>
-      <c r="D81" s="137"/>
+      <c r="D81" s="93"/>
       <c r="E81" s="37">
         <f>(C6+E13)-SUM(E79:E80)</f>
-        <v>849.19999999999891</v>
+        <v>582.49999999999955</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="106" t="s">
+      <c r="A83" s="82" t="s">
         <v>140</v>
       </c>
-      <c r="B83" s="137"/>
-      <c r="C83" s="137"/>
-      <c r="D83" s="137"/>
-      <c r="E83" s="94"/>
+      <c r="B83" s="93"/>
+      <c r="C83" s="93"/>
+      <c r="D83" s="93"/>
+      <c r="E83" s="83"/>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="106" t="s">
+      <c r="A84" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="94"/>
-      <c r="C84" s="106" t="s">
+      <c r="B84" s="83"/>
+      <c r="C84" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="94"/>
+      <c r="D84" s="83"/>
       <c r="E84" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="95" t="s">
+      <c r="A85" s="103" t="s">
         <v>141</v>
       </c>
-      <c r="B85" s="96"/>
-      <c r="C85" s="104"/>
+      <c r="B85" s="104"/>
+      <c r="C85" s="113"/>
       <c r="D85" s="145"/>
       <c r="E85" s="37">
         <f>E81</f>
-        <v>849.19999999999891</v>
+        <v>582.49999999999955</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="95" t="s">
+      <c r="A86" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="B86" s="103"/>
-      <c r="C86" s="91" t="s">
+      <c r="B86" s="112"/>
+      <c r="C86" s="80" t="s">
         <v>171</v>
       </c>
       <c r="D86" s="144"/>
@@ -23284,25 +23299,25 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="95" t="s">
+      <c r="A87" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="96"/>
-      <c r="C87" s="101"/>
-      <c r="D87" s="94"/>
+      <c r="B87" s="104"/>
+      <c r="C87" s="110"/>
+      <c r="D87" s="83"/>
       <c r="E87" s="66">
         <f>C74</f>
         <v>1443</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C88" s="93" t="s">
+      <c r="C88" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="94"/>
+      <c r="D88" s="83"/>
       <c r="E88" s="37">
         <f>(E18+E85)-SUM(E86:E87)</f>
-        <v>911.19999999999891</v>
+        <v>644.49999999999955</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="13.5" customHeight="1">
@@ -23320,72 +23335,72 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="97" t="s">
+      <c r="A91" s="105" t="s">
         <v>137</v>
       </c>
-      <c r="B91" s="98"/>
-      <c r="C91" s="98"/>
-      <c r="D91" s="98"/>
-      <c r="E91" s="99"/>
+      <c r="B91" s="106"/>
+      <c r="C91" s="106"/>
+      <c r="D91" s="106"/>
+      <c r="E91" s="92"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="106" t="s">
+      <c r="A92" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B92" s="94"/>
-      <c r="C92" s="106" t="s">
+      <c r="B92" s="83"/>
+      <c r="C92" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D92" s="94"/>
+      <c r="D92" s="83"/>
       <c r="E92" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="95" t="s">
+      <c r="A93" s="103" t="s">
         <v>142</v>
       </c>
-      <c r="B93" s="96"/>
-      <c r="C93" s="101"/>
-      <c r="D93" s="94"/>
+      <c r="B93" s="104"/>
+      <c r="C93" s="110"/>
+      <c r="D93" s="83"/>
       <c r="E93" s="37">
         <f>E88</f>
-        <v>911.19999999999891</v>
+        <v>644.49999999999955</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="95" t="s">
+      <c r="A94" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="103"/>
-      <c r="C94" s="91" t="s">
+      <c r="B94" s="112"/>
+      <c r="C94" s="80" t="s">
         <v>170</v>
       </c>
-      <c r="D94" s="107"/>
+      <c r="D94" s="115"/>
       <c r="E94" s="52">
         <v>900</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="95" t="s">
+      <c r="A95" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B95" s="96"/>
-      <c r="C95" s="101"/>
-      <c r="D95" s="94"/>
+      <c r="B95" s="104"/>
+      <c r="C95" s="110"/>
+      <c r="D95" s="83"/>
       <c r="E95" s="66">
         <f>C74</f>
         <v>1443</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C96" s="93" t="s">
+      <c r="C96" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="D96" s="94"/>
+      <c r="D96" s="83"/>
       <c r="E96" s="52">
         <f>(E23+E93)-SUM(E94:E95)</f>
-        <v>973.19999999999891</v>
+        <v>706.49999999999955</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="13.5" customHeight="1">
@@ -27092,52 +27107,52 @@
     <mergeCell ref="C96:D96"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C7">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="C5:C7">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="cellIs" dxfId="21" priority="11" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="11" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="cellIs" dxfId="19" priority="7" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="7" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88">
-    <cfRule type="cellIs" dxfId="17" priority="9" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="9" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="cellIs" dxfId="15" priority="5" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="5" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E96">
-    <cfRule type="cellIs" dxfId="13" priority="3" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27149,8 +27164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DD8682-0711-4837-AA14-B5688B0442EE}">
   <dimension ref="A1:Y1009"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C94" sqref="C94:D94"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -27167,13 +27182,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="120"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="122"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -27195,7 +27210,7 @@
       </c>
       <c r="C3" s="5">
         <f>'April 2025 - June 2025'!E96</f>
-        <v>973.19999999999891</v>
+        <v>706.49999999999955</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -27256,9 +27271,9 @@
       <c r="B5" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="57">
         <f>'April 2025 - June 2025'!C5</f>
-        <v>26.2</v>
+        <v>-22.9</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -27290,7 +27305,7 @@
       </c>
       <c r="C6" s="5">
         <f>SUM(C3:C5)</f>
-        <v>999.39999999999895</v>
+        <v>683.59999999999957</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -27376,13 +27391,13 @@
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1"/>
     <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A10" s="122" t="s">
+      <c r="A10" s="124" t="s">
         <v>145</v>
       </c>
-      <c r="B10" s="98"/>
-      <c r="C10" s="98"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="99"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="92"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -27410,10 +27425,10 @@
       <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="123" t="s">
+      <c r="C11" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="94"/>
+      <c r="D11" s="83"/>
       <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
@@ -27425,10 +27440,10 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="121" t="s">
+      <c r="C12" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="96"/>
+      <c r="D12" s="104"/>
       <c r="E12" s="18">
         <v>2405</v>
       </c>
@@ -27450,13 +27465,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="122" t="s">
+      <c r="A15" s="124" t="s">
         <v>154</v>
       </c>
-      <c r="B15" s="98"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="99"/>
+      <c r="B15" s="106"/>
+      <c r="C15" s="106"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="92"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -27484,10 +27499,10 @@
       <c r="B16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="123" t="s">
+      <c r="C16" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="94"/>
+      <c r="D16" s="83"/>
       <c r="E16" s="17" t="s">
         <v>4</v>
       </c>
@@ -27499,10 +27514,10 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="121" t="s">
+      <c r="C17" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="94"/>
+      <c r="D17" s="83"/>
       <c r="E17" s="19">
         <v>2405</v>
       </c>
@@ -27527,13 +27542,13 @@
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="122" t="s">
+      <c r="A20" s="124" t="s">
         <v>150</v>
       </c>
-      <c r="B20" s="98"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="99"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="92"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -27561,10 +27576,10 @@
       <c r="B21" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="124" t="s">
+      <c r="C21" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="82"/>
+      <c r="D21" s="127"/>
       <c r="E21" s="73" t="s">
         <v>4</v>
       </c>
@@ -27576,10 +27591,10 @@
       <c r="B22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="126"/>
+      <c r="D22" s="129"/>
       <c r="E22" s="67">
         <v>2405</v>
       </c>
@@ -27625,8 +27640,8 @@
       <c r="A28" s="146" t="s">
         <v>152</v>
       </c>
-      <c r="B28" s="137"/>
-      <c r="C28" s="94"/>
+      <c r="B28" s="93"/>
+      <c r="C28" s="83"/>
     </row>
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="20" t="s">
@@ -27641,11 +27656,11 @@
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="88" t="s">
+      <c r="A30" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="137"/>
-      <c r="C30" s="94"/>
+      <c r="B30" s="93"/>
+      <c r="C30" s="83"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="25" t="s">
@@ -27687,16 +27702,16 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="130" t="s">
+      <c r="A35" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="131"/>
-      <c r="C35" s="132"/>
+      <c r="B35" s="133"/>
+      <c r="C35" s="134"/>
     </row>
     <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="133"/>
-      <c r="B36" s="134"/>
-      <c r="C36" s="135"/>
+      <c r="A36" s="135"/>
+      <c r="B36" s="91"/>
+      <c r="C36" s="136"/>
     </row>
     <row r="37" spans="1:3" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -27745,11 +27760,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A42" s="88" t="s">
+      <c r="A42" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="137"/>
-      <c r="C42" s="94"/>
+      <c r="B42" s="93"/>
+      <c r="C42" s="83"/>
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
@@ -27784,11 +27799,11 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A46" s="88" t="s">
+      <c r="A46" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="89"/>
-      <c r="C46" s="90"/>
+      <c r="B46" s="86"/>
+      <c r="C46" s="87"/>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -27830,11 +27845,11 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="88" t="s">
+      <c r="A51" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="89"/>
-      <c r="C51" s="90"/>
+      <c r="B51" s="86"/>
+      <c r="C51" s="87"/>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="2" t="s">
@@ -27858,11 +27873,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="80" t="s">
+      <c r="A54" s="139" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="81"/>
-      <c r="C54" s="82"/>
+      <c r="B54" s="140"/>
+      <c r="C54" s="127"/>
     </row>
     <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="32" t="s">
@@ -27886,11 +27901,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="141" t="s">
+      <c r="A57" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="134"/>
-      <c r="C57" s="99"/>
+      <c r="B57" s="91"/>
+      <c r="C57" s="92"/>
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
       <c r="A58" s="26" t="s">
@@ -27934,11 +27949,11 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A62" s="83" t="s">
+      <c r="A62" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="84"/>
-      <c r="C62" s="85"/>
+      <c r="B62" s="141"/>
+      <c r="C62" s="109"/>
     </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1">
       <c r="A63" s="58" t="s">
@@ -28005,11 +28020,11 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A69" s="83" t="s">
+      <c r="A69" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="100"/>
-      <c r="C69" s="85"/>
+      <c r="B69" s="108"/>
+      <c r="C69" s="109"/>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1">
       <c r="A70" s="42" t="s">
@@ -28068,23 +28083,23 @@
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A77" s="106" t="s">
+      <c r="A77" s="82" t="s">
         <v>147</v>
       </c>
-      <c r="B77" s="137"/>
-      <c r="C77" s="137"/>
-      <c r="D77" s="137"/>
-      <c r="E77" s="94"/>
+      <c r="B77" s="93"/>
+      <c r="C77" s="93"/>
+      <c r="D77" s="93"/>
+      <c r="E77" s="83"/>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A78" s="108" t="s">
+      <c r="A78" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B78" s="82"/>
-      <c r="C78" s="108" t="s">
+      <c r="B78" s="127"/>
+      <c r="C78" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="82"/>
+      <c r="D78" s="127"/>
       <c r="E78" s="43" t="s">
         <v>4</v>
       </c>
@@ -28120,53 +28135,53 @@
       <c r="C81" s="159" t="s">
         <v>41</v>
       </c>
-      <c r="D81" s="134"/>
+      <c r="D81" s="91"/>
       <c r="E81" s="76">
         <f>(C6+E13)-SUM(E79:E80)</f>
-        <v>1061.3999999999987</v>
+        <v>745.59999999999945</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="13.5" customHeight="1"/>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A83" s="106" t="s">
+      <c r="A83" s="82" t="s">
         <v>156</v>
       </c>
-      <c r="B83" s="137"/>
-      <c r="C83" s="137"/>
-      <c r="D83" s="137"/>
-      <c r="E83" s="94"/>
+      <c r="B83" s="93"/>
+      <c r="C83" s="93"/>
+      <c r="D83" s="93"/>
+      <c r="E83" s="83"/>
     </row>
     <row r="84" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A84" s="106" t="s">
+      <c r="A84" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="94"/>
-      <c r="C84" s="106" t="s">
+      <c r="B84" s="83"/>
+      <c r="C84" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="94"/>
+      <c r="D84" s="83"/>
       <c r="E84" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A85" s="95" t="s">
+      <c r="A85" s="103" t="s">
         <v>148</v>
       </c>
-      <c r="B85" s="96"/>
-      <c r="C85" s="104"/>
+      <c r="B85" s="104"/>
+      <c r="C85" s="113"/>
       <c r="D85" s="145"/>
       <c r="E85" s="37">
         <f>E81</f>
-        <v>1061.3999999999987</v>
+        <v>745.59999999999945</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A86" s="95" t="s">
+      <c r="A86" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="B86" s="103"/>
-      <c r="C86" s="91" t="s">
+      <c r="B86" s="112"/>
+      <c r="C86" s="80" t="s">
         <v>170</v>
       </c>
       <c r="D86" s="144"/>
@@ -28175,25 +28190,25 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A87" s="95" t="s">
+      <c r="A87" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="96"/>
-      <c r="C87" s="101"/>
-      <c r="D87" s="94"/>
+      <c r="B87" s="104"/>
+      <c r="C87" s="110"/>
+      <c r="D87" s="83"/>
       <c r="E87" s="66">
         <f>C74</f>
         <v>1443</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C88" s="93" t="s">
+      <c r="C88" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="94"/>
+      <c r="D88" s="83"/>
       <c r="E88" s="37">
         <f>(E18+E85)-SUM(E86:E87)</f>
-        <v>1123.3999999999987</v>
+        <v>807.59999999999945</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="13.5" customHeight="1">
@@ -28211,72 +28226,72 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A91" s="97" t="s">
+      <c r="A91" s="105" t="s">
         <v>153</v>
       </c>
-      <c r="B91" s="98"/>
-      <c r="C91" s="98"/>
-      <c r="D91" s="98"/>
-      <c r="E91" s="99"/>
+      <c r="B91" s="106"/>
+      <c r="C91" s="106"/>
+      <c r="D91" s="106"/>
+      <c r="E91" s="92"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A92" s="106" t="s">
+      <c r="A92" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B92" s="94"/>
-      <c r="C92" s="106" t="s">
+      <c r="B92" s="83"/>
+      <c r="C92" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D92" s="94"/>
+      <c r="D92" s="83"/>
       <c r="E92" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A93" s="95" t="s">
+      <c r="A93" s="103" t="s">
         <v>157</v>
       </c>
-      <c r="B93" s="96"/>
-      <c r="C93" s="101"/>
-      <c r="D93" s="94"/>
+      <c r="B93" s="104"/>
+      <c r="C93" s="110"/>
+      <c r="D93" s="83"/>
       <c r="E93" s="37">
         <f>E88</f>
-        <v>1123.3999999999987</v>
+        <v>807.59999999999945</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A94" s="95" t="s">
+      <c r="A94" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="103"/>
-      <c r="C94" s="91" t="s">
+      <c r="B94" s="112"/>
+      <c r="C94" s="80" t="s">
         <v>174</v>
       </c>
-      <c r="D94" s="107"/>
+      <c r="D94" s="115"/>
       <c r="E94" s="52">
         <v>939</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A95" s="95" t="s">
+      <c r="A95" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B95" s="96"/>
-      <c r="C95" s="101"/>
-      <c r="D95" s="94"/>
+      <c r="B95" s="104"/>
+      <c r="C95" s="110"/>
+      <c r="D95" s="83"/>
       <c r="E95" s="66">
         <f>C74</f>
         <v>1443</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C96" s="93" t="s">
+      <c r="C96" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="D96" s="94"/>
+      <c r="D96" s="83"/>
       <c r="E96" s="52">
         <f>(E23+E93)-SUM(E94:E95)</f>
-        <v>1146.3999999999987</v>
+        <v>830.59999999999945</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="13.5" customHeight="1">
@@ -31983,52 +31998,57 @@
     <mergeCell ref="A28:C28"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:C7">
     <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C7">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="E81">
+    <cfRule type="cellIs" dxfId="10" priority="12" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E81">
-    <cfRule type="cellIs" dxfId="9" priority="11" stopIfTrue="1" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88">
-    <cfRule type="cellIs" dxfId="5" priority="9" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="10" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E96">
-    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>